<commit_message>
- Added Wind Chill in health plot; - Improved label visualization.
</commit_message>
<xml_diff>
--- a/data/simpleWeather.xlsx
+++ b/data/simpleWeather.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Foglio1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Foglio1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
@@ -790,17 +790,17 @@
     <row r="2">
       <c r="A2" s="115" t="inlineStr">
         <is>
-          <t>2023-11-05 03:00 dom</t>
-        </is>
-      </c>
-      <c r="B2" s="119" t="n">
-        <v>15</v>
-      </c>
-      <c r="C2" s="119" t="n">
-        <v>10</v>
-      </c>
-      <c r="D2" s="123" t="n">
-        <v>71</v>
+          <t>2024-01-13 15:00 Sat</t>
+        </is>
+      </c>
+      <c r="B2" s="121" t="n">
+        <v>8</v>
+      </c>
+      <c r="C2" s="121" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="119" t="n">
+        <v>58</v>
       </c>
       <c r="E2" s="115" t="n">
         <v>0</v>
@@ -828,36 +828,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K2" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L2" s="120" t="inlineStr">
-        <is>
-          <t>4.9</t>
-        </is>
-      </c>
-      <c r="M2" s="126" t="inlineStr">
-        <is>
-          <t>10.4</t>
+      <c r="K2" s="126" t="inlineStr">
+        <is>
+          <t>17.8</t>
+        </is>
+      </c>
+      <c r="L2" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M2" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="115" t="inlineStr">
         <is>
-          <t>2023-11-05 06:00 dom</t>
-        </is>
-      </c>
-      <c r="B3" s="119" t="n">
-        <v>17</v>
-      </c>
-      <c r="C3" s="117" t="n">
-        <v>12</v>
-      </c>
-      <c r="D3" s="123" t="n">
-        <v>71</v>
+          <t>2024-01-13 18:00 Sat</t>
+        </is>
+      </c>
+      <c r="B3" s="121" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" s="121" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="121" t="n">
+        <v>69</v>
       </c>
       <c r="E3" s="115" t="n">
         <v>0</v>
@@ -885,36 +885,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K3" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L3" s="120" t="inlineStr">
-        <is>
-          <t>2.4</t>
-        </is>
-      </c>
-      <c r="M3" s="125" t="inlineStr">
-        <is>
-          <t>9.3</t>
+      <c r="K3" s="126" t="inlineStr">
+        <is>
+          <t>10.7</t>
+        </is>
+      </c>
+      <c r="L3" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M3" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="115" t="inlineStr">
         <is>
-          <t>2023-11-05 09:00 dom</t>
-        </is>
-      </c>
-      <c r="B4" s="119" t="n">
-        <v>21</v>
-      </c>
-      <c r="C4" s="117" t="n">
-        <v>12</v>
-      </c>
-      <c r="D4" s="119" t="n">
-        <v>57</v>
+          <t>2024-01-13 21:00 Sat</t>
+        </is>
+      </c>
+      <c r="B4" s="121" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" s="121" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="123" t="n">
+        <v>75</v>
       </c>
       <c r="E4" s="115" t="n">
         <v>0</v>
@@ -942,9 +942,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K4" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K4" s="120" t="inlineStr">
+        <is>
+          <t>4.9</t>
         </is>
       </c>
       <c r="L4" s="115" t="inlineStr">
@@ -952,26 +952,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M4" s="125" t="inlineStr">
-        <is>
-          <t>6.2</t>
+      <c r="M4" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="115" t="inlineStr">
         <is>
-          <t>2023-11-05 12:00 dom</t>
-        </is>
-      </c>
-      <c r="B5" s="119" t="n">
-        <v>22</v>
-      </c>
-      <c r="C5" s="118" t="n">
-        <v>13</v>
-      </c>
-      <c r="D5" s="119" t="n">
-        <v>56</v>
+          <t>2024-01-14 00:00 Sun</t>
+        </is>
+      </c>
+      <c r="B5" s="121" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="121" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="123" t="n">
+        <v>74</v>
       </c>
       <c r="E5" s="115" t="n">
         <v>0</v>
@@ -999,9 +999,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K5" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K5" s="120" t="inlineStr">
+        <is>
+          <t>2.7</t>
         </is>
       </c>
       <c r="L5" s="115" t="inlineStr">
@@ -1009,26 +1009,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M5" s="120" t="inlineStr">
-        <is>
-          <t>3.1</t>
+      <c r="M5" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="115" t="inlineStr">
         <is>
-          <t>2023-11-05 15:00 dom</t>
-        </is>
-      </c>
-      <c r="B6" s="119" t="n">
-        <v>21</v>
-      </c>
-      <c r="C6" s="118" t="n">
-        <v>15</v>
+          <t>2024-01-14 03:00 Sun</t>
+        </is>
+      </c>
+      <c r="B6" s="121" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="121" t="n">
+        <v>1</v>
       </c>
       <c r="D6" s="123" t="n">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="E6" s="115" t="n">
         <v>0</v>
@@ -1056,36 +1056,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K6" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L6" s="120" t="inlineStr">
-        <is>
-          <t>0.4</t>
-        </is>
-      </c>
-      <c r="M6" s="120" t="inlineStr">
-        <is>
-          <t>1.8</t>
+      <c r="K6" s="120" t="inlineStr">
+        <is>
+          <t>0.1</t>
+        </is>
+      </c>
+      <c r="L6" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M6" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="115" t="inlineStr">
         <is>
-          <t>2023-11-05 18:00 dom</t>
-        </is>
-      </c>
-      <c r="B7" s="119" t="n">
-        <v>20</v>
-      </c>
-      <c r="C7" s="118" t="n">
-        <v>14</v>
-      </c>
-      <c r="D7" s="121" t="n">
-        <v>70</v>
+          <t>2024-01-14 06:00 Sun</t>
+        </is>
+      </c>
+      <c r="B7" s="121" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" s="121" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="123" t="n">
+        <v>78</v>
       </c>
       <c r="E7" s="115" t="n">
         <v>0</v>
@@ -1113,36 +1113,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K7" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L7" s="120" t="inlineStr">
-        <is>
-          <t>0.4</t>
-        </is>
-      </c>
-      <c r="M7" s="120" t="inlineStr">
-        <is>
-          <t>4.2</t>
+      <c r="K7" s="120" t="inlineStr">
+        <is>
+          <t>0.9</t>
+        </is>
+      </c>
+      <c r="L7" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M7" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="115" t="inlineStr">
         <is>
-          <t>2023-11-05 21:00 dom</t>
-        </is>
-      </c>
-      <c r="B8" s="119" t="n">
-        <v>18</v>
-      </c>
-      <c r="C8" s="118" t="n">
-        <v>14</v>
-      </c>
-      <c r="D8" s="123" t="n">
-        <v>79</v>
+          <t>2024-01-14 09:00 Sun</t>
+        </is>
+      </c>
+      <c r="B8" s="121" t="n">
+        <v>9</v>
+      </c>
+      <c r="C8" s="121" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="119" t="n">
+        <v>59</v>
       </c>
       <c r="E8" s="115" t="n">
         <v>0</v>
@@ -1150,9 +1150,9 @@
       <c r="F8" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G8" s="131" t="inlineStr">
-        <is>
-          <t>4.8e-06</t>
+      <c r="G8" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H8" s="120" t="inlineStr">
@@ -1170,9 +1170,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K8" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K8" s="120" t="inlineStr">
+        <is>
+          <t>2.6</t>
         </is>
       </c>
       <c r="L8" s="115" t="inlineStr">
@@ -1189,17 +1189,17 @@
     <row r="9">
       <c r="A9" s="115" t="inlineStr">
         <is>
-          <t>2023-11-06 00:00 lun</t>
-        </is>
-      </c>
-      <c r="B9" s="119" t="n">
-        <v>18</v>
-      </c>
-      <c r="C9" s="118" t="n">
-        <v>14</v>
-      </c>
-      <c r="D9" s="123" t="n">
-        <v>78</v>
+          <t>2024-01-14 12:00 Sun</t>
+        </is>
+      </c>
+      <c r="B9" s="121" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" s="121" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" s="119" t="n">
+        <v>55</v>
       </c>
       <c r="E9" s="115" t="n">
         <v>0</v>
@@ -1227,9 +1227,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K9" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K9" s="120" t="inlineStr">
+        <is>
+          <t>3.6</t>
         </is>
       </c>
       <c r="L9" s="115" t="inlineStr">
@@ -1237,26 +1237,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M9" s="126" t="inlineStr">
-        <is>
-          <t>11.1</t>
+      <c r="M9" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="115" t="inlineStr">
         <is>
-          <t>2023-11-06 03:00 lun</t>
-        </is>
-      </c>
-      <c r="B10" s="119" t="n">
-        <v>17</v>
-      </c>
-      <c r="C10" s="118" t="n">
-        <v>13</v>
-      </c>
-      <c r="D10" s="123" t="n">
-        <v>81</v>
+          <t>2024-01-14 15:00 Sun</t>
+        </is>
+      </c>
+      <c r="B10" s="121" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" s="121" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" s="121" t="n">
+        <v>62</v>
       </c>
       <c r="E10" s="115" t="n">
         <v>0</v>
@@ -1284,9 +1284,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K10" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K10" s="120" t="inlineStr">
+        <is>
+          <t>0.4</t>
         </is>
       </c>
       <c r="L10" s="115" t="inlineStr">
@@ -1294,26 +1294,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M10" s="130" t="inlineStr">
-        <is>
-          <t>39.5</t>
+      <c r="M10" s="120" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="115" t="inlineStr">
         <is>
-          <t>2023-11-06 06:00 lun</t>
-        </is>
-      </c>
-      <c r="B11" s="119" t="n">
-        <v>16</v>
-      </c>
-      <c r="C11" s="118" t="n">
-        <v>13</v>
+          <t>2024-01-14 18:00 Sun</t>
+        </is>
+      </c>
+      <c r="B11" s="121" t="n">
+        <v>7</v>
+      </c>
+      <c r="C11" s="121" t="n">
+        <v>2</v>
       </c>
       <c r="D11" s="123" t="n">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E11" s="115" t="n">
         <v>0</v>
@@ -1341,9 +1341,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K11" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K11" s="120" t="inlineStr">
+        <is>
+          <t>3.5</t>
         </is>
       </c>
       <c r="L11" s="115" t="inlineStr">
@@ -1353,24 +1353,24 @@
       </c>
       <c r="M11" s="126" t="inlineStr">
         <is>
-          <t>19.8</t>
+          <t>17</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="115" t="inlineStr">
         <is>
-          <t>2023-11-06 09:00 lun</t>
-        </is>
-      </c>
-      <c r="B12" s="119" t="n">
-        <v>21</v>
-      </c>
-      <c r="C12" s="117" t="n">
-        <v>12</v>
-      </c>
-      <c r="D12" s="119" t="n">
-        <v>54</v>
+          <t>2024-01-14 21:00 Sun</t>
+        </is>
+      </c>
+      <c r="B12" s="121" t="n">
+        <v>8</v>
+      </c>
+      <c r="C12" s="121" t="n">
+        <v>3</v>
+      </c>
+      <c r="D12" s="123" t="n">
+        <v>74</v>
       </c>
       <c r="E12" s="115" t="n">
         <v>0</v>
@@ -1398,36 +1398,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K12" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L12" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M12" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K12" s="120" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L12" s="129" t="inlineStr">
+        <is>
+          <t>63.4</t>
+        </is>
+      </c>
+      <c r="M12" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="115" t="inlineStr">
         <is>
-          <t>2023-11-06 12:00 lun</t>
-        </is>
-      </c>
-      <c r="B13" s="119" t="n">
-        <v>22</v>
-      </c>
-      <c r="C13" s="117" t="n">
-        <v>11</v>
-      </c>
-      <c r="D13" s="119" t="n">
-        <v>49</v>
+          <t>2024-01-15 00:00 Mon</t>
+        </is>
+      </c>
+      <c r="B13" s="121" t="n">
+        <v>8</v>
+      </c>
+      <c r="C13" s="121" t="n">
+        <v>4</v>
+      </c>
+      <c r="D13" s="123" t="n">
+        <v>78</v>
       </c>
       <c r="E13" s="115" t="n">
         <v>0</v>
@@ -1435,9 +1435,9 @@
       <c r="F13" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G13" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G13" s="131" t="inlineStr">
+        <is>
+          <t>8.8e-06</t>
         </is>
       </c>
       <c r="H13" s="120" t="inlineStr">
@@ -1457,34 +1457,34 @@
       </c>
       <c r="K13" s="120" t="inlineStr">
         <is>
-          <t>0.5</t>
-        </is>
-      </c>
-      <c r="L13" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M13" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L13" s="128" t="inlineStr">
+        <is>
+          <t>81.7</t>
+        </is>
+      </c>
+      <c r="M13" s="129" t="inlineStr">
+        <is>
+          <t>71.9</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="115" t="inlineStr">
         <is>
-          <t>2023-11-06 15:00 lun</t>
-        </is>
-      </c>
-      <c r="B14" s="119" t="n">
-        <v>20</v>
-      </c>
-      <c r="C14" s="117" t="n">
-        <v>11</v>
-      </c>
-      <c r="D14" s="119" t="n">
-        <v>56</v>
+          <t>2024-01-15 03:00 Mon</t>
+        </is>
+      </c>
+      <c r="B14" s="121" t="n">
+        <v>10</v>
+      </c>
+      <c r="C14" s="119" t="n">
+        <v>7</v>
+      </c>
+      <c r="D14" s="123" t="n">
+        <v>81</v>
       </c>
       <c r="E14" s="115" t="n">
         <v>0</v>
@@ -1512,36 +1512,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K14" s="120" t="inlineStr">
-        <is>
-          <t>0.2</t>
-        </is>
-      </c>
-      <c r="L14" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M14" s="125" t="inlineStr">
-        <is>
-          <t>5.6</t>
+      <c r="K14" s="130" t="inlineStr">
+        <is>
+          <t>38.4</t>
+        </is>
+      </c>
+      <c r="L14" s="128" t="inlineStr">
+        <is>
+          <t>90.9</t>
+        </is>
+      </c>
+      <c r="M14" s="130" t="inlineStr">
+        <is>
+          <t>55.9</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="115" t="inlineStr">
         <is>
-          <t>2023-11-06 18:00 lun</t>
-        </is>
-      </c>
-      <c r="B15" s="119" t="n">
-        <v>18</v>
-      </c>
-      <c r="C15" s="117" t="n">
-        <v>12</v>
+          <t>2024-01-15 06:00 Mon</t>
+        </is>
+      </c>
+      <c r="B15" s="127" t="n">
+        <v>11</v>
+      </c>
+      <c r="C15" s="119" t="n">
+        <v>8</v>
       </c>
       <c r="D15" s="123" t="n">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="E15" s="115" t="n">
         <v>0</v>
@@ -1549,14 +1549,14 @@
       <c r="F15" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G15" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H15" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G15" s="131" t="inlineStr">
+        <is>
+          <t>1.04e-05</t>
+        </is>
+      </c>
+      <c r="H15" s="119" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I15" s="120" t="inlineStr">
@@ -1569,36 +1569,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K15" s="120" t="inlineStr">
-        <is>
-          <t>0.1</t>
-        </is>
-      </c>
-      <c r="L15" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M15" s="125" t="inlineStr">
-        <is>
-          <t>6.7</t>
+      <c r="K15" s="129" t="inlineStr">
+        <is>
+          <t>69.1</t>
+        </is>
+      </c>
+      <c r="L15" s="128" t="inlineStr">
+        <is>
+          <t>91.6</t>
+        </is>
+      </c>
+      <c r="M15" s="129" t="inlineStr">
+        <is>
+          <t>66.4</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="115" t="inlineStr">
         <is>
-          <t>2023-11-06 21:00 lun</t>
-        </is>
-      </c>
-      <c r="B16" s="119" t="n">
-        <v>17</v>
-      </c>
-      <c r="C16" s="117" t="n">
-        <v>11</v>
-      </c>
-      <c r="D16" s="121" t="n">
-        <v>68</v>
+          <t>2024-01-15 09:00 Mon</t>
+        </is>
+      </c>
+      <c r="B16" s="127" t="n">
+        <v>13</v>
+      </c>
+      <c r="C16" s="119" t="n">
+        <v>9</v>
+      </c>
+      <c r="D16" s="123" t="n">
+        <v>76</v>
       </c>
       <c r="E16" s="115" t="n">
         <v>0</v>
@@ -1606,9 +1606,9 @@
       <c r="F16" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G16" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G16" s="131" t="inlineStr">
+        <is>
+          <t>8e-07</t>
         </is>
       </c>
       <c r="H16" s="120" t="inlineStr">
@@ -1626,36 +1626,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K16" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L16" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M16" s="125" t="inlineStr">
-        <is>
-          <t>5.7</t>
+      <c r="K16" s="129" t="inlineStr">
+        <is>
+          <t>67.2</t>
+        </is>
+      </c>
+      <c r="L16" s="128" t="inlineStr">
+        <is>
+          <t>99.4</t>
+        </is>
+      </c>
+      <c r="M16" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="115" t="inlineStr">
         <is>
-          <t>2023-11-07 00:00 mar</t>
-        </is>
-      </c>
-      <c r="B17" s="119" t="n">
-        <v>17</v>
-      </c>
-      <c r="C17" s="117" t="n">
-        <v>11</v>
-      </c>
-      <c r="D17" s="121" t="n">
-        <v>68</v>
+          <t>2024-01-15 12:00 Mon</t>
+        </is>
+      </c>
+      <c r="B17" s="127" t="n">
+        <v>12</v>
+      </c>
+      <c r="C17" s="119" t="n">
+        <v>9</v>
+      </c>
+      <c r="D17" s="123" t="n">
+        <v>82</v>
       </c>
       <c r="E17" s="115" t="n">
         <v>0</v>
@@ -1663,9 +1663,9 @@
       <c r="F17" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G17" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G17" s="131" t="inlineStr">
+        <is>
+          <t>2e-06</t>
         </is>
       </c>
       <c r="H17" s="120" t="inlineStr">
@@ -1683,36 +1683,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K17" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L17" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M17" s="120" t="inlineStr">
-        <is>
-          <t>4.9</t>
+      <c r="K17" s="129" t="inlineStr">
+        <is>
+          <t>63.7</t>
+        </is>
+      </c>
+      <c r="L17" s="128" t="inlineStr">
+        <is>
+          <t>80.9</t>
+        </is>
+      </c>
+      <c r="M17" s="128" t="inlineStr">
+        <is>
+          <t>99.7</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="115" t="inlineStr">
         <is>
-          <t>2023-11-07 03:00 mar</t>
-        </is>
-      </c>
-      <c r="B18" s="119" t="n">
-        <v>16</v>
-      </c>
-      <c r="C18" s="117" t="n">
+          <t>2024-01-15 15:00 Mon</t>
+        </is>
+      </c>
+      <c r="B18" s="127" t="n">
         <v>12</v>
       </c>
+      <c r="C18" s="119" t="n">
+        <v>10</v>
+      </c>
       <c r="D18" s="123" t="n">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E18" s="115" t="n">
         <v>0</v>
@@ -1740,36 +1740,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K18" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L18" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M18" s="120" t="inlineStr">
-        <is>
-          <t>2.6</t>
+      <c r="K18" s="129" t="inlineStr">
+        <is>
+          <t>63.3</t>
+        </is>
+      </c>
+      <c r="L18" s="130" t="inlineStr">
+        <is>
+          <t>35.3</t>
+        </is>
+      </c>
+      <c r="M18" s="130" t="inlineStr">
+        <is>
+          <t>55.5</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="115" t="inlineStr">
         <is>
-          <t>2023-11-07 06:00 mar</t>
-        </is>
-      </c>
-      <c r="B19" s="119" t="n">
-        <v>16</v>
-      </c>
-      <c r="C19" s="118" t="n">
-        <v>13</v>
+          <t>2024-01-15 18:00 Mon</t>
+        </is>
+      </c>
+      <c r="B19" s="121" t="n">
+        <v>10</v>
+      </c>
+      <c r="C19" s="119" t="n">
+        <v>9</v>
       </c>
       <c r="D19" s="123" t="n">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="E19" s="115" t="n">
         <v>0</v>
@@ -1797,36 +1797,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K19" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L19" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M19" s="120" t="inlineStr">
-        <is>
-          <t>4.2</t>
+      <c r="K19" s="130" t="inlineStr">
+        <is>
+          <t>35.1</t>
+        </is>
+      </c>
+      <c r="L19" s="126" t="inlineStr">
+        <is>
+          <t>17.6</t>
+        </is>
+      </c>
+      <c r="M19" s="127" t="inlineStr">
+        <is>
+          <t>28.3</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="115" t="inlineStr">
         <is>
-          <t>2023-11-07 09:00 mar</t>
-        </is>
-      </c>
-      <c r="B20" s="119" t="n">
-        <v>21</v>
-      </c>
-      <c r="C20" s="117" t="n">
-        <v>12</v>
-      </c>
-      <c r="D20" s="119" t="n">
-        <v>56</v>
+          <t>2024-01-15 21:00 Mon</t>
+        </is>
+      </c>
+      <c r="B20" s="127" t="n">
+        <v>11</v>
+      </c>
+      <c r="C20" s="119" t="n">
+        <v>9</v>
+      </c>
+      <c r="D20" s="123" t="n">
+        <v>89</v>
       </c>
       <c r="E20" s="115" t="n">
         <v>0</v>
@@ -1854,36 +1854,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K20" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L20" s="120" t="inlineStr">
-        <is>
-          <t>1.7</t>
-        </is>
-      </c>
-      <c r="M20" s="129" t="inlineStr">
-        <is>
-          <t>68.7</t>
+      <c r="K20" s="120" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L20" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M20" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="115" t="inlineStr">
         <is>
-          <t>2023-11-07 12:00 mar</t>
-        </is>
-      </c>
-      <c r="B21" s="117" t="n">
-        <v>23</v>
-      </c>
-      <c r="C21" s="117" t="n">
-        <v>12</v>
-      </c>
-      <c r="D21" s="119" t="n">
-        <v>49</v>
+          <t>2024-01-16 00:00 Tue</t>
+        </is>
+      </c>
+      <c r="B21" s="127" t="n">
+        <v>11</v>
+      </c>
+      <c r="C21" s="119" t="n">
+        <v>9</v>
+      </c>
+      <c r="D21" s="123" t="n">
+        <v>90</v>
       </c>
       <c r="E21" s="115" t="n">
         <v>0</v>
@@ -1911,36 +1911,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K21" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L21" s="120" t="inlineStr">
-        <is>
-          <t>3.3</t>
-        </is>
-      </c>
-      <c r="M21" s="129" t="inlineStr">
-        <is>
-          <t>72.6</t>
+      <c r="K21" s="120" t="inlineStr">
+        <is>
+          <t>2.5</t>
+        </is>
+      </c>
+      <c r="L21" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M21" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="115" t="inlineStr">
         <is>
-          <t>2023-11-07 15:00 mar</t>
-        </is>
-      </c>
-      <c r="B22" s="119" t="n">
-        <v>21</v>
-      </c>
-      <c r="C22" s="117" t="n">
-        <v>12</v>
-      </c>
-      <c r="D22" s="119" t="n">
-        <v>56</v>
+          <t>2024-01-16 03:00 Tue</t>
+        </is>
+      </c>
+      <c r="B22" s="121" t="n">
+        <v>10</v>
+      </c>
+      <c r="C22" s="119" t="n">
+        <v>9</v>
+      </c>
+      <c r="D22" s="123" t="n">
+        <v>90</v>
       </c>
       <c r="E22" s="115" t="n">
         <v>0</v>
@@ -1975,29 +1975,29 @@
       </c>
       <c r="L22" s="120" t="inlineStr">
         <is>
-          <t>3.3</t>
-        </is>
-      </c>
-      <c r="M22" s="130" t="inlineStr">
-        <is>
-          <t>38.6</t>
+          <t>0.1</t>
+        </is>
+      </c>
+      <c r="M22" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="115" t="inlineStr">
         <is>
-          <t>2023-11-07 18:00 mar</t>
-        </is>
-      </c>
-      <c r="B23" s="119" t="n">
-        <v>18</v>
-      </c>
-      <c r="C23" s="118" t="n">
-        <v>13</v>
+          <t>2024-01-16 06:00 Tue</t>
+        </is>
+      </c>
+      <c r="B23" s="121" t="n">
+        <v>9</v>
+      </c>
+      <c r="C23" s="119" t="n">
+        <v>7</v>
       </c>
       <c r="D23" s="123" t="n">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E23" s="115" t="n">
         <v>0</v>
@@ -2030,31 +2030,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L23" s="120" t="inlineStr">
-        <is>
-          <t>1.9</t>
-        </is>
-      </c>
-      <c r="M23" s="126" t="inlineStr">
-        <is>
-          <t>21.8</t>
+      <c r="L23" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M23" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="115" t="inlineStr">
         <is>
-          <t>2023-11-07 21:00 mar</t>
+          <t>2024-01-16 09:00 Tue</t>
         </is>
       </c>
       <c r="B24" s="119" t="n">
-        <v>18</v>
-      </c>
-      <c r="C24" s="118" t="n">
-        <v>16</v>
-      </c>
-      <c r="D24" s="123" t="n">
-        <v>89</v>
+        <v>14</v>
+      </c>
+      <c r="C24" s="119" t="n">
+        <v>7</v>
+      </c>
+      <c r="D24" s="121" t="n">
+        <v>63</v>
       </c>
       <c r="E24" s="115" t="n">
         <v>0</v>
@@ -2082,36 +2082,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K24" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L24" s="120" t="inlineStr">
-        <is>
-          <t>1.8</t>
-        </is>
-      </c>
-      <c r="M24" s="125" t="inlineStr">
-        <is>
-          <t>5</t>
+      <c r="K24" s="120" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+      <c r="L24" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M24" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="115" t="inlineStr">
         <is>
-          <t>2023-11-08 00:00 mer</t>
+          <t>2024-01-16 12:00 Tue</t>
         </is>
       </c>
       <c r="B25" s="119" t="n">
-        <v>18</v>
-      </c>
-      <c r="C25" s="118" t="n">
-        <v>17</v>
-      </c>
-      <c r="D25" s="123" t="n">
-        <v>92</v>
+        <v>15</v>
+      </c>
+      <c r="C25" s="119" t="n">
+        <v>6</v>
+      </c>
+      <c r="D25" s="119" t="n">
+        <v>55</v>
       </c>
       <c r="E25" s="115" t="n">
         <v>0</v>
@@ -2139,36 +2139,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K25" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L25" s="120" t="inlineStr">
-        <is>
-          <t>3.5</t>
-        </is>
-      </c>
-      <c r="M25" s="126" t="inlineStr">
-        <is>
-          <t>16.2</t>
+      <c r="K25" s="125" t="inlineStr">
+        <is>
+          <t>6.6</t>
+        </is>
+      </c>
+      <c r="L25" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M25" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="115" t="inlineStr">
         <is>
-          <t>2023-11-08 03:00 mer</t>
+          <t>2024-01-16 15:00 Tue</t>
         </is>
       </c>
       <c r="B26" s="119" t="n">
-        <v>18</v>
-      </c>
-      <c r="C26" s="118" t="n">
-        <v>17</v>
-      </c>
-      <c r="D26" s="123" t="n">
-        <v>93</v>
+        <v>14</v>
+      </c>
+      <c r="C26" s="119" t="n">
+        <v>8</v>
+      </c>
+      <c r="D26" s="121" t="n">
+        <v>69</v>
       </c>
       <c r="E26" s="115" t="n">
         <v>0</v>
@@ -2196,36 +2196,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K26" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L26" s="129" t="inlineStr">
-        <is>
-          <t>74.7</t>
-        </is>
-      </c>
-      <c r="M26" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="K26" s="129" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="L26" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M26" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="115" t="inlineStr">
         <is>
-          <t>2023-11-08 06:00 mer</t>
-        </is>
-      </c>
-      <c r="B27" s="119" t="n">
-        <v>18</v>
-      </c>
-      <c r="C27" s="118" t="n">
-        <v>17</v>
+          <t>2024-01-16 18:00 Tue</t>
+        </is>
+      </c>
+      <c r="B27" s="127" t="n">
+        <v>12</v>
+      </c>
+      <c r="C27" s="119" t="n">
+        <v>8</v>
       </c>
       <c r="D27" s="123" t="n">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="E27" s="115" t="n">
         <v>0</v>
@@ -2253,36 +2253,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K27" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L27" s="128" t="inlineStr">
-        <is>
-          <t>87.4</t>
-        </is>
-      </c>
-      <c r="M27" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="K27" s="128" t="inlineStr">
+        <is>
+          <t>87.5</t>
+        </is>
+      </c>
+      <c r="L27" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M27" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="115" t="inlineStr">
         <is>
-          <t>2023-11-08 09:00 mer</t>
-        </is>
-      </c>
-      <c r="B28" s="119" t="n">
-        <v>20</v>
-      </c>
-      <c r="C28" s="118" t="n">
-        <v>16</v>
+          <t>2024-01-16 21:00 Tue</t>
+        </is>
+      </c>
+      <c r="B28" s="127" t="n">
+        <v>12</v>
+      </c>
+      <c r="C28" s="119" t="n">
+        <v>8</v>
       </c>
       <c r="D28" s="123" t="n">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E28" s="115" t="n">
         <v>0</v>
@@ -2290,9 +2290,9 @@
       <c r="F28" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G28" s="131" t="inlineStr">
-        <is>
-          <t>8e-07</t>
+      <c r="G28" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H28" s="120" t="inlineStr">
@@ -2310,36 +2310,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K28" s="126" t="inlineStr">
-        <is>
-          <t>13.9</t>
-        </is>
-      </c>
-      <c r="L28" s="128" t="inlineStr">
+      <c r="K28" s="128" t="inlineStr">
         <is>
           <t>100</t>
         </is>
       </c>
-      <c r="M28" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="L28" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M28" s="120" t="inlineStr">
+        <is>
+          <t>0.5</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="115" t="inlineStr">
         <is>
-          <t>2023-11-08 12:00 mer</t>
-        </is>
-      </c>
-      <c r="B29" s="119" t="n">
-        <v>22</v>
-      </c>
-      <c r="C29" s="118" t="n">
-        <v>13</v>
-      </c>
-      <c r="D29" s="119" t="n">
-        <v>57</v>
+          <t>2024-01-17 00:00 Wed</t>
+        </is>
+      </c>
+      <c r="B29" s="127" t="n">
+        <v>11</v>
+      </c>
+      <c r="C29" s="119" t="n">
+        <v>8</v>
+      </c>
+      <c r="D29" s="123" t="n">
+        <v>83</v>
       </c>
       <c r="E29" s="115" t="n">
         <v>0</v>
@@ -2367,36 +2367,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K29" s="126" t="inlineStr">
-        <is>
-          <t>16.5</t>
-        </is>
-      </c>
-      <c r="L29" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="M29" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="K29" s="129" t="inlineStr">
+        <is>
+          <t>68.6</t>
+        </is>
+      </c>
+      <c r="L29" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M29" s="120" t="inlineStr">
+        <is>
+          <t>0.2</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="115" t="inlineStr">
         <is>
-          <t>2023-11-08 15:00 mer</t>
-        </is>
-      </c>
-      <c r="B30" s="119" t="n">
-        <v>16</v>
-      </c>
-      <c r="C30" s="118" t="n">
-        <v>13</v>
+          <t>2024-01-17 03:00 Wed</t>
+        </is>
+      </c>
+      <c r="B30" s="121" t="n">
+        <v>10</v>
+      </c>
+      <c r="C30" s="119" t="n">
+        <v>7</v>
       </c>
       <c r="D30" s="123" t="n">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E30" s="115" t="n">
         <v>0</v>
@@ -2424,36 +2424,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K30" s="130" t="inlineStr">
-        <is>
-          <t>40.2</t>
-        </is>
-      </c>
-      <c r="L30" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="M30" s="129" t="inlineStr">
-        <is>
-          <t>69</t>
+      <c r="K30" s="120" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L30" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M30" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="115" t="inlineStr">
         <is>
-          <t>2023-11-08 18:00 mer</t>
-        </is>
-      </c>
-      <c r="B31" s="119" t="n">
-        <v>16</v>
-      </c>
-      <c r="C31" s="117" t="n">
-        <v>11</v>
+          <t>2024-01-17 06:00 Wed</t>
+        </is>
+      </c>
+      <c r="B31" s="121" t="n">
+        <v>9</v>
+      </c>
+      <c r="C31" s="119" t="n">
+        <v>8</v>
       </c>
       <c r="D31" s="123" t="n">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="E31" s="115" t="n">
         <v>0</v>
@@ -2481,36 +2481,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K31" s="130" t="inlineStr">
-        <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="L31" s="130" t="inlineStr">
-        <is>
-          <t>52.7</t>
-        </is>
-      </c>
-      <c r="M31" s="130" t="inlineStr">
-        <is>
-          <t>36</t>
+      <c r="K31" s="120" t="inlineStr">
+        <is>
+          <t>3.1</t>
+        </is>
+      </c>
+      <c r="L31" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M31" s="120" t="inlineStr">
+        <is>
+          <t>1.7</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="115" t="inlineStr">
         <is>
-          <t>2023-11-08 21:00 mer</t>
+          <t>2024-01-17 09:00 Wed</t>
         </is>
       </c>
       <c r="B32" s="119" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32" s="119" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D32" s="121" t="n">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E32" s="115" t="n">
         <v>0</v>
@@ -2538,9 +2538,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K32" s="130" t="inlineStr">
-        <is>
-          <t>45.2</t>
+      <c r="K32" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L32" s="115" t="inlineStr">
@@ -2548,26 +2548,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M32" s="129" t="inlineStr">
-        <is>
-          <t>63.4</t>
+      <c r="M32" s="125" t="inlineStr">
+        <is>
+          <t>5.4</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="115" t="inlineStr">
         <is>
-          <t>2023-11-09 00:00 gio</t>
+          <t>2024-01-17 12:00 Wed</t>
         </is>
       </c>
       <c r="B33" s="119" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C33" s="119" t="n">
-        <v>8</v>
-      </c>
-      <c r="D33" s="121" t="n">
-        <v>66</v>
+        <v>7</v>
+      </c>
+      <c r="D33" s="119" t="n">
+        <v>56</v>
       </c>
       <c r="E33" s="115" t="n">
         <v>0</v>
@@ -2595,9 +2595,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K33" s="127" t="inlineStr">
-        <is>
-          <t>22.6</t>
+      <c r="K33" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L33" s="115" t="inlineStr">
@@ -2607,24 +2607,24 @@
       </c>
       <c r="M33" s="130" t="inlineStr">
         <is>
-          <t>55.9</t>
+          <t>38.8</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="115" t="inlineStr">
         <is>
-          <t>2023-11-09 03:00 gio</t>
-        </is>
-      </c>
-      <c r="B34" s="119" t="n">
-        <v>14</v>
+          <t>2024-01-17 15:00 Wed</t>
+        </is>
+      </c>
+      <c r="B34" s="127" t="n">
+        <v>13</v>
       </c>
       <c r="C34" s="119" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D34" s="121" t="n">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E34" s="115" t="n">
         <v>0</v>
@@ -2659,29 +2659,29 @@
       </c>
       <c r="L34" s="120" t="inlineStr">
         <is>
-          <t>1.7</t>
-        </is>
-      </c>
-      <c r="M34" s="125" t="inlineStr">
-        <is>
-          <t>9.7</t>
+          <t>2.7</t>
+        </is>
+      </c>
+      <c r="M34" s="129" t="inlineStr">
+        <is>
+          <t>77.9</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="115" t="inlineStr">
         <is>
-          <t>2023-11-09 06:00 gio</t>
-        </is>
-      </c>
-      <c r="B35" s="119" t="n">
-        <v>14</v>
+          <t>2024-01-17 18:00 Wed</t>
+        </is>
+      </c>
+      <c r="B35" s="127" t="n">
+        <v>11</v>
       </c>
       <c r="C35" s="119" t="n">
         <v>8</v>
       </c>
-      <c r="D35" s="121" t="n">
-        <v>68</v>
+      <c r="D35" s="123" t="n">
+        <v>82</v>
       </c>
       <c r="E35" s="115" t="n">
         <v>0</v>
@@ -2714,31 +2714,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L35" s="120" t="inlineStr">
-        <is>
-          <t>3.5</t>
-        </is>
-      </c>
-      <c r="M35" s="126" t="inlineStr">
-        <is>
-          <t>12.6</t>
+      <c r="L35" s="126" t="inlineStr">
+        <is>
+          <t>17.8</t>
+        </is>
+      </c>
+      <c r="M35" s="128" t="inlineStr">
+        <is>
+          <t>86.9</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="115" t="inlineStr">
         <is>
-          <t>2023-11-09 09:00 gio</t>
-        </is>
-      </c>
-      <c r="B36" s="119" t="n">
-        <v>18</v>
+          <t>2024-01-17 21:00 Wed</t>
+        </is>
+      </c>
+      <c r="B36" s="127" t="n">
+        <v>11</v>
       </c>
       <c r="C36" s="119" t="n">
-        <v>8</v>
-      </c>
-      <c r="D36" s="119" t="n">
-        <v>52</v>
+        <v>9</v>
+      </c>
+      <c r="D36" s="123" t="n">
+        <v>86</v>
       </c>
       <c r="E36" s="115" t="n">
         <v>0</v>
@@ -2771,31 +2771,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L36" s="120" t="inlineStr">
-        <is>
-          <t>5</t>
+      <c r="L36" s="128" t="inlineStr">
+        <is>
+          <t>80.5</t>
         </is>
       </c>
       <c r="M36" s="129" t="inlineStr">
         <is>
-          <t>63.9</t>
+          <t>71.8</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="115" t="inlineStr">
         <is>
-          <t>2023-11-09 12:00 gio</t>
-        </is>
-      </c>
-      <c r="B37" s="119" t="n">
-        <v>18</v>
-      </c>
-      <c r="C37" s="119" t="n">
-        <v>8</v>
-      </c>
-      <c r="D37" s="119" t="n">
-        <v>50</v>
+          <t>2024-01-18 00:00 Thu</t>
+        </is>
+      </c>
+      <c r="B37" s="127" t="n">
+        <v>12</v>
+      </c>
+      <c r="C37" s="117" t="n">
+        <v>11</v>
+      </c>
+      <c r="D37" s="123" t="n">
+        <v>93</v>
       </c>
       <c r="E37" s="115" t="n">
         <v>0</v>
@@ -2828,31 +2828,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L37" s="125" t="inlineStr">
-        <is>
-          <t>8.4</t>
-        </is>
-      </c>
-      <c r="M37" s="115" t="inlineStr">
-        <is>
-          <t>81.5</t>
+      <c r="L37" s="130" t="inlineStr">
+        <is>
+          <t>43.8</t>
+        </is>
+      </c>
+      <c r="M37" s="130" t="inlineStr">
+        <is>
+          <t>39.5</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="115" t="inlineStr">
         <is>
-          <t>2023-11-09 15:00 gio</t>
-        </is>
-      </c>
-      <c r="B38" s="119" t="n">
-        <v>17</v>
-      </c>
-      <c r="C38" s="119" t="n">
-        <v>8</v>
-      </c>
-      <c r="D38" s="119" t="n">
-        <v>56</v>
+          <t>2024-01-18 03:00 Thu</t>
+        </is>
+      </c>
+      <c r="B38" s="127" t="n">
+        <v>12</v>
+      </c>
+      <c r="C38" s="117" t="n">
+        <v>11</v>
+      </c>
+      <c r="D38" s="123" t="n">
+        <v>92</v>
       </c>
       <c r="E38" s="115" t="n">
         <v>0</v>
@@ -2860,9 +2860,9 @@
       <c r="F38" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G38" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G38" s="131" t="inlineStr">
+        <is>
+          <t>8e-07</t>
         </is>
       </c>
       <c r="H38" s="120" t="inlineStr">
@@ -2880,36 +2880,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K38" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L38" s="128" t="inlineStr">
-        <is>
-          <t>85.3</t>
+      <c r="K38" s="125" t="inlineStr">
+        <is>
+          <t>8.6</t>
+        </is>
+      </c>
+      <c r="L38" s="126" t="inlineStr">
+        <is>
+          <t>11.4</t>
         </is>
       </c>
       <c r="M38" s="128" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>98.9</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="115" t="inlineStr">
         <is>
-          <t>2023-11-09 18:00 gio</t>
-        </is>
-      </c>
-      <c r="B39" s="119" t="n">
-        <v>14</v>
-      </c>
-      <c r="C39" s="119" t="n">
-        <v>8</v>
-      </c>
-      <c r="D39" s="121" t="n">
-        <v>65</v>
+          <t>2024-01-18 06:00 Thu</t>
+        </is>
+      </c>
+      <c r="B39" s="127" t="n">
+        <v>13</v>
+      </c>
+      <c r="C39" s="117" t="n">
+        <v>12</v>
+      </c>
+      <c r="D39" s="123" t="n">
+        <v>93</v>
       </c>
       <c r="E39" s="115" t="n">
         <v>0</v>
@@ -2917,9 +2917,9 @@
       <c r="F39" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G39" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G39" s="131" t="inlineStr">
+        <is>
+          <t>2.4e-06</t>
         </is>
       </c>
       <c r="H39" s="120" t="inlineStr">
@@ -2937,36 +2937,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K39" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L39" s="129" t="inlineStr">
-        <is>
-          <t>65.4</t>
+      <c r="K39" s="130" t="inlineStr">
+        <is>
+          <t>35.2</t>
+        </is>
+      </c>
+      <c r="L39" s="130" t="inlineStr">
+        <is>
+          <t>36.6</t>
         </is>
       </c>
       <c r="M39" s="128" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>99.5</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="115" t="inlineStr">
         <is>
-          <t>2023-11-09 21:00 gio</t>
-        </is>
-      </c>
-      <c r="B40" s="127" t="n">
-        <v>13</v>
-      </c>
-      <c r="C40" s="119" t="n">
-        <v>8</v>
-      </c>
-      <c r="D40" s="121" t="n">
-        <v>69</v>
+          <t>2024-01-18 09:00 Thu</t>
+        </is>
+      </c>
+      <c r="B40" s="119" t="n">
+        <v>15</v>
+      </c>
+      <c r="C40" s="117" t="n">
+        <v>12</v>
+      </c>
+      <c r="D40" s="123" t="n">
+        <v>84</v>
       </c>
       <c r="E40" s="115" t="n">
         <v>0</v>
@@ -2974,9 +2974,9 @@
       <c r="F40" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G40" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G40" s="131" t="inlineStr">
+        <is>
+          <t>8e-07</t>
         </is>
       </c>
       <c r="H40" s="120" t="inlineStr">
@@ -2994,36 +2994,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K40" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L40" s="130" t="inlineStr">
-        <is>
-          <t>38.7</t>
-        </is>
-      </c>
-      <c r="M40" s="126" t="inlineStr">
-        <is>
-          <t>18.7</t>
+      <c r="K40" s="130" t="inlineStr">
+        <is>
+          <t>51.1</t>
+        </is>
+      </c>
+      <c r="L40" s="129" t="inlineStr">
+        <is>
+          <t>79.7</t>
+        </is>
+      </c>
+      <c r="M40" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="115" t="inlineStr">
         <is>
-          <t>2023-11-10 00:00 ven</t>
-        </is>
-      </c>
-      <c r="B41" s="127" t="n">
+          <t>2024-01-18 12:00 Thu</t>
+        </is>
+      </c>
+      <c r="B41" s="119" t="n">
+        <v>16</v>
+      </c>
+      <c r="C41" s="118" t="n">
         <v>13</v>
       </c>
-      <c r="C41" s="119" t="n">
-        <v>8</v>
-      </c>
       <c r="D41" s="123" t="n">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="E41" s="115" t="n">
         <v>0</v>
@@ -3031,9 +3031,9 @@
       <c r="F41" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G41" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G41" s="131" t="inlineStr">
+        <is>
+          <t>1.6e-06</t>
         </is>
       </c>
       <c r="H41" s="120" t="inlineStr">
@@ -3051,36 +3051,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K41" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L41" s="130" t="inlineStr">
-        <is>
-          <t>42.8</t>
-        </is>
-      </c>
-      <c r="M41" s="126" t="inlineStr">
-        <is>
-          <t>16.9</t>
+      <c r="K41" s="130" t="inlineStr">
+        <is>
+          <t>44.6</t>
+        </is>
+      </c>
+      <c r="L41" s="128" t="inlineStr">
+        <is>
+          <t>87.1</t>
+        </is>
+      </c>
+      <c r="M41" s="115" t="inlineStr">
+        <is>
+          <t>83.7</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="115" t="inlineStr">
         <is>
-          <t>2023-11-10 03:00 ven</t>
-        </is>
-      </c>
-      <c r="B42" s="127" t="n">
+          <t>2024-01-18 15:00 Thu</t>
+        </is>
+      </c>
+      <c r="B42" s="119" t="n">
+        <v>14</v>
+      </c>
+      <c r="C42" s="118" t="n">
         <v>13</v>
       </c>
-      <c r="C42" s="119" t="n">
-        <v>7</v>
-      </c>
-      <c r="D42" s="121" t="n">
-        <v>67</v>
+      <c r="D42" s="123" t="n">
+        <v>90</v>
       </c>
       <c r="E42" s="115" t="n">
         <v>0</v>
@@ -3088,9 +3088,9 @@
       <c r="F42" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G42" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G42" s="131" t="inlineStr">
+        <is>
+          <t>8e-07</t>
         </is>
       </c>
       <c r="H42" s="120" t="inlineStr">
@@ -3108,36 +3108,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K42" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L42" s="128" t="inlineStr">
-        <is>
-          <t>94.2</t>
+      <c r="K42" s="125" t="inlineStr">
+        <is>
+          <t>7.8</t>
+        </is>
+      </c>
+      <c r="L42" s="129" t="inlineStr">
+        <is>
+          <t>69.9</t>
         </is>
       </c>
       <c r="M42" s="128" t="inlineStr">
         <is>
-          <t>91.1</t>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="115" t="inlineStr">
         <is>
-          <t>2023-11-10 06:00 ven</t>
+          <t>2024-01-18 18:00 Thu</t>
         </is>
       </c>
       <c r="B43" s="119" t="n">
         <v>14</v>
       </c>
-      <c r="C43" s="119" t="n">
-        <v>8</v>
-      </c>
-      <c r="D43" s="121" t="n">
-        <v>70</v>
+      <c r="C43" s="118" t="n">
+        <v>13</v>
+      </c>
+      <c r="D43" s="123" t="n">
+        <v>93</v>
       </c>
       <c r="E43" s="115" t="n">
         <v>0</v>
@@ -3165,36 +3165,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K43" s="126" t="inlineStr">
-        <is>
-          <t>15.1</t>
-        </is>
-      </c>
-      <c r="L43" s="128" t="inlineStr">
-        <is>
-          <t>84.5</t>
+      <c r="K43" s="125" t="inlineStr">
+        <is>
+          <t>6.8</t>
+        </is>
+      </c>
+      <c r="L43" s="129" t="inlineStr">
+        <is>
+          <t>76.9</t>
         </is>
       </c>
       <c r="M43" s="128" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="115" t="inlineStr">
         <is>
-          <t>2023-11-10 09:00 ven</t>
+          <t>2024-01-18 21:00 Thu</t>
         </is>
       </c>
       <c r="B44" s="119" t="n">
-        <v>19</v>
-      </c>
-      <c r="C44" s="119" t="n">
-        <v>10</v>
-      </c>
-      <c r="D44" s="119" t="n">
-        <v>55</v>
+        <v>14</v>
+      </c>
+      <c r="C44" s="118" t="n">
+        <v>13</v>
+      </c>
+      <c r="D44" s="123" t="n">
+        <v>92</v>
       </c>
       <c r="E44" s="115" t="n">
         <v>0</v>
@@ -3222,36 +3222,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K44" s="129" t="inlineStr">
-        <is>
-          <t>68.2</t>
-        </is>
-      </c>
-      <c r="L44" s="128" t="inlineStr">
-        <is>
-          <t>97</t>
+      <c r="K44" s="126" t="inlineStr">
+        <is>
+          <t>19.1</t>
+        </is>
+      </c>
+      <c r="L44" s="120" t="inlineStr">
+        <is>
+          <t>1.6</t>
         </is>
       </c>
       <c r="M44" s="128" t="inlineStr">
         <is>
-          <t>99.9</t>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="115" t="inlineStr">
         <is>
-          <t>2023-11-10 12:00 ven</t>
-        </is>
-      </c>
-      <c r="B45" s="119" t="n">
-        <v>19</v>
-      </c>
-      <c r="C45" s="118" t="n">
+          <t>2024-01-19 00:00 Fri</t>
+        </is>
+      </c>
+      <c r="B45" s="127" t="n">
         <v>13</v>
       </c>
-      <c r="D45" s="121" t="n">
-        <v>65</v>
+      <c r="C45" s="117" t="n">
+        <v>11</v>
+      </c>
+      <c r="D45" s="123" t="n">
+        <v>90</v>
       </c>
       <c r="E45" s="115" t="n">
         <v>0</v>
@@ -3259,9 +3259,9 @@
       <c r="F45" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G45" s="131" t="inlineStr">
-        <is>
-          <t>5.92e-05</t>
+      <c r="G45" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H45" s="120" t="inlineStr">
@@ -3279,19 +3279,19 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K45" s="128" t="inlineStr">
-        <is>
-          <t>81.5</t>
-        </is>
-      </c>
-      <c r="L45" s="128" t="inlineStr">
-        <is>
-          <t>89.9</t>
+      <c r="K45" s="126" t="inlineStr">
+        <is>
+          <t>10.5</t>
+        </is>
+      </c>
+      <c r="L45" s="126" t="inlineStr">
+        <is>
+          <t>15.8</t>
         </is>
       </c>
       <c r="M45" s="128" t="inlineStr">
         <is>
-          <t>98.5</t>
+          <t>100</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
- Improved Heat index calculation - Modified scale rain from 5 to 2.5 mm
</commit_message>
<xml_diff>
--- a/data/simpleWeather.xlsx
+++ b/data/simpleWeather.xlsx
@@ -790,17 +790,17 @@
     <row r="2">
       <c r="A2" s="115" t="inlineStr">
         <is>
-          <t>2024-01-13 15:00 Sat</t>
+          <t>2024-01-14 03:00 Sun</t>
         </is>
       </c>
       <c r="B2" s="121" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C2" s="121" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" s="119" t="n">
-        <v>58</v>
+        <v>1</v>
+      </c>
+      <c r="D2" s="123" t="n">
+        <v>80</v>
       </c>
       <c r="E2" s="115" t="n">
         <v>0</v>
@@ -828,9 +828,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K2" s="126" t="inlineStr">
-        <is>
-          <t>17.8</t>
+      <c r="K2" s="120" t="inlineStr">
+        <is>
+          <t>5</t>
         </is>
       </c>
       <c r="L2" s="115" t="inlineStr">
@@ -847,17 +847,17 @@
     <row r="3">
       <c r="A3" s="115" t="inlineStr">
         <is>
-          <t>2024-01-13 18:00 Sat</t>
+          <t>2024-01-14 06:00 Sun</t>
         </is>
       </c>
       <c r="B3" s="121" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="121" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="121" t="n">
-        <v>69</v>
+      <c r="D3" s="123" t="n">
+        <v>75</v>
       </c>
       <c r="E3" s="115" t="n">
         <v>0</v>
@@ -885,9 +885,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K3" s="126" t="inlineStr">
-        <is>
-          <t>10.7</t>
+      <c r="K3" s="120" t="inlineStr">
+        <is>
+          <t>3.4</t>
         </is>
       </c>
       <c r="L3" s="115" t="inlineStr">
@@ -904,17 +904,17 @@
     <row r="4">
       <c r="A4" s="115" t="inlineStr">
         <is>
-          <t>2024-01-13 21:00 Sat</t>
+          <t>2024-01-14 09:00 Sun</t>
         </is>
       </c>
       <c r="B4" s="121" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C4" s="121" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="123" t="n">
-        <v>75</v>
+        <v>1</v>
+      </c>
+      <c r="D4" s="119" t="n">
+        <v>60</v>
       </c>
       <c r="E4" s="115" t="n">
         <v>0</v>
@@ -942,9 +942,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K4" s="120" t="inlineStr">
-        <is>
-          <t>4.9</t>
+      <c r="K4" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L4" s="115" t="inlineStr">
@@ -961,17 +961,17 @@
     <row r="5">
       <c r="A5" s="115" t="inlineStr">
         <is>
-          <t>2024-01-14 00:00 Sun</t>
-        </is>
-      </c>
-      <c r="B5" s="121" t="n">
-        <v>4</v>
+          <t>2024-01-14 12:00 Sun</t>
+        </is>
+      </c>
+      <c r="B5" s="127" t="n">
+        <v>12</v>
       </c>
       <c r="C5" s="121" t="n">
         <v>0</v>
       </c>
-      <c r="D5" s="123" t="n">
-        <v>74</v>
+      <c r="D5" s="119" t="n">
+        <v>44</v>
       </c>
       <c r="E5" s="115" t="n">
         <v>0</v>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K5" s="120" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="L5" s="115" t="inlineStr">
@@ -1018,17 +1018,17 @@
     <row r="6">
       <c r="A6" s="115" t="inlineStr">
         <is>
-          <t>2024-01-14 03:00 Sun</t>
+          <t>2024-01-14 15:00 Sun</t>
         </is>
       </c>
       <c r="B6" s="121" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C6" s="121" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" s="123" t="n">
-        <v>80</v>
+        <v>3</v>
+      </c>
+      <c r="D6" s="121" t="n">
+        <v>62</v>
       </c>
       <c r="E6" s="115" t="n">
         <v>0</v>
@@ -1056,9 +1056,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K6" s="120" t="inlineStr">
-        <is>
-          <t>0.1</t>
+      <c r="K6" s="130" t="inlineStr">
+        <is>
+          <t>33.5</t>
         </is>
       </c>
       <c r="L6" s="115" t="inlineStr">
@@ -1066,26 +1066,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M6" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M6" s="120" t="inlineStr">
+        <is>
+          <t>0.4</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="115" t="inlineStr">
         <is>
-          <t>2024-01-14 06:00 Sun</t>
+          <t>2024-01-14 18:00 Sun</t>
         </is>
       </c>
       <c r="B7" s="121" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C7" s="121" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="123" t="n">
-        <v>78</v>
+        <v>2</v>
+      </c>
+      <c r="D7" s="121" t="n">
+        <v>66</v>
       </c>
       <c r="E7" s="115" t="n">
         <v>0</v>
@@ -1113,9 +1113,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K7" s="120" t="inlineStr">
-        <is>
-          <t>0.9</t>
+      <c r="K7" s="130" t="inlineStr">
+        <is>
+          <t>52.8</t>
         </is>
       </c>
       <c r="L7" s="115" t="inlineStr">
@@ -1123,26 +1123,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M7" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M7" s="126" t="inlineStr">
+        <is>
+          <t>18.5</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="115" t="inlineStr">
         <is>
-          <t>2024-01-14 09:00 Sun</t>
+          <t>2024-01-14 21:00 Sun</t>
         </is>
       </c>
       <c r="B8" s="121" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8" s="121" t="n">
-        <v>2</v>
-      </c>
-      <c r="D8" s="119" t="n">
-        <v>59</v>
+        <v>3</v>
+      </c>
+      <c r="D8" s="123" t="n">
+        <v>73</v>
       </c>
       <c r="E8" s="115" t="n">
         <v>0</v>
@@ -1170,36 +1170,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K8" s="120" t="inlineStr">
-        <is>
-          <t>2.6</t>
-        </is>
-      </c>
-      <c r="L8" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M8" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K8" s="127" t="inlineStr">
+        <is>
+          <t>28.9</t>
+        </is>
+      </c>
+      <c r="L8" s="125" t="inlineStr">
+        <is>
+          <t>8.4</t>
+        </is>
+      </c>
+      <c r="M8" s="129" t="inlineStr">
+        <is>
+          <t>69.5</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="115" t="inlineStr">
         <is>
-          <t>2024-01-14 12:00 Sun</t>
+          <t>2024-01-15 00:00 Mon</t>
         </is>
       </c>
       <c r="B9" s="121" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" s="121" t="n">
-        <v>2</v>
-      </c>
-      <c r="D9" s="119" t="n">
-        <v>55</v>
+        <v>4</v>
+      </c>
+      <c r="D9" s="123" t="n">
+        <v>77</v>
       </c>
       <c r="E9" s="115" t="n">
         <v>0</v>
@@ -1227,36 +1227,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K9" s="120" t="inlineStr">
-        <is>
-          <t>3.6</t>
-        </is>
-      </c>
-      <c r="L9" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M9" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K9" s="126" t="inlineStr">
+        <is>
+          <t>16.9</t>
+        </is>
+      </c>
+      <c r="L9" s="125" t="inlineStr">
+        <is>
+          <t>6.8</t>
+        </is>
+      </c>
+      <c r="M9" s="130" t="inlineStr">
+        <is>
+          <t>41.2</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="115" t="inlineStr">
         <is>
-          <t>2024-01-14 15:00 Sun</t>
+          <t>2024-01-15 03:00 Mon</t>
         </is>
       </c>
       <c r="B10" s="121" t="n">
-        <v>9</v>
-      </c>
-      <c r="C10" s="121" t="n">
-        <v>2</v>
-      </c>
-      <c r="D10" s="121" t="n">
-        <v>62</v>
+        <v>10</v>
+      </c>
+      <c r="C10" s="119" t="n">
+        <v>7</v>
+      </c>
+      <c r="D10" s="123" t="n">
+        <v>82</v>
       </c>
       <c r="E10" s="115" t="n">
         <v>0</v>
@@ -1264,9 +1264,9 @@
       <c r="F10" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G10" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G10" s="131" t="inlineStr">
+        <is>
+          <t>1.6e-06</t>
         </is>
       </c>
       <c r="H10" s="120" t="inlineStr">
@@ -1284,36 +1284,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K10" s="120" t="inlineStr">
-        <is>
-          <t>0.4</t>
-        </is>
-      </c>
-      <c r="L10" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M10" s="120" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="K10" s="126" t="inlineStr">
+        <is>
+          <t>19.9</t>
+        </is>
+      </c>
+      <c r="L10" s="129" t="inlineStr">
+        <is>
+          <t>76.8</t>
+        </is>
+      </c>
+      <c r="M10" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="115" t="inlineStr">
         <is>
-          <t>2024-01-14 18:00 Sun</t>
+          <t>2024-01-15 06:00 Mon</t>
         </is>
       </c>
       <c r="B11" s="121" t="n">
-        <v>7</v>
-      </c>
-      <c r="C11" s="121" t="n">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="C11" s="119" t="n">
+        <v>8</v>
       </c>
       <c r="D11" s="123" t="n">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="E11" s="115" t="n">
         <v>0</v>
@@ -1321,14 +1321,14 @@
       <c r="F11" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G11" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H11" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G11" s="131" t="inlineStr">
+        <is>
+          <t>0.000124</t>
+        </is>
+      </c>
+      <c r="H11" s="119" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I11" s="120" t="inlineStr">
@@ -1341,36 +1341,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K11" s="120" t="inlineStr">
-        <is>
-          <t>3.5</t>
-        </is>
-      </c>
-      <c r="L11" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M11" s="126" t="inlineStr">
-        <is>
-          <t>17</t>
+      <c r="K11" s="130" t="inlineStr">
+        <is>
+          <t>59.1</t>
+        </is>
+      </c>
+      <c r="L11" s="128" t="inlineStr">
+        <is>
+          <t>88.4</t>
+        </is>
+      </c>
+      <c r="M11" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="115" t="inlineStr">
         <is>
-          <t>2024-01-14 21:00 Sun</t>
-        </is>
-      </c>
-      <c r="B12" s="121" t="n">
-        <v>8</v>
-      </c>
-      <c r="C12" s="121" t="n">
-        <v>3</v>
+          <t>2024-01-15 09:00 Mon</t>
+        </is>
+      </c>
+      <c r="B12" s="127" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" s="119" t="n">
+        <v>9</v>
       </c>
       <c r="D12" s="123" t="n">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="E12" s="115" t="n">
         <v>0</v>
@@ -1378,14 +1378,14 @@
       <c r="F12" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G12" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H12" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G12" s="131" t="inlineStr">
+        <is>
+          <t>9.68e-05</t>
+        </is>
+      </c>
+      <c r="H12" s="119" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I12" s="120" t="inlineStr">
@@ -1398,36 +1398,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K12" s="120" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="L12" s="129" t="inlineStr">
-        <is>
-          <t>63.4</t>
+      <c r="K12" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="L12" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
       <c r="M12" s="128" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>98</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="115" t="inlineStr">
         <is>
-          <t>2024-01-15 00:00 Mon</t>
-        </is>
-      </c>
-      <c r="B13" s="121" t="n">
-        <v>8</v>
-      </c>
-      <c r="C13" s="121" t="n">
-        <v>4</v>
+          <t>2024-01-15 12:00 Mon</t>
+        </is>
+      </c>
+      <c r="B13" s="127" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" s="119" t="n">
+        <v>9</v>
       </c>
       <c r="D13" s="123" t="n">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E13" s="115" t="n">
         <v>0</v>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="G13" s="131" t="inlineStr">
         <is>
-          <t>8.8e-06</t>
+          <t>1.2e-06</t>
         </is>
       </c>
       <c r="H13" s="120" t="inlineStr">
@@ -1455,36 +1455,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K13" s="120" t="inlineStr">
-        <is>
-          <t>5</t>
+      <c r="K13" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
       <c r="L13" s="128" t="inlineStr">
         <is>
-          <t>81.7</t>
-        </is>
-      </c>
-      <c r="M13" s="129" t="inlineStr">
-        <is>
-          <t>71.9</t>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="M13" s="128" t="inlineStr">
+        <is>
+          <t>90.9</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="115" t="inlineStr">
         <is>
-          <t>2024-01-15 03:00 Mon</t>
-        </is>
-      </c>
-      <c r="B14" s="121" t="n">
-        <v>10</v>
+          <t>2024-01-15 15:00 Mon</t>
+        </is>
+      </c>
+      <c r="B14" s="127" t="n">
+        <v>12</v>
       </c>
       <c r="C14" s="119" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D14" s="123" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E14" s="115" t="n">
         <v>0</v>
@@ -1514,34 +1514,34 @@
       </c>
       <c r="K14" s="130" t="inlineStr">
         <is>
-          <t>38.4</t>
-        </is>
-      </c>
-      <c r="L14" s="128" t="inlineStr">
-        <is>
-          <t>90.9</t>
-        </is>
-      </c>
-      <c r="M14" s="130" t="inlineStr">
-        <is>
-          <t>55.9</t>
+          <t>31.5</t>
+        </is>
+      </c>
+      <c r="L14" s="130" t="inlineStr">
+        <is>
+          <t>56.9</t>
+        </is>
+      </c>
+      <c r="M14" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="115" t="inlineStr">
         <is>
-          <t>2024-01-15 06:00 Mon</t>
-        </is>
-      </c>
-      <c r="B15" s="127" t="n">
-        <v>11</v>
+          <t>2024-01-15 18:00 Mon</t>
+        </is>
+      </c>
+      <c r="B15" s="121" t="n">
+        <v>10</v>
       </c>
       <c r="C15" s="119" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D15" s="123" t="n">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="E15" s="115" t="n">
         <v>0</v>
@@ -1549,14 +1549,14 @@
       <c r="F15" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G15" s="131" t="inlineStr">
-        <is>
-          <t>1.04e-05</t>
-        </is>
-      </c>
-      <c r="H15" s="119" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="G15" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H15" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="I15" s="120" t="inlineStr">
@@ -1569,36 +1569,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K15" s="129" t="inlineStr">
-        <is>
-          <t>69.1</t>
-        </is>
-      </c>
-      <c r="L15" s="128" t="inlineStr">
-        <is>
-          <t>91.6</t>
-        </is>
-      </c>
-      <c r="M15" s="129" t="inlineStr">
-        <is>
-          <t>66.4</t>
+      <c r="K15" s="126" t="inlineStr">
+        <is>
+          <t>17.3</t>
+        </is>
+      </c>
+      <c r="L15" s="127" t="inlineStr">
+        <is>
+          <t>28.5</t>
+        </is>
+      </c>
+      <c r="M15" s="130" t="inlineStr">
+        <is>
+          <t>52.4</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="115" t="inlineStr">
         <is>
-          <t>2024-01-15 09:00 Mon</t>
-        </is>
-      </c>
-      <c r="B16" s="127" t="n">
-        <v>13</v>
+          <t>2024-01-15 21:00 Mon</t>
+        </is>
+      </c>
+      <c r="B16" s="121" t="n">
+        <v>10</v>
       </c>
       <c r="C16" s="119" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D16" s="123" t="n">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="E16" s="115" t="n">
         <v>0</v>
@@ -1626,36 +1626,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K16" s="129" t="inlineStr">
-        <is>
-          <t>67.2</t>
-        </is>
-      </c>
-      <c r="L16" s="128" t="inlineStr">
-        <is>
-          <t>99.4</t>
-        </is>
-      </c>
-      <c r="M16" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="K16" s="120" t="inlineStr">
+        <is>
+          <t>3.3</t>
+        </is>
+      </c>
+      <c r="L16" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M16" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="115" t="inlineStr">
         <is>
-          <t>2024-01-15 12:00 Mon</t>
-        </is>
-      </c>
-      <c r="B17" s="127" t="n">
-        <v>12</v>
+          <t>2024-01-16 00:00 Tue</t>
+        </is>
+      </c>
+      <c r="B17" s="121" t="n">
+        <v>10</v>
       </c>
       <c r="C17" s="119" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" s="123" t="n">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E17" s="115" t="n">
         <v>0</v>
@@ -1663,9 +1663,9 @@
       <c r="F17" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G17" s="131" t="inlineStr">
-        <is>
-          <t>2e-06</t>
+      <c r="G17" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H17" s="120" t="inlineStr">
@@ -1683,36 +1683,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K17" s="129" t="inlineStr">
-        <is>
-          <t>63.7</t>
-        </is>
-      </c>
-      <c r="L17" s="128" t="inlineStr">
-        <is>
-          <t>80.9</t>
-        </is>
-      </c>
-      <c r="M17" s="128" t="inlineStr">
-        <is>
-          <t>99.7</t>
+      <c r="K17" s="120" t="inlineStr">
+        <is>
+          <t>2.8</t>
+        </is>
+      </c>
+      <c r="L17" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M17" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="115" t="inlineStr">
         <is>
-          <t>2024-01-15 15:00 Mon</t>
-        </is>
-      </c>
-      <c r="B18" s="127" t="n">
-        <v>12</v>
+          <t>2024-01-16 03:00 Tue</t>
+        </is>
+      </c>
+      <c r="B18" s="121" t="n">
+        <v>10</v>
       </c>
       <c r="C18" s="119" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D18" s="123" t="n">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E18" s="115" t="n">
         <v>0</v>
@@ -1740,36 +1740,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K18" s="129" t="inlineStr">
-        <is>
-          <t>63.3</t>
-        </is>
-      </c>
-      <c r="L18" s="130" t="inlineStr">
-        <is>
-          <t>35.3</t>
-        </is>
-      </c>
-      <c r="M18" s="130" t="inlineStr">
-        <is>
-          <t>55.5</t>
+      <c r="K18" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L18" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M18" s="120" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="115" t="inlineStr">
         <is>
-          <t>2024-01-15 18:00 Mon</t>
+          <t>2024-01-16 06:00 Tue</t>
         </is>
       </c>
       <c r="B19" s="121" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" s="119" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D19" s="123" t="n">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E19" s="115" t="n">
         <v>0</v>
@@ -1797,36 +1797,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K19" s="130" t="inlineStr">
-        <is>
-          <t>35.1</t>
-        </is>
-      </c>
-      <c r="L19" s="126" t="inlineStr">
-        <is>
-          <t>17.6</t>
-        </is>
-      </c>
-      <c r="M19" s="127" t="inlineStr">
-        <is>
-          <t>28.3</t>
+      <c r="K19" s="120" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="L19" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M19" s="120" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="115" t="inlineStr">
         <is>
-          <t>2024-01-15 21:00 Mon</t>
+          <t>2024-01-16 09:00 Tue</t>
         </is>
       </c>
       <c r="B20" s="127" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C20" s="119" t="n">
-        <v>9</v>
-      </c>
-      <c r="D20" s="123" t="n">
-        <v>89</v>
+        <v>8</v>
+      </c>
+      <c r="D20" s="121" t="n">
+        <v>68</v>
       </c>
       <c r="E20" s="115" t="n">
         <v>0</v>
@@ -1854,9 +1854,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K20" s="120" t="inlineStr">
-        <is>
-          <t>5</t>
+      <c r="K20" s="126" t="inlineStr">
+        <is>
+          <t>13.7</t>
         </is>
       </c>
       <c r="L20" s="115" t="inlineStr">
@@ -1873,17 +1873,17 @@
     <row r="21">
       <c r="A21" s="115" t="inlineStr">
         <is>
-          <t>2024-01-16 00:00 Tue</t>
-        </is>
-      </c>
-      <c r="B21" s="127" t="n">
-        <v>11</v>
+          <t>2024-01-16 12:00 Tue</t>
+        </is>
+      </c>
+      <c r="B21" s="119" t="n">
+        <v>15</v>
       </c>
       <c r="C21" s="119" t="n">
-        <v>9</v>
-      </c>
-      <c r="D21" s="123" t="n">
-        <v>90</v>
+        <v>8</v>
+      </c>
+      <c r="D21" s="119" t="n">
+        <v>59</v>
       </c>
       <c r="E21" s="115" t="n">
         <v>0</v>
@@ -1891,9 +1891,9 @@
       <c r="F21" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G21" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G21" s="131" t="inlineStr">
+        <is>
+          <t>5.6e-06</t>
         </is>
       </c>
       <c r="H21" s="120" t="inlineStr">
@@ -1911,9 +1911,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K21" s="120" t="inlineStr">
-        <is>
-          <t>2.5</t>
+      <c r="K21" s="126" t="inlineStr">
+        <is>
+          <t>19.8</t>
         </is>
       </c>
       <c r="L21" s="115" t="inlineStr">
@@ -1930,17 +1930,17 @@
     <row r="22">
       <c r="A22" s="115" t="inlineStr">
         <is>
-          <t>2024-01-16 03:00 Tue</t>
-        </is>
-      </c>
-      <c r="B22" s="121" t="n">
-        <v>10</v>
+          <t>2024-01-16 15:00 Tue</t>
+        </is>
+      </c>
+      <c r="B22" s="119" t="n">
+        <v>14</v>
       </c>
       <c r="C22" s="119" t="n">
         <v>9</v>
       </c>
       <c r="D22" s="123" t="n">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="E22" s="115" t="n">
         <v>0</v>
@@ -1968,14 +1968,14 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K22" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L22" s="120" t="inlineStr">
-        <is>
-          <t>0.1</t>
+      <c r="K22" s="126" t="inlineStr">
+        <is>
+          <t>10.4</t>
+        </is>
+      </c>
+      <c r="L22" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="M22" s="115" t="inlineStr">
@@ -1987,14 +1987,14 @@
     <row r="23">
       <c r="A23" s="115" t="inlineStr">
         <is>
-          <t>2024-01-16 06:00 Tue</t>
-        </is>
-      </c>
-      <c r="B23" s="121" t="n">
+          <t>2024-01-16 18:00 Tue</t>
+        </is>
+      </c>
+      <c r="B23" s="127" t="n">
+        <v>11</v>
+      </c>
+      <c r="C23" s="119" t="n">
         <v>9</v>
-      </c>
-      <c r="C23" s="119" t="n">
-        <v>7</v>
       </c>
       <c r="D23" s="123" t="n">
         <v>86</v>
@@ -2025,9 +2025,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K23" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K23" s="130" t="inlineStr">
+        <is>
+          <t>39.1</t>
         </is>
       </c>
       <c r="L23" s="115" t="inlineStr">
@@ -2035,26 +2035,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M23" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M23" s="120" t="inlineStr">
+        <is>
+          <t>1.7</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="115" t="inlineStr">
         <is>
-          <t>2024-01-16 09:00 Tue</t>
-        </is>
-      </c>
-      <c r="B24" s="119" t="n">
-        <v>14</v>
+          <t>2024-01-16 21:00 Tue</t>
+        </is>
+      </c>
+      <c r="B24" s="127" t="n">
+        <v>12</v>
       </c>
       <c r="C24" s="119" t="n">
-        <v>7</v>
-      </c>
-      <c r="D24" s="121" t="n">
-        <v>63</v>
+        <v>10</v>
+      </c>
+      <c r="D24" s="123" t="n">
+        <v>85</v>
       </c>
       <c r="E24" s="115" t="n">
         <v>0</v>
@@ -2062,9 +2062,9 @@
       <c r="F24" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G24" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G24" s="131" t="inlineStr">
+        <is>
+          <t>8.8e-06</t>
         </is>
       </c>
       <c r="H24" s="120" t="inlineStr">
@@ -2082,9 +2082,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K24" s="120" t="inlineStr">
-        <is>
-          <t>4.1</t>
+      <c r="K24" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
       <c r="L24" s="115" t="inlineStr">
@@ -2092,26 +2092,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M24" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M24" s="120" t="inlineStr">
+        <is>
+          <t>1.6</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="115" t="inlineStr">
         <is>
-          <t>2024-01-16 12:00 Tue</t>
-        </is>
-      </c>
-      <c r="B25" s="119" t="n">
-        <v>15</v>
+          <t>2024-01-17 00:00 Wed</t>
+        </is>
+      </c>
+      <c r="B25" s="127" t="n">
+        <v>12</v>
       </c>
       <c r="C25" s="119" t="n">
-        <v>6</v>
-      </c>
-      <c r="D25" s="119" t="n">
-        <v>55</v>
+        <v>9</v>
+      </c>
+      <c r="D25" s="123" t="n">
+        <v>84</v>
       </c>
       <c r="E25" s="115" t="n">
         <v>0</v>
@@ -2139,9 +2139,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K25" s="125" t="inlineStr">
-        <is>
-          <t>6.6</t>
+      <c r="K25" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
       <c r="L25" s="115" t="inlineStr">
@@ -2149,26 +2149,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M25" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M25" s="120" t="inlineStr">
+        <is>
+          <t>0.7</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="115" t="inlineStr">
         <is>
-          <t>2024-01-16 15:00 Tue</t>
-        </is>
-      </c>
-      <c r="B26" s="119" t="n">
-        <v>14</v>
+          <t>2024-01-17 03:00 Wed</t>
+        </is>
+      </c>
+      <c r="B26" s="127" t="n">
+        <v>12</v>
       </c>
       <c r="C26" s="119" t="n">
         <v>8</v>
       </c>
-      <c r="D26" s="121" t="n">
-        <v>69</v>
+      <c r="D26" s="123" t="n">
+        <v>75</v>
       </c>
       <c r="E26" s="115" t="n">
         <v>0</v>
@@ -2196,9 +2196,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K26" s="129" t="inlineStr">
-        <is>
-          <t>75</t>
+      <c r="K26" s="128" t="inlineStr">
+        <is>
+          <t>98.6</t>
         </is>
       </c>
       <c r="L26" s="115" t="inlineStr">
@@ -2215,17 +2215,17 @@
     <row r="27">
       <c r="A27" s="115" t="inlineStr">
         <is>
-          <t>2024-01-16 18:00 Tue</t>
-        </is>
-      </c>
-      <c r="B27" s="127" t="n">
-        <v>12</v>
+          <t>2024-01-17 06:00 Wed</t>
+        </is>
+      </c>
+      <c r="B27" s="121" t="n">
+        <v>10</v>
       </c>
       <c r="C27" s="119" t="n">
         <v>8</v>
       </c>
       <c r="D27" s="123" t="n">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E27" s="115" t="n">
         <v>0</v>
@@ -2253,9 +2253,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K27" s="128" t="inlineStr">
-        <is>
-          <t>87.5</t>
+      <c r="K27" s="129" t="inlineStr">
+        <is>
+          <t>74.7</t>
         </is>
       </c>
       <c r="L27" s="115" t="inlineStr">
@@ -2263,26 +2263,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M27" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M27" s="126" t="inlineStr">
+        <is>
+          <t>16.5</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="115" t="inlineStr">
         <is>
-          <t>2024-01-16 21:00 Tue</t>
-        </is>
-      </c>
-      <c r="B28" s="127" t="n">
-        <v>12</v>
+          <t>2024-01-17 09:00 Wed</t>
+        </is>
+      </c>
+      <c r="B28" s="119" t="n">
+        <v>14</v>
       </c>
       <c r="C28" s="119" t="n">
         <v>8</v>
       </c>
-      <c r="D28" s="123" t="n">
-        <v>75</v>
+      <c r="D28" s="121" t="n">
+        <v>67</v>
       </c>
       <c r="E28" s="115" t="n">
         <v>0</v>
@@ -2310,9 +2310,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K28" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="K28" s="127" t="inlineStr">
+        <is>
+          <t>27.6</t>
         </is>
       </c>
       <c r="L28" s="115" t="inlineStr">
@@ -2322,24 +2322,24 @@
       </c>
       <c r="M28" s="120" t="inlineStr">
         <is>
-          <t>0.5</t>
+          <t>4.9</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="115" t="inlineStr">
         <is>
-          <t>2024-01-17 00:00 Wed</t>
-        </is>
-      </c>
-      <c r="B29" s="127" t="n">
-        <v>11</v>
+          <t>2024-01-17 12:00 Wed</t>
+        </is>
+      </c>
+      <c r="B29" s="119" t="n">
+        <v>16</v>
       </c>
       <c r="C29" s="119" t="n">
-        <v>8</v>
-      </c>
-      <c r="D29" s="123" t="n">
-        <v>83</v>
+        <v>7</v>
+      </c>
+      <c r="D29" s="119" t="n">
+        <v>55</v>
       </c>
       <c r="E29" s="115" t="n">
         <v>0</v>
@@ -2367,9 +2367,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K29" s="129" t="inlineStr">
-        <is>
-          <t>68.6</t>
+      <c r="K29" s="126" t="inlineStr">
+        <is>
+          <t>14.1</t>
         </is>
       </c>
       <c r="L29" s="115" t="inlineStr">
@@ -2377,26 +2377,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M29" s="120" t="inlineStr">
-        <is>
-          <t>0.2</t>
+      <c r="M29" s="125" t="inlineStr">
+        <is>
+          <t>6</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="115" t="inlineStr">
         <is>
-          <t>2024-01-17 03:00 Wed</t>
-        </is>
-      </c>
-      <c r="B30" s="121" t="n">
-        <v>10</v>
+          <t>2024-01-17 15:00 Wed</t>
+        </is>
+      </c>
+      <c r="B30" s="119" t="n">
+        <v>14</v>
       </c>
       <c r="C30" s="119" t="n">
-        <v>7</v>
-      </c>
-      <c r="D30" s="123" t="n">
-        <v>84</v>
+        <v>8</v>
+      </c>
+      <c r="D30" s="121" t="n">
+        <v>69</v>
       </c>
       <c r="E30" s="115" t="n">
         <v>0</v>
@@ -2426,7 +2426,7 @@
       </c>
       <c r="K30" s="120" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="L30" s="115" t="inlineStr">
@@ -2434,26 +2434,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M30" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M30" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="115" t="inlineStr">
         <is>
-          <t>2024-01-17 06:00 Wed</t>
+          <t>2024-01-17 18:00 Wed</t>
         </is>
       </c>
       <c r="B31" s="121" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C31" s="119" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D31" s="123" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E31" s="115" t="n">
         <v>0</v>
@@ -2483,7 +2483,7 @@
       </c>
       <c r="K31" s="120" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>0.1</t>
         </is>
       </c>
       <c r="L31" s="115" t="inlineStr">
@@ -2491,26 +2491,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M31" s="120" t="inlineStr">
-        <is>
-          <t>1.7</t>
+      <c r="M31" s="128" t="inlineStr">
+        <is>
+          <t>86.6</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="115" t="inlineStr">
         <is>
-          <t>2024-01-17 09:00 Wed</t>
-        </is>
-      </c>
-      <c r="B32" s="119" t="n">
-        <v>14</v>
+          <t>2024-01-17 21:00 Wed</t>
+        </is>
+      </c>
+      <c r="B32" s="127" t="n">
+        <v>11</v>
       </c>
       <c r="C32" s="119" t="n">
-        <v>8</v>
-      </c>
-      <c r="D32" s="121" t="n">
-        <v>68</v>
+        <v>9</v>
+      </c>
+      <c r="D32" s="123" t="n">
+        <v>88</v>
       </c>
       <c r="E32" s="115" t="n">
         <v>0</v>
@@ -2548,26 +2548,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M32" s="125" t="inlineStr">
-        <is>
-          <t>5.4</t>
+      <c r="M32" s="128" t="inlineStr">
+        <is>
+          <t>87.9</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="115" t="inlineStr">
         <is>
-          <t>2024-01-17 12:00 Wed</t>
-        </is>
-      </c>
-      <c r="B33" s="119" t="n">
-        <v>15</v>
-      </c>
-      <c r="C33" s="119" t="n">
-        <v>7</v>
-      </c>
-      <c r="D33" s="119" t="n">
-        <v>56</v>
+          <t>2024-01-18 00:00 Thu</t>
+        </is>
+      </c>
+      <c r="B33" s="127" t="n">
+        <v>12</v>
+      </c>
+      <c r="C33" s="117" t="n">
+        <v>11</v>
+      </c>
+      <c r="D33" s="123" t="n">
+        <v>90</v>
       </c>
       <c r="E33" s="115" t="n">
         <v>0</v>
@@ -2595,36 +2595,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K33" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L33" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M33" s="130" t="inlineStr">
-        <is>
-          <t>38.8</t>
+      <c r="K33" s="120" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="L33" s="126" t="inlineStr">
+        <is>
+          <t>18.8</t>
+        </is>
+      </c>
+      <c r="M33" s="128" t="inlineStr">
+        <is>
+          <t>94</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="115" t="inlineStr">
         <is>
-          <t>2024-01-17 15:00 Wed</t>
+          <t>2024-01-18 03:00 Thu</t>
         </is>
       </c>
       <c r="B34" s="127" t="n">
         <v>13</v>
       </c>
-      <c r="C34" s="119" t="n">
-        <v>8</v>
-      </c>
-      <c r="D34" s="121" t="n">
-        <v>67</v>
+      <c r="C34" s="117" t="n">
+        <v>11</v>
+      </c>
+      <c r="D34" s="123" t="n">
+        <v>89</v>
       </c>
       <c r="E34" s="115" t="n">
         <v>0</v>
@@ -2632,14 +2632,14 @@
       <c r="F34" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G34" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H34" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G34" s="131" t="inlineStr">
+        <is>
+          <t>3.2e-05</t>
+        </is>
+      </c>
+      <c r="H34" s="119" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I34" s="120" t="inlineStr">
@@ -2652,36 +2652,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K34" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L34" s="120" t="inlineStr">
-        <is>
-          <t>2.7</t>
-        </is>
-      </c>
-      <c r="M34" s="129" t="inlineStr">
-        <is>
-          <t>77.9</t>
+      <c r="K34" s="126" t="inlineStr">
+        <is>
+          <t>17.4</t>
+        </is>
+      </c>
+      <c r="L34" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="M34" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="115" t="inlineStr">
         <is>
-          <t>2024-01-17 18:00 Wed</t>
+          <t>2024-01-18 06:00 Thu</t>
         </is>
       </c>
       <c r="B35" s="127" t="n">
-        <v>11</v>
-      </c>
-      <c r="C35" s="119" t="n">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="C35" s="117" t="n">
+        <v>12</v>
       </c>
       <c r="D35" s="123" t="n">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="E35" s="115" t="n">
         <v>0</v>
@@ -2689,9 +2689,9 @@
       <c r="F35" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G35" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G35" s="131" t="inlineStr">
+        <is>
+          <t>3.2e-06</t>
         </is>
       </c>
       <c r="H35" s="120" t="inlineStr">
@@ -2709,36 +2709,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K35" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L35" s="126" t="inlineStr">
-        <is>
-          <t>17.8</t>
+      <c r="K35" s="130" t="inlineStr">
+        <is>
+          <t>58.6</t>
+        </is>
+      </c>
+      <c r="L35" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
       <c r="M35" s="128" t="inlineStr">
         <is>
-          <t>86.9</t>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="115" t="inlineStr">
         <is>
-          <t>2024-01-17 21:00 Wed</t>
-        </is>
-      </c>
-      <c r="B36" s="127" t="n">
-        <v>11</v>
-      </c>
-      <c r="C36" s="119" t="n">
-        <v>9</v>
+          <t>2024-01-18 09:00 Thu</t>
+        </is>
+      </c>
+      <c r="B36" s="119" t="n">
+        <v>15</v>
+      </c>
+      <c r="C36" s="117" t="n">
+        <v>12</v>
       </c>
       <c r="D36" s="123" t="n">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E36" s="115" t="n">
         <v>0</v>
@@ -2766,36 +2766,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K36" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L36" s="128" t="inlineStr">
-        <is>
-          <t>80.5</t>
+      <c r="K36" s="129" t="inlineStr">
+        <is>
+          <t>79.8</t>
+        </is>
+      </c>
+      <c r="L36" s="129" t="inlineStr">
+        <is>
+          <t>69.8</t>
         </is>
       </c>
       <c r="M36" s="129" t="inlineStr">
         <is>
-          <t>71.8</t>
+          <t>68.6</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="115" t="inlineStr">
         <is>
-          <t>2024-01-18 00:00 Thu</t>
-        </is>
-      </c>
-      <c r="B37" s="127" t="n">
+          <t>2024-01-18 12:00 Thu</t>
+        </is>
+      </c>
+      <c r="B37" s="119" t="n">
+        <v>17</v>
+      </c>
+      <c r="C37" s="117" t="n">
         <v>12</v>
       </c>
-      <c r="C37" s="117" t="n">
-        <v>11</v>
-      </c>
       <c r="D37" s="123" t="n">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="E37" s="115" t="n">
         <v>0</v>
@@ -2823,36 +2823,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K37" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K37" s="130" t="inlineStr">
+        <is>
+          <t>42.7</t>
         </is>
       </c>
       <c r="L37" s="130" t="inlineStr">
         <is>
-          <t>43.8</t>
+          <t>37.4</t>
         </is>
       </c>
       <c r="M37" s="130" t="inlineStr">
         <is>
-          <t>39.5</t>
+          <t>44.3</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="115" t="inlineStr">
         <is>
-          <t>2024-01-18 03:00 Thu</t>
-        </is>
-      </c>
-      <c r="B38" s="127" t="n">
-        <v>12</v>
-      </c>
-      <c r="C38" s="117" t="n">
-        <v>11</v>
+          <t>2024-01-18 15:00 Thu</t>
+        </is>
+      </c>
+      <c r="B38" s="119" t="n">
+        <v>15</v>
+      </c>
+      <c r="C38" s="118" t="n">
+        <v>13</v>
       </c>
       <c r="D38" s="123" t="n">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E38" s="115" t="n">
         <v>0</v>
@@ -2860,9 +2860,9 @@
       <c r="F38" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G38" s="131" t="inlineStr">
-        <is>
-          <t>8e-07</t>
+      <c r="G38" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H38" s="120" t="inlineStr">
@@ -2880,36 +2880,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K38" s="125" t="inlineStr">
-        <is>
-          <t>8.6</t>
-        </is>
-      </c>
-      <c r="L38" s="126" t="inlineStr">
-        <is>
-          <t>11.4</t>
-        </is>
-      </c>
-      <c r="M38" s="128" t="inlineStr">
-        <is>
-          <t>98.9</t>
+      <c r="K38" s="120" t="inlineStr">
+        <is>
+          <t>3.3</t>
+        </is>
+      </c>
+      <c r="L38" s="129" t="inlineStr">
+        <is>
+          <t>78.6</t>
+        </is>
+      </c>
+      <c r="M38" s="130" t="inlineStr">
+        <is>
+          <t>42.9</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="115" t="inlineStr">
         <is>
-          <t>2024-01-18 06:00 Thu</t>
-        </is>
-      </c>
-      <c r="B39" s="127" t="n">
+          <t>2024-01-18 18:00 Thu</t>
+        </is>
+      </c>
+      <c r="B39" s="119" t="n">
+        <v>14</v>
+      </c>
+      <c r="C39" s="118" t="n">
         <v>13</v>
       </c>
-      <c r="C39" s="117" t="n">
-        <v>12</v>
-      </c>
       <c r="D39" s="123" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E39" s="115" t="n">
         <v>0</v>
@@ -2917,9 +2917,9 @@
       <c r="F39" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G39" s="131" t="inlineStr">
-        <is>
-          <t>2.4e-06</t>
+      <c r="G39" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H39" s="120" t="inlineStr">
@@ -2937,36 +2937,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K39" s="130" t="inlineStr">
-        <is>
-          <t>35.2</t>
-        </is>
-      </c>
-      <c r="L39" s="130" t="inlineStr">
-        <is>
-          <t>36.6</t>
-        </is>
-      </c>
-      <c r="M39" s="128" t="inlineStr">
-        <is>
-          <t>99.5</t>
+      <c r="K39" s="126" t="inlineStr">
+        <is>
+          <t>14.4</t>
+        </is>
+      </c>
+      <c r="L39" s="129" t="inlineStr">
+        <is>
+          <t>70.3</t>
+        </is>
+      </c>
+      <c r="M39" s="129" t="inlineStr">
+        <is>
+          <t>71.4</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="115" t="inlineStr">
         <is>
-          <t>2024-01-18 09:00 Thu</t>
+          <t>2024-01-18 21:00 Thu</t>
         </is>
       </c>
       <c r="B40" s="119" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C40" s="117" t="n">
         <v>12</v>
       </c>
       <c r="D40" s="123" t="n">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E40" s="115" t="n">
         <v>0</v>
@@ -2974,9 +2974,9 @@
       <c r="F40" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G40" s="131" t="inlineStr">
-        <is>
-          <t>8e-07</t>
+      <c r="G40" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H40" s="120" t="inlineStr">
@@ -2994,14 +2994,14 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K40" s="130" t="inlineStr">
-        <is>
-          <t>51.1</t>
-        </is>
-      </c>
-      <c r="L40" s="129" t="inlineStr">
-        <is>
-          <t>79.7</t>
+      <c r="K40" s="120" t="inlineStr">
+        <is>
+          <t>0.3</t>
+        </is>
+      </c>
+      <c r="L40" s="120" t="inlineStr">
+        <is>
+          <t>4.2</t>
         </is>
       </c>
       <c r="M40" s="128" t="inlineStr">
@@ -3013,17 +3013,17 @@
     <row r="41">
       <c r="A41" s="115" t="inlineStr">
         <is>
-          <t>2024-01-18 12:00 Thu</t>
+          <t>2024-01-19 00:00 Fri</t>
         </is>
       </c>
       <c r="B41" s="119" t="n">
-        <v>16</v>
-      </c>
-      <c r="C41" s="118" t="n">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="C41" s="117" t="n">
+        <v>11</v>
       </c>
       <c r="D41" s="123" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E41" s="115" t="n">
         <v>0</v>
@@ -3031,9 +3031,9 @@
       <c r="F41" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G41" s="131" t="inlineStr">
-        <is>
-          <t>1.6e-06</t>
+      <c r="G41" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H41" s="120" t="inlineStr">
@@ -3051,36 +3051,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K41" s="130" t="inlineStr">
-        <is>
-          <t>44.6</t>
-        </is>
-      </c>
-      <c r="L41" s="128" t="inlineStr">
-        <is>
-          <t>87.1</t>
-        </is>
-      </c>
-      <c r="M41" s="115" t="inlineStr">
-        <is>
-          <t>83.7</t>
+      <c r="K41" s="120" t="inlineStr">
+        <is>
+          <t>0.1</t>
+        </is>
+      </c>
+      <c r="L41" s="130" t="inlineStr">
+        <is>
+          <t>36.6</t>
+        </is>
+      </c>
+      <c r="M41" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="115" t="inlineStr">
         <is>
-          <t>2024-01-18 15:00 Thu</t>
+          <t>2024-01-19 03:00 Fri</t>
         </is>
       </c>
       <c r="B42" s="119" t="n">
         <v>14</v>
       </c>
-      <c r="C42" s="118" t="n">
-        <v>13</v>
+      <c r="C42" s="117" t="n">
+        <v>11</v>
       </c>
       <c r="D42" s="123" t="n">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="E42" s="115" t="n">
         <v>0</v>
@@ -3088,9 +3088,9 @@
       <c r="F42" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G42" s="131" t="inlineStr">
-        <is>
-          <t>8e-07</t>
+      <c r="G42" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H42" s="120" t="inlineStr">
@@ -3108,36 +3108,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K42" s="125" t="inlineStr">
-        <is>
-          <t>7.8</t>
-        </is>
-      </c>
-      <c r="L42" s="129" t="inlineStr">
-        <is>
-          <t>69.9</t>
+      <c r="K42" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L42" s="130" t="inlineStr">
+        <is>
+          <t>59.6</t>
         </is>
       </c>
       <c r="M42" s="128" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>97.6</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="115" t="inlineStr">
         <is>
-          <t>2024-01-18 18:00 Thu</t>
-        </is>
-      </c>
-      <c r="B43" s="119" t="n">
-        <v>14</v>
-      </c>
-      <c r="C43" s="118" t="n">
+          <t>2024-01-19 06:00 Fri</t>
+        </is>
+      </c>
+      <c r="B43" s="127" t="n">
         <v>13</v>
       </c>
+      <c r="C43" s="117" t="n">
+        <v>11</v>
+      </c>
       <c r="D43" s="123" t="n">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E43" s="115" t="n">
         <v>0</v>
@@ -3165,36 +3165,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K43" s="125" t="inlineStr">
-        <is>
-          <t>6.8</t>
-        </is>
-      </c>
-      <c r="L43" s="129" t="inlineStr">
-        <is>
-          <t>76.9</t>
-        </is>
-      </c>
-      <c r="M43" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="K43" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L43" s="130" t="inlineStr">
+        <is>
+          <t>32.4</t>
+        </is>
+      </c>
+      <c r="M43" s="115" t="inlineStr">
+        <is>
+          <t>82.9</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="115" t="inlineStr">
         <is>
-          <t>2024-01-18 21:00 Thu</t>
+          <t>2024-01-19 09:00 Fri</t>
         </is>
       </c>
       <c r="B44" s="119" t="n">
-        <v>14</v>
-      </c>
-      <c r="C44" s="118" t="n">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="C44" s="117" t="n">
+        <v>12</v>
       </c>
       <c r="D44" s="123" t="n">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="E44" s="115" t="n">
         <v>0</v>
@@ -3222,36 +3222,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K44" s="126" t="inlineStr">
-        <is>
-          <t>19.1</t>
-        </is>
-      </c>
-      <c r="L44" s="120" t="inlineStr">
-        <is>
-          <t>1.6</t>
+      <c r="K44" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L44" s="130" t="inlineStr">
+        <is>
+          <t>34.3</t>
         </is>
       </c>
       <c r="M44" s="128" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>91.7</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="115" t="inlineStr">
         <is>
-          <t>2024-01-19 00:00 Fri</t>
-        </is>
-      </c>
-      <c r="B45" s="127" t="n">
-        <v>13</v>
+          <t>2024-01-19 12:00 Fri</t>
+        </is>
+      </c>
+      <c r="B45" s="119" t="n">
+        <v>16</v>
       </c>
       <c r="C45" s="117" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D45" s="123" t="n">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E45" s="115" t="n">
         <v>0</v>
@@ -3259,9 +3259,9 @@
       <c r="F45" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G45" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G45" s="131" t="inlineStr">
+        <is>
+          <t>8e-07</t>
         </is>
       </c>
       <c r="H45" s="120" t="inlineStr">
@@ -3279,19 +3279,19 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K45" s="126" t="inlineStr">
-        <is>
-          <t>10.5</t>
-        </is>
-      </c>
-      <c r="L45" s="126" t="inlineStr">
-        <is>
-          <t>15.8</t>
+      <c r="K45" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L45" s="129" t="inlineStr">
+        <is>
+          <t>67.1</t>
         </is>
       </c>
       <c r="M45" s="128" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>95.9</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified .gitignore in a way to add xlsx files
</commit_message>
<xml_diff>
--- a/data/simpleWeather.xlsx
+++ b/data/simpleWeather.xlsx
@@ -790,17 +790,17 @@
     <row r="2">
       <c r="A2" s="115" t="inlineStr">
         <is>
-          <t>2024-01-14 03:00 Sun</t>
-        </is>
-      </c>
-      <c r="B2" s="121" t="n">
-        <v>4</v>
-      </c>
-      <c r="C2" s="121" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="123" t="n">
-        <v>80</v>
+          <t>2024-11-22 15:00 Fri</t>
+        </is>
+      </c>
+      <c r="B2" s="119" t="n">
+        <v>20</v>
+      </c>
+      <c r="C2" s="117" t="n">
+        <v>12</v>
+      </c>
+      <c r="D2" s="119" t="n">
+        <v>60</v>
       </c>
       <c r="E2" s="115" t="n">
         <v>0</v>
@@ -808,9 +808,9 @@
       <c r="F2" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G2" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G2" s="131" t="inlineStr">
+        <is>
+          <t>5.08e-05</t>
         </is>
       </c>
       <c r="H2" s="120" t="inlineStr">
@@ -828,36 +828,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K2" s="120" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="L2" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M2" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K2" s="130" t="inlineStr">
+        <is>
+          <t>38.8</t>
+        </is>
+      </c>
+      <c r="L2" s="130" t="inlineStr">
+        <is>
+          <t>30.8</t>
+        </is>
+      </c>
+      <c r="M2" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="115" t="inlineStr">
         <is>
-          <t>2024-01-14 06:00 Sun</t>
-        </is>
-      </c>
-      <c r="B3" s="121" t="n">
-        <v>4</v>
-      </c>
-      <c r="C3" s="121" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="123" t="n">
-        <v>75</v>
+          <t>2024-11-22 18:00 Fri</t>
+        </is>
+      </c>
+      <c r="B3" s="119" t="n">
+        <v>18</v>
+      </c>
+      <c r="C3" s="119" t="n">
+        <v>10</v>
+      </c>
+      <c r="D3" s="119" t="n">
+        <v>60</v>
       </c>
       <c r="E3" s="115" t="n">
         <v>0</v>
@@ -865,9 +865,9 @@
       <c r="F3" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G3" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G3" s="131" t="inlineStr">
+        <is>
+          <t>5.6e-06</t>
         </is>
       </c>
       <c r="H3" s="120" t="inlineStr">
@@ -885,36 +885,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K3" s="120" t="inlineStr">
-        <is>
-          <t>3.4</t>
-        </is>
-      </c>
-      <c r="L3" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M3" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K3" s="129" t="inlineStr">
+        <is>
+          <t>69.4</t>
+        </is>
+      </c>
+      <c r="L3" s="129" t="inlineStr">
+        <is>
+          <t>65.4</t>
+        </is>
+      </c>
+      <c r="M3" s="128" t="inlineStr">
+        <is>
+          <t>99.4</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="115" t="inlineStr">
         <is>
-          <t>2024-01-14 09:00 Sun</t>
-        </is>
-      </c>
-      <c r="B4" s="121" t="n">
-        <v>9</v>
-      </c>
-      <c r="C4" s="121" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="119" t="n">
-        <v>60</v>
+          <t>2024-11-22 21:00 Fri</t>
+        </is>
+      </c>
+      <c r="B4" s="127" t="n">
+        <v>12</v>
+      </c>
+      <c r="C4" s="119" t="n">
+        <v>7</v>
+      </c>
+      <c r="D4" s="123" t="n">
+        <v>71</v>
       </c>
       <c r="E4" s="115" t="n">
         <v>0</v>
@@ -942,9 +942,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K4" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K4" s="130" t="inlineStr">
+        <is>
+          <t>32</t>
         </is>
       </c>
       <c r="L4" s="115" t="inlineStr">
@@ -961,17 +961,17 @@
     <row r="5">
       <c r="A5" s="115" t="inlineStr">
         <is>
-          <t>2024-01-14 12:00 Sun</t>
+          <t>2024-11-23 00:00 Sat</t>
         </is>
       </c>
       <c r="B5" s="127" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="121" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="119" t="n">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E5" s="115" t="n">
         <v>0</v>
@@ -999,9 +999,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K5" s="120" t="inlineStr">
-        <is>
-          <t>0.1</t>
+      <c r="K5" s="126" t="inlineStr">
+        <is>
+          <t>16.6</t>
         </is>
       </c>
       <c r="L5" s="115" t="inlineStr">
@@ -1018,17 +1018,17 @@
     <row r="6">
       <c r="A6" s="115" t="inlineStr">
         <is>
-          <t>2024-01-14 15:00 Sun</t>
-        </is>
-      </c>
-      <c r="B6" s="121" t="n">
-        <v>10</v>
+          <t>2024-11-23 03:00 Sat</t>
+        </is>
+      </c>
+      <c r="B6" s="127" t="n">
+        <v>11</v>
       </c>
       <c r="C6" s="121" t="n">
-        <v>3</v>
-      </c>
-      <c r="D6" s="121" t="n">
-        <v>62</v>
+        <v>-1</v>
+      </c>
+      <c r="D6" s="119" t="n">
+        <v>42</v>
       </c>
       <c r="E6" s="115" t="n">
         <v>0</v>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="K6" s="130" t="inlineStr">
         <is>
-          <t>33.5</t>
+          <t>50</t>
         </is>
       </c>
       <c r="L6" s="115" t="inlineStr">
@@ -1066,26 +1066,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M6" s="120" t="inlineStr">
-        <is>
-          <t>0.4</t>
+      <c r="M6" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="115" t="inlineStr">
         <is>
-          <t>2024-01-14 18:00 Sun</t>
+          <t>2024-11-23 06:00 Sat</t>
         </is>
       </c>
       <c r="B7" s="121" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C7" s="121" t="n">
-        <v>2</v>
-      </c>
-      <c r="D7" s="121" t="n">
-        <v>66</v>
+        <v>-3</v>
+      </c>
+      <c r="D7" s="119" t="n">
+        <v>37</v>
       </c>
       <c r="E7" s="115" t="n">
         <v>0</v>
@@ -1115,34 +1115,34 @@
       </c>
       <c r="K7" s="130" t="inlineStr">
         <is>
-          <t>52.8</t>
-        </is>
-      </c>
-      <c r="L7" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M7" s="126" t="inlineStr">
-        <is>
-          <t>18.5</t>
+          <t>58.6</t>
+        </is>
+      </c>
+      <c r="L7" s="130" t="inlineStr">
+        <is>
+          <t>33.3</t>
+        </is>
+      </c>
+      <c r="M7" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="115" t="inlineStr">
         <is>
-          <t>2024-01-14 21:00 Sun</t>
-        </is>
-      </c>
-      <c r="B8" s="121" t="n">
-        <v>7</v>
+          <t>2024-11-23 09:00 Sat</t>
+        </is>
+      </c>
+      <c r="B8" s="127" t="n">
+        <v>12</v>
       </c>
       <c r="C8" s="121" t="n">
-        <v>3</v>
-      </c>
-      <c r="D8" s="123" t="n">
-        <v>73</v>
+        <v>-6</v>
+      </c>
+      <c r="D8" s="117" t="n">
+        <v>26</v>
       </c>
       <c r="E8" s="115" t="n">
         <v>0</v>
@@ -1170,36 +1170,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K8" s="127" t="inlineStr">
-        <is>
-          <t>28.9</t>
-        </is>
-      </c>
-      <c r="L8" s="125" t="inlineStr">
-        <is>
-          <t>8.4</t>
-        </is>
-      </c>
-      <c r="M8" s="129" t="inlineStr">
-        <is>
-          <t>69.5</t>
+      <c r="K8" s="120" t="inlineStr">
+        <is>
+          <t>0.4</t>
+        </is>
+      </c>
+      <c r="L8" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M8" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="115" t="inlineStr">
         <is>
-          <t>2024-01-15 00:00 Mon</t>
-        </is>
-      </c>
-      <c r="B9" s="121" t="n">
-        <v>8</v>
+          <t>2024-11-23 12:00 Sat</t>
+        </is>
+      </c>
+      <c r="B9" s="127" t="n">
+        <v>12</v>
       </c>
       <c r="C9" s="121" t="n">
-        <v>4</v>
-      </c>
-      <c r="D9" s="123" t="n">
-        <v>77</v>
+        <v>-6</v>
+      </c>
+      <c r="D9" s="117" t="n">
+        <v>26</v>
       </c>
       <c r="E9" s="115" t="n">
         <v>0</v>
@@ -1227,36 +1227,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K9" s="126" t="inlineStr">
-        <is>
-          <t>16.9</t>
-        </is>
-      </c>
-      <c r="L9" s="125" t="inlineStr">
-        <is>
-          <t>6.8</t>
-        </is>
-      </c>
-      <c r="M9" s="130" t="inlineStr">
-        <is>
-          <t>41.2</t>
+      <c r="K9" s="120" t="inlineStr">
+        <is>
+          <t>1.7</t>
+        </is>
+      </c>
+      <c r="L9" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M9" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="115" t="inlineStr">
         <is>
-          <t>2024-01-15 03:00 Mon</t>
-        </is>
-      </c>
-      <c r="B10" s="121" t="n">
-        <v>10</v>
-      </c>
-      <c r="C10" s="119" t="n">
-        <v>7</v>
-      </c>
-      <c r="D10" s="123" t="n">
-        <v>82</v>
+          <t>2024-11-23 15:00 Sat</t>
+        </is>
+      </c>
+      <c r="B10" s="127" t="n">
+        <v>11</v>
+      </c>
+      <c r="C10" s="121" t="n">
+        <v>-3</v>
+      </c>
+      <c r="D10" s="119" t="n">
+        <v>34</v>
       </c>
       <c r="E10" s="115" t="n">
         <v>0</v>
@@ -1264,9 +1264,9 @@
       <c r="F10" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G10" s="131" t="inlineStr">
-        <is>
-          <t>1.6e-06</t>
+      <c r="G10" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H10" s="120" t="inlineStr">
@@ -1284,36 +1284,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K10" s="126" t="inlineStr">
-        <is>
-          <t>19.9</t>
-        </is>
-      </c>
-      <c r="L10" s="129" t="inlineStr">
-        <is>
-          <t>76.8</t>
-        </is>
-      </c>
-      <c r="M10" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="K10" s="120" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L10" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M10" s="120" t="inlineStr">
+        <is>
+          <t>0.4</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="115" t="inlineStr">
         <is>
-          <t>2024-01-15 06:00 Mon</t>
+          <t>2024-11-23 18:00 Sat</t>
         </is>
       </c>
       <c r="B11" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="C11" s="119" t="n">
-        <v>8</v>
-      </c>
-      <c r="D11" s="123" t="n">
-        <v>86</v>
+      <c r="C11" s="121" t="n">
+        <v>-2</v>
+      </c>
+      <c r="D11" s="119" t="n">
+        <v>39</v>
       </c>
       <c r="E11" s="115" t="n">
         <v>0</v>
@@ -1321,14 +1321,14 @@
       <c r="F11" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G11" s="131" t="inlineStr">
-        <is>
-          <t>0.000124</t>
-        </is>
-      </c>
-      <c r="H11" s="119" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="G11" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H11" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="I11" s="120" t="inlineStr">
@@ -1341,36 +1341,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K11" s="130" t="inlineStr">
-        <is>
-          <t>59.1</t>
-        </is>
-      </c>
-      <c r="L11" s="128" t="inlineStr">
-        <is>
-          <t>88.4</t>
-        </is>
-      </c>
-      <c r="M11" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="K11" s="120" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
+      <c r="L11" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M11" s="120" t="inlineStr">
+        <is>
+          <t>2.7</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="115" t="inlineStr">
         <is>
-          <t>2024-01-15 09:00 Mon</t>
-        </is>
-      </c>
-      <c r="B12" s="127" t="n">
-        <v>11</v>
-      </c>
-      <c r="C12" s="119" t="n">
+          <t>2024-11-23 21:00 Sat</t>
+        </is>
+      </c>
+      <c r="B12" s="121" t="n">
         <v>9</v>
       </c>
-      <c r="D12" s="123" t="n">
-        <v>89</v>
+      <c r="C12" s="121" t="n">
+        <v>-3</v>
+      </c>
+      <c r="D12" s="119" t="n">
+        <v>39</v>
       </c>
       <c r="E12" s="115" t="n">
         <v>0</v>
@@ -1378,14 +1378,14 @@
       <c r="F12" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G12" s="131" t="inlineStr">
-        <is>
-          <t>9.68e-05</t>
-        </is>
-      </c>
-      <c r="H12" s="119" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="G12" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H12" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="I12" s="120" t="inlineStr">
@@ -1398,36 +1398,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K12" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="L12" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="M12" s="128" t="inlineStr">
-        <is>
-          <t>98</t>
+      <c r="K12" s="120" t="inlineStr">
+        <is>
+          <t>1.6</t>
+        </is>
+      </c>
+      <c r="L12" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M12" s="120" t="inlineStr">
+        <is>
+          <t>1.6</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="115" t="inlineStr">
         <is>
-          <t>2024-01-15 12:00 Mon</t>
-        </is>
-      </c>
-      <c r="B13" s="127" t="n">
-        <v>12</v>
-      </c>
-      <c r="C13" s="119" t="n">
-        <v>9</v>
-      </c>
-      <c r="D13" s="123" t="n">
-        <v>82</v>
+          <t>2024-11-24 00:00 Sun</t>
+        </is>
+      </c>
+      <c r="B13" s="121" t="n">
+        <v>8</v>
+      </c>
+      <c r="C13" s="121" t="n">
+        <v>-4</v>
+      </c>
+      <c r="D13" s="119" t="n">
+        <v>38</v>
       </c>
       <c r="E13" s="115" t="n">
         <v>0</v>
@@ -1435,9 +1435,9 @@
       <c r="F13" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G13" s="131" t="inlineStr">
-        <is>
-          <t>1.2e-06</t>
+      <c r="G13" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H13" s="120" t="inlineStr">
@@ -1455,36 +1455,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K13" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="L13" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="M13" s="128" t="inlineStr">
-        <is>
-          <t>90.9</t>
+      <c r="K13" s="120" t="inlineStr">
+        <is>
+          <t>0.8</t>
+        </is>
+      </c>
+      <c r="L13" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M13" s="120" t="inlineStr">
+        <is>
+          <t>0.8</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="115" t="inlineStr">
         <is>
-          <t>2024-01-15 15:00 Mon</t>
-        </is>
-      </c>
-      <c r="B14" s="127" t="n">
-        <v>12</v>
-      </c>
-      <c r="C14" s="119" t="n">
-        <v>9</v>
-      </c>
-      <c r="D14" s="123" t="n">
-        <v>82</v>
+          <t>2024-11-24 03:00 Sun</t>
+        </is>
+      </c>
+      <c r="B14" s="121" t="n">
+        <v>8</v>
+      </c>
+      <c r="C14" s="121" t="n">
+        <v>-4</v>
+      </c>
+      <c r="D14" s="119" t="n">
+        <v>39</v>
       </c>
       <c r="E14" s="115" t="n">
         <v>0</v>
@@ -1512,36 +1512,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K14" s="130" t="inlineStr">
-        <is>
-          <t>31.5</t>
-        </is>
-      </c>
-      <c r="L14" s="130" t="inlineStr">
-        <is>
-          <t>56.9</t>
-        </is>
-      </c>
-      <c r="M14" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="K14" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L14" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M14" s="120" t="inlineStr">
+        <is>
+          <t>1.6</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="115" t="inlineStr">
         <is>
-          <t>2024-01-15 18:00 Mon</t>
+          <t>2024-11-24 06:00 Sun</t>
         </is>
       </c>
       <c r="B15" s="121" t="n">
-        <v>10</v>
-      </c>
-      <c r="C15" s="119" t="n">
-        <v>9</v>
-      </c>
-      <c r="D15" s="123" t="n">
-        <v>92</v>
+        <v>8</v>
+      </c>
+      <c r="C15" s="121" t="n">
+        <v>-3</v>
+      </c>
+      <c r="D15" s="119" t="n">
+        <v>43</v>
       </c>
       <c r="E15" s="115" t="n">
         <v>0</v>
@@ -1569,36 +1569,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K15" s="126" t="inlineStr">
-        <is>
-          <t>17.3</t>
-        </is>
-      </c>
-      <c r="L15" s="127" t="inlineStr">
-        <is>
-          <t>28.5</t>
+      <c r="K15" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L15" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="M15" s="130" t="inlineStr">
         <is>
-          <t>52.4</t>
+          <t>30.9</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="115" t="inlineStr">
         <is>
-          <t>2024-01-15 21:00 Mon</t>
-        </is>
-      </c>
-      <c r="B16" s="121" t="n">
-        <v>10</v>
-      </c>
-      <c r="C16" s="119" t="n">
-        <v>8</v>
-      </c>
-      <c r="D16" s="123" t="n">
-        <v>87</v>
+          <t>2024-11-24 09:00 Sun</t>
+        </is>
+      </c>
+      <c r="B16" s="127" t="n">
+        <v>13</v>
+      </c>
+      <c r="C16" s="121" t="n">
+        <v>-2</v>
+      </c>
+      <c r="D16" s="119" t="n">
+        <v>33</v>
       </c>
       <c r="E16" s="115" t="n">
         <v>0</v>
@@ -1606,9 +1606,9 @@
       <c r="F16" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G16" s="131" t="inlineStr">
-        <is>
-          <t>8e-07</t>
+      <c r="G16" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H16" s="120" t="inlineStr">
@@ -1626,9 +1626,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K16" s="120" t="inlineStr">
-        <is>
-          <t>3.3</t>
+      <c r="K16" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L16" s="115" t="inlineStr">
@@ -1636,26 +1636,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M16" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M16" s="120" t="inlineStr">
+        <is>
+          <t>1.7</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="115" t="inlineStr">
         <is>
-          <t>2024-01-16 00:00 Tue</t>
-        </is>
-      </c>
-      <c r="B17" s="121" t="n">
-        <v>10</v>
-      </c>
-      <c r="C17" s="119" t="n">
-        <v>8</v>
-      </c>
-      <c r="D17" s="123" t="n">
-        <v>89</v>
+          <t>2024-11-24 12:00 Sun</t>
+        </is>
+      </c>
+      <c r="B17" s="119" t="n">
+        <v>14</v>
+      </c>
+      <c r="C17" s="121" t="n">
+        <v>-2</v>
+      </c>
+      <c r="D17" s="119" t="n">
+        <v>31</v>
       </c>
       <c r="E17" s="115" t="n">
         <v>0</v>
@@ -1683,9 +1683,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K17" s="120" t="inlineStr">
-        <is>
-          <t>2.8</t>
+      <c r="K17" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L17" s="115" t="inlineStr">
@@ -1693,26 +1693,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M17" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M17" s="120" t="inlineStr">
+        <is>
+          <t>0.8</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="115" t="inlineStr">
         <is>
-          <t>2024-01-16 03:00 Tue</t>
-        </is>
-      </c>
-      <c r="B18" s="121" t="n">
-        <v>10</v>
-      </c>
-      <c r="C18" s="119" t="n">
-        <v>8</v>
-      </c>
-      <c r="D18" s="123" t="n">
-        <v>88</v>
+          <t>2024-11-24 15:00 Sun</t>
+        </is>
+      </c>
+      <c r="B18" s="127" t="n">
+        <v>11</v>
+      </c>
+      <c r="C18" s="121" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="119" t="n">
+        <v>42</v>
       </c>
       <c r="E18" s="115" t="n">
         <v>0</v>
@@ -1750,26 +1750,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M18" s="120" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="M18" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="115" t="inlineStr">
         <is>
-          <t>2024-01-16 06:00 Tue</t>
+          <t>2024-11-24 18:00 Sun</t>
         </is>
       </c>
       <c r="B19" s="121" t="n">
         <v>9</v>
       </c>
-      <c r="C19" s="119" t="n">
-        <v>6</v>
-      </c>
-      <c r="D19" s="123" t="n">
-        <v>85</v>
+      <c r="C19" s="121" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="119" t="n">
+        <v>49</v>
       </c>
       <c r="E19" s="115" t="n">
         <v>0</v>
@@ -1797,9 +1797,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K19" s="120" t="inlineStr">
-        <is>
-          <t>0.2</t>
+      <c r="K19" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L19" s="115" t="inlineStr">
@@ -1807,26 +1807,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M19" s="120" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="M19" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="115" t="inlineStr">
         <is>
-          <t>2024-01-16 09:00 Tue</t>
-        </is>
-      </c>
-      <c r="B20" s="127" t="n">
-        <v>13</v>
-      </c>
-      <c r="C20" s="119" t="n">
-        <v>8</v>
-      </c>
-      <c r="D20" s="121" t="n">
-        <v>68</v>
+          <t>2024-11-24 21:00 Sun</t>
+        </is>
+      </c>
+      <c r="B20" s="121" t="n">
+        <v>9</v>
+      </c>
+      <c r="C20" s="121" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="119" t="n">
+        <v>51</v>
       </c>
       <c r="E20" s="115" t="n">
         <v>0</v>
@@ -1854,9 +1854,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K20" s="126" t="inlineStr">
-        <is>
-          <t>13.7</t>
+      <c r="K20" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L20" s="115" t="inlineStr">
@@ -1864,26 +1864,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M20" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M20" s="130" t="inlineStr">
+        <is>
+          <t>39.1</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="115" t="inlineStr">
         <is>
-          <t>2024-01-16 12:00 Tue</t>
-        </is>
-      </c>
-      <c r="B21" s="119" t="n">
-        <v>15</v>
-      </c>
-      <c r="C21" s="119" t="n">
+          <t>2024-11-25 00:00 Mon</t>
+        </is>
+      </c>
+      <c r="B21" s="121" t="n">
         <v>8</v>
       </c>
+      <c r="C21" s="121" t="n">
+        <v>0</v>
+      </c>
       <c r="D21" s="119" t="n">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E21" s="115" t="n">
         <v>0</v>
@@ -1891,9 +1891,9 @@
       <c r="F21" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G21" s="131" t="inlineStr">
-        <is>
-          <t>5.6e-06</t>
+      <c r="G21" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H21" s="120" t="inlineStr">
@@ -1911,9 +1911,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K21" s="126" t="inlineStr">
-        <is>
-          <t>19.8</t>
+      <c r="K21" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L21" s="115" t="inlineStr">
@@ -1921,26 +1921,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M21" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M21" s="130" t="inlineStr">
+        <is>
+          <t>49.2</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="115" t="inlineStr">
         <is>
-          <t>2024-01-16 15:00 Tue</t>
-        </is>
-      </c>
-      <c r="B22" s="119" t="n">
-        <v>14</v>
-      </c>
-      <c r="C22" s="119" t="n">
-        <v>9</v>
-      </c>
-      <c r="D22" s="123" t="n">
-        <v>71</v>
+          <t>2024-11-25 03:00 Mon</t>
+        </is>
+      </c>
+      <c r="B22" s="121" t="n">
+        <v>7</v>
+      </c>
+      <c r="C22" s="121" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="119" t="n">
+        <v>54</v>
       </c>
       <c r="E22" s="115" t="n">
         <v>0</v>
@@ -1968,9 +1968,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K22" s="126" t="inlineStr">
-        <is>
-          <t>10.4</t>
+      <c r="K22" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L22" s="115" t="inlineStr">
@@ -1978,26 +1978,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M22" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M22" s="130" t="inlineStr">
+        <is>
+          <t>36.6</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="115" t="inlineStr">
         <is>
-          <t>2024-01-16 18:00 Tue</t>
-        </is>
-      </c>
-      <c r="B23" s="127" t="n">
-        <v>11</v>
-      </c>
-      <c r="C23" s="119" t="n">
-        <v>9</v>
-      </c>
-      <c r="D23" s="123" t="n">
-        <v>86</v>
+          <t>2024-11-25 06:00 Mon</t>
+        </is>
+      </c>
+      <c r="B23" s="121" t="n">
+        <v>7</v>
+      </c>
+      <c r="C23" s="121" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="119" t="n">
+        <v>56</v>
       </c>
       <c r="E23" s="115" t="n">
         <v>0</v>
@@ -2025,9 +2025,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K23" s="130" t="inlineStr">
-        <is>
-          <t>39.1</t>
+      <c r="K23" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L23" s="115" t="inlineStr">
@@ -2035,26 +2035,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M23" s="120" t="inlineStr">
-        <is>
-          <t>1.7</t>
+      <c r="M23" s="126" t="inlineStr">
+        <is>
+          <t>20.8</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="115" t="inlineStr">
         <is>
-          <t>2024-01-16 21:00 Tue</t>
+          <t>2024-11-25 09:00 Mon</t>
         </is>
       </c>
       <c r="B24" s="127" t="n">
-        <v>12</v>
-      </c>
-      <c r="C24" s="119" t="n">
-        <v>10</v>
-      </c>
-      <c r="D24" s="123" t="n">
-        <v>85</v>
+        <v>13</v>
+      </c>
+      <c r="C24" s="121" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="119" t="n">
+        <v>43</v>
       </c>
       <c r="E24" s="115" t="n">
         <v>0</v>
@@ -2062,9 +2062,9 @@
       <c r="F24" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G24" s="131" t="inlineStr">
-        <is>
-          <t>8.8e-06</t>
+      <c r="G24" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H24" s="120" t="inlineStr">
@@ -2082,9 +2082,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K24" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="K24" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L24" s="115" t="inlineStr">
@@ -2092,26 +2092,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M24" s="120" t="inlineStr">
-        <is>
-          <t>1.6</t>
+      <c r="M24" s="125" t="inlineStr">
+        <is>
+          <t>5.5</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="115" t="inlineStr">
         <is>
-          <t>2024-01-17 00:00 Wed</t>
-        </is>
-      </c>
-      <c r="B25" s="127" t="n">
-        <v>12</v>
-      </c>
-      <c r="C25" s="119" t="n">
-        <v>9</v>
-      </c>
-      <c r="D25" s="123" t="n">
-        <v>84</v>
+          <t>2024-11-25 12:00 Mon</t>
+        </is>
+      </c>
+      <c r="B25" s="119" t="n">
+        <v>15</v>
+      </c>
+      <c r="C25" s="121" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="119" t="n">
+        <v>37</v>
       </c>
       <c r="E25" s="115" t="n">
         <v>0</v>
@@ -2139,9 +2139,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K25" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="K25" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L25" s="115" t="inlineStr">
@@ -2149,26 +2149,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M25" s="120" t="inlineStr">
-        <is>
-          <t>0.7</t>
+      <c r="M25" s="125" t="inlineStr">
+        <is>
+          <t>5.2</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="115" t="inlineStr">
         <is>
-          <t>2024-01-17 03:00 Wed</t>
+          <t>2024-11-25 15:00 Mon</t>
         </is>
       </c>
       <c r="B26" s="127" t="n">
         <v>12</v>
       </c>
-      <c r="C26" s="119" t="n">
-        <v>8</v>
-      </c>
-      <c r="D26" s="123" t="n">
-        <v>75</v>
+      <c r="C26" s="121" t="n">
+        <v>3</v>
+      </c>
+      <c r="D26" s="119" t="n">
+        <v>54</v>
       </c>
       <c r="E26" s="115" t="n">
         <v>0</v>
@@ -2196,9 +2196,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K26" s="128" t="inlineStr">
-        <is>
-          <t>98.6</t>
+      <c r="K26" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L26" s="115" t="inlineStr">
@@ -2206,26 +2206,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M26" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M26" s="120" t="inlineStr">
+        <is>
+          <t>1.7</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="115" t="inlineStr">
         <is>
-          <t>2024-01-17 06:00 Wed</t>
+          <t>2024-11-25 18:00 Mon</t>
         </is>
       </c>
       <c r="B27" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="C27" s="119" t="n">
-        <v>8</v>
-      </c>
-      <c r="D27" s="123" t="n">
-        <v>84</v>
+      <c r="C27" s="121" t="n">
+        <v>4</v>
+      </c>
+      <c r="D27" s="121" t="n">
+        <v>64</v>
       </c>
       <c r="E27" s="115" t="n">
         <v>0</v>
@@ -2253,9 +2253,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K27" s="129" t="inlineStr">
-        <is>
-          <t>74.7</t>
+      <c r="K27" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L27" s="115" t="inlineStr">
@@ -2263,26 +2263,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M27" s="126" t="inlineStr">
-        <is>
-          <t>16.5</t>
+      <c r="M27" s="120" t="inlineStr">
+        <is>
+          <t>0.8</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="115" t="inlineStr">
         <is>
-          <t>2024-01-17 09:00 Wed</t>
-        </is>
-      </c>
-      <c r="B28" s="119" t="n">
-        <v>14</v>
-      </c>
-      <c r="C28" s="119" t="n">
-        <v>8</v>
+          <t>2024-11-25 21:00 Mon</t>
+        </is>
+      </c>
+      <c r="B28" s="121" t="n">
+        <v>9</v>
+      </c>
+      <c r="C28" s="121" t="n">
+        <v>4</v>
       </c>
       <c r="D28" s="121" t="n">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E28" s="115" t="n">
         <v>0</v>
@@ -2310,9 +2310,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K28" s="127" t="inlineStr">
-        <is>
-          <t>27.6</t>
+      <c r="K28" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L28" s="115" t="inlineStr">
@@ -2322,24 +2322,24 @@
       </c>
       <c r="M28" s="120" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>0.8</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="115" t="inlineStr">
         <is>
-          <t>2024-01-17 12:00 Wed</t>
-        </is>
-      </c>
-      <c r="B29" s="119" t="n">
-        <v>16</v>
-      </c>
-      <c r="C29" s="119" t="n">
-        <v>7</v>
-      </c>
-      <c r="D29" s="119" t="n">
-        <v>55</v>
+          <t>2024-11-26 00:00 Tue</t>
+        </is>
+      </c>
+      <c r="B29" s="121" t="n">
+        <v>8</v>
+      </c>
+      <c r="C29" s="121" t="n">
+        <v>4</v>
+      </c>
+      <c r="D29" s="123" t="n">
+        <v>73</v>
       </c>
       <c r="E29" s="115" t="n">
         <v>0</v>
@@ -2367,9 +2367,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K29" s="126" t="inlineStr">
-        <is>
-          <t>14.1</t>
+      <c r="K29" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L29" s="115" t="inlineStr">
@@ -2377,26 +2377,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M29" s="125" t="inlineStr">
-        <is>
-          <t>6</t>
+      <c r="M29" s="120" t="inlineStr">
+        <is>
+          <t>0.4</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="115" t="inlineStr">
         <is>
-          <t>2024-01-17 15:00 Wed</t>
-        </is>
-      </c>
-      <c r="B30" s="119" t="n">
-        <v>14</v>
-      </c>
-      <c r="C30" s="119" t="n">
+          <t>2024-11-26 03:00 Tue</t>
+        </is>
+      </c>
+      <c r="B30" s="121" t="n">
         <v>8</v>
       </c>
-      <c r="D30" s="121" t="n">
-        <v>69</v>
+      <c r="C30" s="121" t="n">
+        <v>4</v>
+      </c>
+      <c r="D30" s="123" t="n">
+        <v>75</v>
       </c>
       <c r="E30" s="115" t="n">
         <v>0</v>
@@ -2424,9 +2424,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K30" s="120" t="inlineStr">
-        <is>
-          <t>0.1</t>
+      <c r="K30" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L30" s="115" t="inlineStr">
@@ -2434,26 +2434,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M30" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="M30" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="115" t="inlineStr">
         <is>
-          <t>2024-01-17 18:00 Wed</t>
+          <t>2024-11-26 06:00 Tue</t>
         </is>
       </c>
       <c r="B31" s="121" t="n">
-        <v>10</v>
-      </c>
-      <c r="C31" s="119" t="n">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C31" s="121" t="n">
+        <v>4</v>
       </c>
       <c r="D31" s="123" t="n">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E31" s="115" t="n">
         <v>0</v>
@@ -2481,9 +2481,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K31" s="120" t="inlineStr">
-        <is>
-          <t>0.1</t>
+      <c r="K31" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L31" s="115" t="inlineStr">
@@ -2491,26 +2491,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M31" s="128" t="inlineStr">
-        <is>
-          <t>86.6</t>
+      <c r="M31" s="120" t="inlineStr">
+        <is>
+          <t>0.8</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="115" t="inlineStr">
         <is>
-          <t>2024-01-17 21:00 Wed</t>
-        </is>
-      </c>
-      <c r="B32" s="127" t="n">
-        <v>11</v>
-      </c>
-      <c r="C32" s="119" t="n">
-        <v>9</v>
-      </c>
-      <c r="D32" s="123" t="n">
-        <v>88</v>
+          <t>2024-11-26 09:00 Tue</t>
+        </is>
+      </c>
+      <c r="B32" s="119" t="n">
+        <v>14</v>
+      </c>
+      <c r="C32" s="121" t="n">
+        <v>2</v>
+      </c>
+      <c r="D32" s="119" t="n">
+        <v>45</v>
       </c>
       <c r="E32" s="115" t="n">
         <v>0</v>
@@ -2548,26 +2548,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M32" s="128" t="inlineStr">
-        <is>
-          <t>87.9</t>
+      <c r="M32" s="120" t="inlineStr">
+        <is>
+          <t>1.7</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="115" t="inlineStr">
         <is>
-          <t>2024-01-18 00:00 Thu</t>
-        </is>
-      </c>
-      <c r="B33" s="127" t="n">
-        <v>12</v>
-      </c>
-      <c r="C33" s="117" t="n">
-        <v>11</v>
-      </c>
-      <c r="D33" s="123" t="n">
-        <v>90</v>
+          <t>2024-11-26 12:00 Tue</t>
+        </is>
+      </c>
+      <c r="B33" s="119" t="n">
+        <v>16</v>
+      </c>
+      <c r="C33" s="121" t="n">
+        <v>3</v>
+      </c>
+      <c r="D33" s="119" t="n">
+        <v>42</v>
       </c>
       <c r="E33" s="115" t="n">
         <v>0</v>
@@ -2595,36 +2595,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K33" s="120" t="inlineStr">
-        <is>
-          <t>0.2</t>
-        </is>
-      </c>
-      <c r="L33" s="126" t="inlineStr">
-        <is>
-          <t>18.8</t>
-        </is>
-      </c>
-      <c r="M33" s="128" t="inlineStr">
-        <is>
-          <t>94</t>
+      <c r="K33" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L33" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M33" s="120" t="inlineStr">
+        <is>
+          <t>0.8</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="115" t="inlineStr">
         <is>
-          <t>2024-01-18 03:00 Thu</t>
-        </is>
-      </c>
-      <c r="B34" s="127" t="n">
-        <v>13</v>
-      </c>
-      <c r="C34" s="117" t="n">
-        <v>11</v>
-      </c>
-      <c r="D34" s="123" t="n">
-        <v>89</v>
+          <t>2024-11-26 15:00 Tue</t>
+        </is>
+      </c>
+      <c r="B34" s="119" t="n">
+        <v>14</v>
+      </c>
+      <c r="C34" s="119" t="n">
+        <v>6</v>
+      </c>
+      <c r="D34" s="119" t="n">
+        <v>57</v>
       </c>
       <c r="E34" s="115" t="n">
         <v>0</v>
@@ -2632,14 +2632,14 @@
       <c r="F34" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G34" s="131" t="inlineStr">
-        <is>
-          <t>3.2e-05</t>
-        </is>
-      </c>
-      <c r="H34" s="119" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="G34" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H34" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="I34" s="120" t="inlineStr">
@@ -2652,36 +2652,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K34" s="126" t="inlineStr">
-        <is>
-          <t>17.4</t>
-        </is>
-      </c>
-      <c r="L34" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="M34" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="K34" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L34" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M34" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="115" t="inlineStr">
         <is>
-          <t>2024-01-18 06:00 Thu</t>
+          <t>2024-11-26 18:00 Tue</t>
         </is>
       </c>
       <c r="B35" s="127" t="n">
-        <v>13</v>
-      </c>
-      <c r="C35" s="117" t="n">
         <v>12</v>
       </c>
-      <c r="D35" s="123" t="n">
-        <v>91</v>
+      <c r="C35" s="119" t="n">
+        <v>6</v>
+      </c>
+      <c r="D35" s="121" t="n">
+        <v>67</v>
       </c>
       <c r="E35" s="115" t="n">
         <v>0</v>
@@ -2689,9 +2689,9 @@
       <c r="F35" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G35" s="131" t="inlineStr">
-        <is>
-          <t>3.2e-06</t>
+      <c r="G35" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H35" s="120" t="inlineStr">
@@ -2709,36 +2709,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K35" s="130" t="inlineStr">
-        <is>
-          <t>58.6</t>
-        </is>
-      </c>
-      <c r="L35" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="M35" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="K35" s="120" t="inlineStr">
+        <is>
+          <t>1.7</t>
+        </is>
+      </c>
+      <c r="L35" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M35" s="120" t="inlineStr">
+        <is>
+          <t>1.4</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="115" t="inlineStr">
         <is>
-          <t>2024-01-18 09:00 Thu</t>
-        </is>
-      </c>
-      <c r="B36" s="119" t="n">
-        <v>15</v>
-      </c>
-      <c r="C36" s="117" t="n">
-        <v>12</v>
+          <t>2024-11-26 21:00 Tue</t>
+        </is>
+      </c>
+      <c r="B36" s="127" t="n">
+        <v>11</v>
+      </c>
+      <c r="C36" s="119" t="n">
+        <v>6</v>
       </c>
       <c r="D36" s="123" t="n">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="E36" s="115" t="n">
         <v>0</v>
@@ -2766,36 +2766,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K36" s="129" t="inlineStr">
-        <is>
-          <t>79.8</t>
-        </is>
-      </c>
-      <c r="L36" s="129" t="inlineStr">
-        <is>
-          <t>69.8</t>
-        </is>
-      </c>
-      <c r="M36" s="129" t="inlineStr">
-        <is>
-          <t>68.6</t>
+      <c r="K36" s="120" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L36" s="120" t="inlineStr">
+        <is>
+          <t>0.3</t>
+        </is>
+      </c>
+      <c r="M36" s="127" t="inlineStr">
+        <is>
+          <t>24.8</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="115" t="inlineStr">
         <is>
-          <t>2024-01-18 12:00 Thu</t>
-        </is>
-      </c>
-      <c r="B37" s="119" t="n">
-        <v>17</v>
-      </c>
-      <c r="C37" s="117" t="n">
-        <v>12</v>
+          <t>2024-11-27 00:00 Wed</t>
+        </is>
+      </c>
+      <c r="B37" s="121" t="n">
+        <v>10</v>
+      </c>
+      <c r="C37" s="119" t="n">
+        <v>7</v>
       </c>
       <c r="D37" s="123" t="n">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E37" s="115" t="n">
         <v>0</v>
@@ -2823,36 +2823,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K37" s="130" t="inlineStr">
-        <is>
-          <t>42.7</t>
-        </is>
-      </c>
-      <c r="L37" s="130" t="inlineStr">
-        <is>
-          <t>37.4</t>
-        </is>
-      </c>
-      <c r="M37" s="130" t="inlineStr">
-        <is>
-          <t>44.3</t>
+      <c r="K37" s="120" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L37" s="120" t="inlineStr">
+        <is>
+          <t>3.4</t>
+        </is>
+      </c>
+      <c r="M37" s="126" t="inlineStr">
+        <is>
+          <t>16.8</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="115" t="inlineStr">
         <is>
-          <t>2024-01-18 15:00 Thu</t>
-        </is>
-      </c>
-      <c r="B38" s="119" t="n">
-        <v>15</v>
-      </c>
-      <c r="C38" s="118" t="n">
-        <v>13</v>
+          <t>2024-11-27 03:00 Wed</t>
+        </is>
+      </c>
+      <c r="B38" s="121" t="n">
+        <v>10</v>
+      </c>
+      <c r="C38" s="119" t="n">
+        <v>7</v>
       </c>
       <c r="D38" s="123" t="n">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E38" s="115" t="n">
         <v>0</v>
@@ -2882,34 +2882,34 @@
       </c>
       <c r="K38" s="120" t="inlineStr">
         <is>
-          <t>3.3</t>
-        </is>
-      </c>
-      <c r="L38" s="129" t="inlineStr">
-        <is>
-          <t>78.6</t>
-        </is>
-      </c>
-      <c r="M38" s="130" t="inlineStr">
-        <is>
-          <t>42.9</t>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L38" s="120" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M38" s="125" t="inlineStr">
+        <is>
+          <t>8.9</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="115" t="inlineStr">
         <is>
-          <t>2024-01-18 18:00 Thu</t>
-        </is>
-      </c>
-      <c r="B39" s="119" t="n">
-        <v>14</v>
-      </c>
-      <c r="C39" s="118" t="n">
-        <v>13</v>
+          <t>2024-11-27 06:00 Wed</t>
+        </is>
+      </c>
+      <c r="B39" s="121" t="n">
+        <v>10</v>
+      </c>
+      <c r="C39" s="119" t="n">
+        <v>7</v>
       </c>
       <c r="D39" s="123" t="n">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E39" s="115" t="n">
         <v>0</v>
@@ -2937,36 +2937,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K39" s="126" t="inlineStr">
-        <is>
-          <t>14.4</t>
-        </is>
-      </c>
-      <c r="L39" s="129" t="inlineStr">
-        <is>
-          <t>70.3</t>
-        </is>
-      </c>
-      <c r="M39" s="129" t="inlineStr">
-        <is>
-          <t>71.4</t>
+      <c r="K39" s="120" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L39" s="120" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M39" s="126" t="inlineStr">
+        <is>
+          <t>14.5</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="115" t="inlineStr">
         <is>
-          <t>2024-01-18 21:00 Thu</t>
+          <t>2024-11-27 09:00 Wed</t>
         </is>
       </c>
       <c r="B40" s="119" t="n">
-        <v>14</v>
-      </c>
-      <c r="C40" s="117" t="n">
-        <v>12</v>
-      </c>
-      <c r="D40" s="123" t="n">
-        <v>88</v>
+        <v>15</v>
+      </c>
+      <c r="C40" s="119" t="n">
+        <v>8</v>
+      </c>
+      <c r="D40" s="121" t="n">
+        <v>61</v>
       </c>
       <c r="E40" s="115" t="n">
         <v>0</v>
@@ -2996,34 +2996,34 @@
       </c>
       <c r="K40" s="120" t="inlineStr">
         <is>
-          <t>0.3</t>
-        </is>
-      </c>
-      <c r="L40" s="120" t="inlineStr">
-        <is>
-          <t>4.2</t>
-        </is>
-      </c>
-      <c r="M40" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L40" s="125" t="inlineStr">
+        <is>
+          <t>6.5</t>
+        </is>
+      </c>
+      <c r="M40" s="130" t="inlineStr">
+        <is>
+          <t>48.6</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="115" t="inlineStr">
         <is>
-          <t>2024-01-19 00:00 Fri</t>
+          <t>2024-11-27 12:00 Wed</t>
         </is>
       </c>
       <c r="B41" s="119" t="n">
-        <v>14</v>
-      </c>
-      <c r="C41" s="117" t="n">
-        <v>11</v>
-      </c>
-      <c r="D41" s="123" t="n">
-        <v>82</v>
+        <v>18</v>
+      </c>
+      <c r="C41" s="119" t="n">
+        <v>9</v>
+      </c>
+      <c r="D41" s="119" t="n">
+        <v>54</v>
       </c>
       <c r="E41" s="115" t="n">
         <v>0</v>
@@ -3053,34 +3053,34 @@
       </c>
       <c r="K41" s="120" t="inlineStr">
         <is>
-          <t>0.1</t>
-        </is>
-      </c>
-      <c r="L41" s="130" t="inlineStr">
-        <is>
-          <t>36.6</t>
-        </is>
-      </c>
-      <c r="M41" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L41" s="125" t="inlineStr">
+        <is>
+          <t>8.3</t>
+        </is>
+      </c>
+      <c r="M41" s="130" t="inlineStr">
+        <is>
+          <t>36.3</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="115" t="inlineStr">
         <is>
-          <t>2024-01-19 03:00 Fri</t>
+          <t>2024-11-27 15:00 Wed</t>
         </is>
       </c>
       <c r="B42" s="119" t="n">
-        <v>14</v>
-      </c>
-      <c r="C42" s="117" t="n">
-        <v>11</v>
-      </c>
-      <c r="D42" s="123" t="n">
-        <v>79</v>
+        <v>16</v>
+      </c>
+      <c r="C42" s="119" t="n">
+        <v>10</v>
+      </c>
+      <c r="D42" s="121" t="n">
+        <v>67</v>
       </c>
       <c r="E42" s="115" t="n">
         <v>0</v>
@@ -3108,36 +3108,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K42" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L42" s="130" t="inlineStr">
-        <is>
-          <t>59.6</t>
-        </is>
-      </c>
-      <c r="M42" s="128" t="inlineStr">
-        <is>
-          <t>97.6</t>
+      <c r="K42" s="120" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L42" s="125" t="inlineStr">
+        <is>
+          <t>6.2</t>
+        </is>
+      </c>
+      <c r="M42" s="126" t="inlineStr">
+        <is>
+          <t>17.6</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="115" t="inlineStr">
         <is>
-          <t>2024-01-19 06:00 Fri</t>
+          <t>2024-11-27 18:00 Wed</t>
         </is>
       </c>
       <c r="B43" s="127" t="n">
         <v>13</v>
       </c>
-      <c r="C43" s="117" t="n">
-        <v>11</v>
+      <c r="C43" s="119" t="n">
+        <v>10</v>
       </c>
       <c r="D43" s="123" t="n">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E43" s="115" t="n">
         <v>0</v>
@@ -3165,36 +3165,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K43" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L43" s="130" t="inlineStr">
-        <is>
-          <t>32.4</t>
-        </is>
-      </c>
-      <c r="M43" s="115" t="inlineStr">
-        <is>
-          <t>82.9</t>
+      <c r="K43" s="120" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="L43" s="125" t="inlineStr">
+        <is>
+          <t>5.6</t>
+        </is>
+      </c>
+      <c r="M43" s="126" t="inlineStr">
+        <is>
+          <t>13.6</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="115" t="inlineStr">
         <is>
-          <t>2024-01-19 09:00 Fri</t>
-        </is>
-      </c>
-      <c r="B44" s="119" t="n">
-        <v>16</v>
-      </c>
-      <c r="C44" s="117" t="n">
-        <v>12</v>
+          <t>2024-11-27 21:00 Wed</t>
+        </is>
+      </c>
+      <c r="B44" s="127" t="n">
+        <v>13</v>
+      </c>
+      <c r="C44" s="119" t="n">
+        <v>10</v>
       </c>
       <c r="D44" s="123" t="n">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="E44" s="115" t="n">
         <v>0</v>
@@ -3222,36 +3222,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K44" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L44" s="130" t="inlineStr">
-        <is>
-          <t>34.3</t>
-        </is>
-      </c>
-      <c r="M44" s="128" t="inlineStr">
-        <is>
-          <t>91.7</t>
+      <c r="K44" s="125" t="inlineStr">
+        <is>
+          <t>7.4</t>
+        </is>
+      </c>
+      <c r="L44" s="120" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M44" s="125" t="inlineStr">
+        <is>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="115" t="inlineStr">
         <is>
-          <t>2024-01-19 12:00 Fri</t>
-        </is>
-      </c>
-      <c r="B45" s="119" t="n">
-        <v>16</v>
+          <t>2024-11-28 00:00 Thu</t>
+        </is>
+      </c>
+      <c r="B45" s="127" t="n">
+        <v>13</v>
       </c>
       <c r="C45" s="117" t="n">
         <v>12</v>
       </c>
       <c r="D45" s="123" t="n">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="E45" s="115" t="n">
         <v>0</v>
@@ -3259,9 +3259,9 @@
       <c r="F45" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G45" s="131" t="inlineStr">
-        <is>
-          <t>8e-07</t>
+      <c r="G45" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H45" s="120" t="inlineStr">
@@ -3279,19 +3279,19 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K45" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L45" s="129" t="inlineStr">
-        <is>
-          <t>67.1</t>
-        </is>
-      </c>
-      <c r="M45" s="128" t="inlineStr">
-        <is>
-          <t>95.9</t>
+      <c r="K45" s="127" t="inlineStr">
+        <is>
+          <t>26.7</t>
+        </is>
+      </c>
+      <c r="L45" s="120" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M45" s="126" t="inlineStr">
+        <is>
+          <t>13.6</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
"Modified comment about description"
</commit_message>
<xml_diff>
--- a/data/simpleWeather.xlsx
+++ b/data/simpleWeather.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Foglio1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
@@ -790,17 +790,17 @@
     <row r="2">
       <c r="A2" s="115" t="inlineStr">
         <is>
-          <t>2024-11-22 15:00 Fri</t>
+          <t>2025-01-26 09:00 dom</t>
         </is>
       </c>
       <c r="B2" s="119" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C2" s="117" t="n">
-        <v>12</v>
-      </c>
-      <c r="D2" s="119" t="n">
-        <v>60</v>
+        <v>11</v>
+      </c>
+      <c r="D2" s="123" t="n">
+        <v>77</v>
       </c>
       <c r="E2" s="115" t="n">
         <v>0</v>
@@ -808,9 +808,9 @@
       <c r="F2" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G2" s="131" t="inlineStr">
-        <is>
-          <t>5.08e-05</t>
+      <c r="G2" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H2" s="120" t="inlineStr">
@@ -828,14 +828,14 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K2" s="130" t="inlineStr">
-        <is>
-          <t>38.8</t>
-        </is>
-      </c>
-      <c r="L2" s="130" t="inlineStr">
-        <is>
-          <t>30.8</t>
+      <c r="K2" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L2" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
       <c r="M2" s="128" t="inlineStr">
@@ -847,17 +847,17 @@
     <row r="3">
       <c r="A3" s="115" t="inlineStr">
         <is>
-          <t>2024-11-22 18:00 Fri</t>
+          <t>2025-01-26 12:00 dom</t>
         </is>
       </c>
       <c r="B3" s="119" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" s="119" t="n">
         <v>10</v>
       </c>
-      <c r="D3" s="119" t="n">
-        <v>60</v>
+      <c r="D3" s="121" t="n">
+        <v>68</v>
       </c>
       <c r="E3" s="115" t="n">
         <v>0</v>
@@ -865,9 +865,9 @@
       <c r="F3" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G3" s="131" t="inlineStr">
-        <is>
-          <t>5.6e-06</t>
+      <c r="G3" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H3" s="120" t="inlineStr">
@@ -885,36 +885,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K3" s="129" t="inlineStr">
-        <is>
-          <t>69.4</t>
-        </is>
-      </c>
-      <c r="L3" s="129" t="inlineStr">
-        <is>
-          <t>65.4</t>
+      <c r="K3" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L3" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
       <c r="M3" s="128" t="inlineStr">
         <is>
-          <t>99.4</t>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="115" t="inlineStr">
         <is>
-          <t>2024-11-22 21:00 Fri</t>
-        </is>
-      </c>
-      <c r="B4" s="127" t="n">
-        <v>12</v>
-      </c>
-      <c r="C4" s="119" t="n">
-        <v>7</v>
+          <t>2025-01-26 15:00 dom</t>
+        </is>
+      </c>
+      <c r="B4" s="119" t="n">
+        <v>14</v>
+      </c>
+      <c r="C4" s="117" t="n">
+        <v>11</v>
       </c>
       <c r="D4" s="123" t="n">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="E4" s="115" t="n">
         <v>0</v>
@@ -942,36 +942,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K4" s="130" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
-      </c>
-      <c r="L4" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M4" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K4" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L4" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="M4" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="115" t="inlineStr">
         <is>
-          <t>2024-11-23 00:00 Sat</t>
+          <t>2025-01-26 18:00 dom</t>
         </is>
       </c>
       <c r="B5" s="127" t="n">
+        <v>13</v>
+      </c>
+      <c r="C5" s="117" t="n">
         <v>11</v>
       </c>
-      <c r="C5" s="121" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="119" t="n">
-        <v>51</v>
+      <c r="D5" s="123" t="n">
+        <v>90</v>
       </c>
       <c r="E5" s="115" t="n">
         <v>0</v>
@@ -999,36 +999,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K5" s="126" t="inlineStr">
-        <is>
-          <t>16.6</t>
-        </is>
-      </c>
-      <c r="L5" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M5" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K5" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L5" s="128" t="inlineStr">
+        <is>
+          <t>90.3</t>
+        </is>
+      </c>
+      <c r="M5" s="128" t="inlineStr">
+        <is>
+          <t>86</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="115" t="inlineStr">
         <is>
-          <t>2024-11-23 03:00 Sat</t>
+          <t>2025-01-26 21:00 dom</t>
         </is>
       </c>
       <c r="B6" s="127" t="n">
+        <v>12</v>
+      </c>
+      <c r="C6" s="117" t="n">
         <v>11</v>
       </c>
-      <c r="C6" s="121" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D6" s="119" t="n">
-        <v>42</v>
+      <c r="D6" s="123" t="n">
+        <v>91</v>
       </c>
       <c r="E6" s="115" t="n">
         <v>0</v>
@@ -1056,36 +1056,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K6" s="130" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="L6" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M6" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K6" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L6" s="130" t="inlineStr">
+        <is>
+          <t>35.3</t>
+        </is>
+      </c>
+      <c r="M6" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="115" t="inlineStr">
         <is>
-          <t>2024-11-23 06:00 Sat</t>
-        </is>
-      </c>
-      <c r="B7" s="121" t="n">
-        <v>10</v>
-      </c>
-      <c r="C7" s="121" t="n">
-        <v>-3</v>
-      </c>
-      <c r="D7" s="119" t="n">
-        <v>37</v>
+          <t>2025-01-27 00:00 lun</t>
+        </is>
+      </c>
+      <c r="B7" s="127" t="n">
+        <v>11</v>
+      </c>
+      <c r="C7" s="117" t="n">
+        <v>11</v>
+      </c>
+      <c r="D7" s="123" t="n">
+        <v>94</v>
       </c>
       <c r="E7" s="115" t="n">
         <v>0</v>
@@ -1113,36 +1113,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K7" s="130" t="inlineStr">
-        <is>
-          <t>58.6</t>
-        </is>
-      </c>
-      <c r="L7" s="130" t="inlineStr">
-        <is>
-          <t>33.3</t>
-        </is>
-      </c>
-      <c r="M7" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K7" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L7" s="126" t="inlineStr">
+        <is>
+          <t>17.6</t>
+        </is>
+      </c>
+      <c r="M7" s="128" t="inlineStr">
+        <is>
+          <t>97.4</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="115" t="inlineStr">
         <is>
-          <t>2024-11-23 09:00 Sat</t>
+          <t>2025-01-27 03:00 lun</t>
         </is>
       </c>
       <c r="B8" s="127" t="n">
-        <v>12</v>
-      </c>
-      <c r="C8" s="121" t="n">
-        <v>-6</v>
-      </c>
-      <c r="D8" s="117" t="n">
-        <v>26</v>
+        <v>11</v>
+      </c>
+      <c r="C8" s="119" t="n">
+        <v>10</v>
+      </c>
+      <c r="D8" s="123" t="n">
+        <v>95</v>
       </c>
       <c r="E8" s="115" t="n">
         <v>0</v>
@@ -1170,9 +1170,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K8" s="120" t="inlineStr">
-        <is>
-          <t>0.4</t>
+      <c r="K8" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L8" s="115" t="inlineStr">
@@ -1180,26 +1180,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M8" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M8" s="120" t="inlineStr">
+        <is>
+          <t>0.5</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="115" t="inlineStr">
         <is>
-          <t>2024-11-23 12:00 Sat</t>
+          <t>2025-01-27 06:00 lun</t>
         </is>
       </c>
       <c r="B9" s="127" t="n">
-        <v>12</v>
-      </c>
-      <c r="C9" s="121" t="n">
-        <v>-6</v>
-      </c>
-      <c r="D9" s="117" t="n">
-        <v>26</v>
+        <v>11</v>
+      </c>
+      <c r="C9" s="119" t="n">
+        <v>10</v>
+      </c>
+      <c r="D9" s="123" t="n">
+        <v>96</v>
       </c>
       <c r="E9" s="115" t="n">
         <v>0</v>
@@ -1227,9 +1227,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K9" s="120" t="inlineStr">
-        <is>
-          <t>1.7</t>
+      <c r="K9" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L9" s="115" t="inlineStr">
@@ -1237,26 +1237,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M9" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M9" s="125" t="inlineStr">
+        <is>
+          <t>7.3</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="115" t="inlineStr">
         <is>
-          <t>2024-11-23 15:00 Sat</t>
-        </is>
-      </c>
-      <c r="B10" s="127" t="n">
+          <t>2025-01-27 09:00 lun</t>
+        </is>
+      </c>
+      <c r="B10" s="119" t="n">
+        <v>15</v>
+      </c>
+      <c r="C10" s="117" t="n">
         <v>11</v>
       </c>
-      <c r="C10" s="121" t="n">
-        <v>-3</v>
-      </c>
-      <c r="D10" s="119" t="n">
-        <v>34</v>
+      <c r="D10" s="123" t="n">
+        <v>76</v>
       </c>
       <c r="E10" s="115" t="n">
         <v>0</v>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="K10" s="120" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1.2</t>
         </is>
       </c>
       <c r="L10" s="115" t="inlineStr">
@@ -1294,26 +1294,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M10" s="120" t="inlineStr">
-        <is>
-          <t>0.4</t>
+      <c r="M10" s="125" t="inlineStr">
+        <is>
+          <t>6.5</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="115" t="inlineStr">
         <is>
-          <t>2024-11-23 18:00 Sat</t>
-        </is>
-      </c>
-      <c r="B11" s="121" t="n">
-        <v>10</v>
-      </c>
-      <c r="C11" s="121" t="n">
-        <v>-2</v>
+          <t>2025-01-27 12:00 lun</t>
+        </is>
+      </c>
+      <c r="B11" s="119" t="n">
+        <v>17</v>
+      </c>
+      <c r="C11" s="119" t="n">
+        <v>9</v>
       </c>
       <c r="D11" s="119" t="n">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="E11" s="115" t="n">
         <v>0</v>
@@ -1343,7 +1343,7 @@
       </c>
       <c r="K11" s="120" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>0.6</t>
         </is>
       </c>
       <c r="L11" s="115" t="inlineStr">
@@ -1351,26 +1351,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M11" s="120" t="inlineStr">
-        <is>
-          <t>2.7</t>
+      <c r="M11" s="130" t="inlineStr">
+        <is>
+          <t>37.4</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="115" t="inlineStr">
         <is>
-          <t>2024-11-23 21:00 Sat</t>
-        </is>
-      </c>
-      <c r="B12" s="121" t="n">
+          <t>2025-01-27 15:00 lun</t>
+        </is>
+      </c>
+      <c r="B12" s="119" t="n">
+        <v>15</v>
+      </c>
+      <c r="C12" s="119" t="n">
         <v>9</v>
       </c>
-      <c r="C12" s="121" t="n">
-        <v>-3</v>
-      </c>
-      <c r="D12" s="119" t="n">
-        <v>39</v>
+      <c r="D12" s="121" t="n">
+        <v>65</v>
       </c>
       <c r="E12" s="115" t="n">
         <v>0</v>
@@ -1398,9 +1398,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K12" s="120" t="inlineStr">
-        <is>
-          <t>1.6</t>
+      <c r="K12" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L12" s="115" t="inlineStr">
@@ -1408,26 +1408,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M12" s="120" t="inlineStr">
-        <is>
-          <t>1.6</t>
+      <c r="M12" s="130" t="inlineStr">
+        <is>
+          <t>38</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="115" t="inlineStr">
         <is>
-          <t>2024-11-24 00:00 Sun</t>
-        </is>
-      </c>
-      <c r="B13" s="121" t="n">
-        <v>8</v>
-      </c>
-      <c r="C13" s="121" t="n">
-        <v>-4</v>
-      </c>
-      <c r="D13" s="119" t="n">
-        <v>38</v>
+          <t>2025-01-27 18:00 lun</t>
+        </is>
+      </c>
+      <c r="B13" s="127" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" s="117" t="n">
+        <v>11</v>
+      </c>
+      <c r="D13" s="123" t="n">
+        <v>95</v>
       </c>
       <c r="E13" s="115" t="n">
         <v>0</v>
@@ -1455,9 +1455,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K13" s="120" t="inlineStr">
-        <is>
-          <t>0.8</t>
+      <c r="K13" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L13" s="115" t="inlineStr">
@@ -1465,26 +1465,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M13" s="120" t="inlineStr">
-        <is>
-          <t>0.8</t>
+      <c r="M13" s="126" t="inlineStr">
+        <is>
+          <t>21.5</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="115" t="inlineStr">
         <is>
-          <t>2024-11-24 03:00 Sun</t>
-        </is>
-      </c>
-      <c r="B14" s="121" t="n">
-        <v>8</v>
-      </c>
-      <c r="C14" s="121" t="n">
-        <v>-4</v>
-      </c>
-      <c r="D14" s="119" t="n">
-        <v>39</v>
+          <t>2025-01-27 21:00 lun</t>
+        </is>
+      </c>
+      <c r="B14" s="127" t="n">
+        <v>11</v>
+      </c>
+      <c r="C14" s="119" t="n">
+        <v>9</v>
+      </c>
+      <c r="D14" s="123" t="n">
+        <v>88</v>
       </c>
       <c r="E14" s="115" t="n">
         <v>0</v>
@@ -1512,9 +1512,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K14" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K14" s="120" t="inlineStr">
+        <is>
+          <t>0.3</t>
         </is>
       </c>
       <c r="L14" s="115" t="inlineStr">
@@ -1522,26 +1522,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M14" s="120" t="inlineStr">
-        <is>
-          <t>1.6</t>
+      <c r="M14" s="128" t="inlineStr">
+        <is>
+          <t>90.3</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="115" t="inlineStr">
         <is>
-          <t>2024-11-24 06:00 Sun</t>
-        </is>
-      </c>
-      <c r="B15" s="121" t="n">
-        <v>8</v>
-      </c>
-      <c r="C15" s="121" t="n">
-        <v>-3</v>
-      </c>
-      <c r="D15" s="119" t="n">
-        <v>43</v>
+          <t>2025-01-28 00:00 mar</t>
+        </is>
+      </c>
+      <c r="B15" s="127" t="n">
+        <v>11</v>
+      </c>
+      <c r="C15" s="119" t="n">
+        <v>9</v>
+      </c>
+      <c r="D15" s="123" t="n">
+        <v>91</v>
       </c>
       <c r="E15" s="115" t="n">
         <v>0</v>
@@ -1569,36 +1569,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K15" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L15" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M15" s="130" t="inlineStr">
-        <is>
-          <t>30.9</t>
+      <c r="K15" s="120" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="L15" s="120" t="inlineStr">
+        <is>
+          <t>1.6</t>
+        </is>
+      </c>
+      <c r="M15" s="129" t="inlineStr">
+        <is>
+          <t>63.3</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="115" t="inlineStr">
         <is>
-          <t>2024-11-24 09:00 Sun</t>
+          <t>2025-01-28 03:00 mar</t>
         </is>
       </c>
       <c r="B16" s="127" t="n">
-        <v>13</v>
-      </c>
-      <c r="C16" s="121" t="n">
-        <v>-2</v>
-      </c>
-      <c r="D16" s="119" t="n">
-        <v>33</v>
+        <v>11</v>
+      </c>
+      <c r="C16" s="119" t="n">
+        <v>9</v>
+      </c>
+      <c r="D16" s="123" t="n">
+        <v>89</v>
       </c>
       <c r="E16" s="115" t="n">
         <v>0</v>
@@ -1631,31 +1631,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L16" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M16" s="120" t="inlineStr">
-        <is>
-          <t>1.7</t>
+      <c r="L16" s="127" t="inlineStr">
+        <is>
+          <t>23.1</t>
+        </is>
+      </c>
+      <c r="M16" s="130" t="inlineStr">
+        <is>
+          <t>52.6</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="115" t="inlineStr">
         <is>
-          <t>2024-11-24 12:00 Sun</t>
-        </is>
-      </c>
-      <c r="B17" s="119" t="n">
-        <v>14</v>
-      </c>
-      <c r="C17" s="121" t="n">
-        <v>-2</v>
-      </c>
-      <c r="D17" s="119" t="n">
-        <v>31</v>
+          <t>2025-01-28 06:00 mar</t>
+        </is>
+      </c>
+      <c r="B17" s="127" t="n">
+        <v>11</v>
+      </c>
+      <c r="C17" s="119" t="n">
+        <v>9</v>
+      </c>
+      <c r="D17" s="123" t="n">
+        <v>87</v>
       </c>
       <c r="E17" s="115" t="n">
         <v>0</v>
@@ -1688,31 +1688,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L17" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M17" s="120" t="inlineStr">
-        <is>
-          <t>0.8</t>
+      <c r="L17" s="126" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="M17" s="130" t="inlineStr">
+        <is>
+          <t>56.9</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="115" t="inlineStr">
         <is>
-          <t>2024-11-24 15:00 Sun</t>
-        </is>
-      </c>
-      <c r="B18" s="127" t="n">
+          <t>2025-01-28 09:00 mar</t>
+        </is>
+      </c>
+      <c r="B18" s="119" t="n">
+        <v>15</v>
+      </c>
+      <c r="C18" s="117" t="n">
         <v>11</v>
       </c>
-      <c r="C18" s="121" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" s="119" t="n">
-        <v>42</v>
+      <c r="D18" s="123" t="n">
+        <v>74</v>
       </c>
       <c r="E18" s="115" t="n">
         <v>0</v>
@@ -1740,9 +1740,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K18" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K18" s="120" t="inlineStr">
+        <is>
+          <t>0.1</t>
         </is>
       </c>
       <c r="L18" s="115" t="inlineStr">
@@ -1750,26 +1750,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M18" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M18" s="129" t="inlineStr">
+        <is>
+          <t>68.1</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="115" t="inlineStr">
         <is>
-          <t>2024-11-24 18:00 Sun</t>
-        </is>
-      </c>
-      <c r="B19" s="121" t="n">
-        <v>9</v>
-      </c>
-      <c r="C19" s="121" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" s="119" t="n">
-        <v>49</v>
+          <t>2025-01-28 12:00 mar</t>
+        </is>
+      </c>
+      <c r="B19" s="119" t="n">
+        <v>16</v>
+      </c>
+      <c r="C19" s="119" t="n">
+        <v>10</v>
+      </c>
+      <c r="D19" s="121" t="n">
+        <v>70</v>
       </c>
       <c r="E19" s="115" t="n">
         <v>0</v>
@@ -1797,36 +1797,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K19" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L19" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M19" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K19" s="120" t="inlineStr">
+        <is>
+          <t>1.7</t>
+        </is>
+      </c>
+      <c r="L19" s="120" t="inlineStr">
+        <is>
+          <t>3.9</t>
+        </is>
+      </c>
+      <c r="M19" s="129" t="inlineStr">
+        <is>
+          <t>74.5</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="115" t="inlineStr">
         <is>
-          <t>2024-11-24 21:00 Sun</t>
-        </is>
-      </c>
-      <c r="B20" s="121" t="n">
-        <v>9</v>
-      </c>
-      <c r="C20" s="121" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" s="119" t="n">
-        <v>51</v>
+          <t>2025-01-28 15:00 mar</t>
+        </is>
+      </c>
+      <c r="B20" s="119" t="n">
+        <v>15</v>
+      </c>
+      <c r="C20" s="117" t="n">
+        <v>12</v>
+      </c>
+      <c r="D20" s="123" t="n">
+        <v>85</v>
       </c>
       <c r="E20" s="115" t="n">
         <v>0</v>
@@ -1854,36 +1854,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K20" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L20" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M20" s="130" t="inlineStr">
-        <is>
-          <t>39.1</t>
+      <c r="K20" s="126" t="inlineStr">
+        <is>
+          <t>14.6</t>
+        </is>
+      </c>
+      <c r="L20" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="M20" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="115" t="inlineStr">
         <is>
-          <t>2024-11-25 00:00 Mon</t>
-        </is>
-      </c>
-      <c r="B21" s="121" t="n">
-        <v>8</v>
-      </c>
-      <c r="C21" s="121" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="119" t="n">
-        <v>53</v>
+          <t>2025-01-28 18:00 mar</t>
+        </is>
+      </c>
+      <c r="B21" s="127" t="n">
+        <v>13</v>
+      </c>
+      <c r="C21" s="117" t="n">
+        <v>12</v>
+      </c>
+      <c r="D21" s="123" t="n">
+        <v>93</v>
       </c>
       <c r="E21" s="115" t="n">
         <v>0</v>
@@ -1911,36 +1911,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K21" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L21" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M21" s="130" t="inlineStr">
-        <is>
-          <t>49.2</t>
+      <c r="K21" s="127" t="inlineStr">
+        <is>
+          <t>26.4</t>
+        </is>
+      </c>
+      <c r="L21" s="128" t="inlineStr">
+        <is>
+          <t>95.5</t>
+        </is>
+      </c>
+      <c r="M21" s="115" t="inlineStr">
+        <is>
+          <t>84</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="115" t="inlineStr">
         <is>
-          <t>2024-11-25 03:00 Mon</t>
-        </is>
-      </c>
-      <c r="B22" s="121" t="n">
-        <v>7</v>
-      </c>
-      <c r="C22" s="121" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="119" t="n">
-        <v>54</v>
+          <t>2025-01-28 21:00 mar</t>
+        </is>
+      </c>
+      <c r="B22" s="127" t="n">
+        <v>13</v>
+      </c>
+      <c r="C22" s="117" t="n">
+        <v>12</v>
+      </c>
+      <c r="D22" s="123" t="n">
+        <v>94</v>
       </c>
       <c r="E22" s="115" t="n">
         <v>0</v>
@@ -1968,36 +1968,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K22" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L22" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K22" s="125" t="inlineStr">
+        <is>
+          <t>6.2</t>
+        </is>
+      </c>
+      <c r="L22" s="127" t="inlineStr">
+        <is>
+          <t>24.7</t>
         </is>
       </c>
       <c r="M22" s="130" t="inlineStr">
         <is>
-          <t>36.6</t>
+          <t>37.6</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="115" t="inlineStr">
         <is>
-          <t>2024-11-25 06:00 Mon</t>
-        </is>
-      </c>
-      <c r="B23" s="121" t="n">
-        <v>7</v>
-      </c>
-      <c r="C23" s="121" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" s="119" t="n">
-        <v>56</v>
+          <t>2025-01-29 00:00 mer</t>
+        </is>
+      </c>
+      <c r="B23" s="127" t="n">
+        <v>13</v>
+      </c>
+      <c r="C23" s="117" t="n">
+        <v>12</v>
+      </c>
+      <c r="D23" s="123" t="n">
+        <v>96</v>
       </c>
       <c r="E23" s="115" t="n">
         <v>0</v>
@@ -2025,36 +2025,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K23" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L23" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M23" s="126" t="inlineStr">
-        <is>
-          <t>20.8</t>
+      <c r="K23" s="125" t="inlineStr">
+        <is>
+          <t>6.7</t>
+        </is>
+      </c>
+      <c r="L23" s="126" t="inlineStr">
+        <is>
+          <t>21.7</t>
+        </is>
+      </c>
+      <c r="M23" s="129" t="inlineStr">
+        <is>
+          <t>68.8</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="115" t="inlineStr">
         <is>
-          <t>2024-11-25 09:00 Mon</t>
+          <t>2025-01-29 03:00 mer</t>
         </is>
       </c>
       <c r="B24" s="127" t="n">
         <v>13</v>
       </c>
-      <c r="C24" s="121" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" s="119" t="n">
-        <v>43</v>
+      <c r="C24" s="117" t="n">
+        <v>12</v>
+      </c>
+      <c r="D24" s="123" t="n">
+        <v>94</v>
       </c>
       <c r="E24" s="115" t="n">
         <v>0</v>
@@ -2062,14 +2062,14 @@
       <c r="F24" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G24" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H24" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G24" s="131" t="inlineStr">
+        <is>
+          <t>0.000104</t>
+        </is>
+      </c>
+      <c r="H24" s="119" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I24" s="120" t="inlineStr">
@@ -2082,36 +2082,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K24" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L24" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M24" s="125" t="inlineStr">
-        <is>
-          <t>5.5</t>
+      <c r="K24" s="120" t="inlineStr">
+        <is>
+          <t>2.1</t>
+        </is>
+      </c>
+      <c r="L24" s="127" t="inlineStr">
+        <is>
+          <t>22.3</t>
+        </is>
+      </c>
+      <c r="M24" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="115" t="inlineStr">
         <is>
-          <t>2024-11-25 12:00 Mon</t>
-        </is>
-      </c>
-      <c r="B25" s="119" t="n">
-        <v>15</v>
-      </c>
-      <c r="C25" s="121" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" s="119" t="n">
-        <v>37</v>
+          <t>2025-01-29 06:00 mer</t>
+        </is>
+      </c>
+      <c r="B25" s="127" t="n">
+        <v>13</v>
+      </c>
+      <c r="C25" s="117" t="n">
+        <v>12</v>
+      </c>
+      <c r="D25" s="123" t="n">
+        <v>94</v>
       </c>
       <c r="E25" s="115" t="n">
         <v>0</v>
@@ -2119,14 +2119,14 @@
       <c r="F25" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G25" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H25" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G25" s="131" t="inlineStr">
+        <is>
+          <t>0.000388</t>
+        </is>
+      </c>
+      <c r="H25" s="119" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I25" s="120" t="inlineStr">
@@ -2139,36 +2139,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K25" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L25" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M25" s="125" t="inlineStr">
-        <is>
-          <t>5.2</t>
+      <c r="K25" s="125" t="inlineStr">
+        <is>
+          <t>6.1</t>
+        </is>
+      </c>
+      <c r="L25" s="130" t="inlineStr">
+        <is>
+          <t>35.6</t>
+        </is>
+      </c>
+      <c r="M25" s="115" t="inlineStr">
+        <is>
+          <t>83.2</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="115" t="inlineStr">
         <is>
-          <t>2024-11-25 15:00 Mon</t>
-        </is>
-      </c>
-      <c r="B26" s="127" t="n">
+          <t>2025-01-29 09:00 mer</t>
+        </is>
+      </c>
+      <c r="B26" s="119" t="n">
+        <v>15</v>
+      </c>
+      <c r="C26" s="117" t="n">
         <v>12</v>
       </c>
-      <c r="C26" s="121" t="n">
-        <v>3</v>
-      </c>
-      <c r="D26" s="119" t="n">
-        <v>54</v>
+      <c r="D26" s="123" t="n">
+        <v>78</v>
       </c>
       <c r="E26" s="115" t="n">
         <v>0</v>
@@ -2176,9 +2176,9 @@
       <c r="F26" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G26" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G26" s="131" t="inlineStr">
+        <is>
+          <t>0.000104</t>
         </is>
       </c>
       <c r="H26" s="120" t="inlineStr">
@@ -2196,36 +2196,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K26" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L26" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M26" s="120" t="inlineStr">
-        <is>
-          <t>1.7</t>
+      <c r="K26" s="129" t="inlineStr">
+        <is>
+          <t>68.5</t>
+        </is>
+      </c>
+      <c r="L26" s="125" t="inlineStr">
+        <is>
+          <t>6.3</t>
+        </is>
+      </c>
+      <c r="M26" s="128" t="inlineStr">
+        <is>
+          <t>85.3</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="115" t="inlineStr">
         <is>
-          <t>2024-11-25 18:00 Mon</t>
-        </is>
-      </c>
-      <c r="B27" s="121" t="n">
-        <v>10</v>
-      </c>
-      <c r="C27" s="121" t="n">
-        <v>4</v>
-      </c>
-      <c r="D27" s="121" t="n">
-        <v>64</v>
+          <t>2025-01-29 12:00 mer</t>
+        </is>
+      </c>
+      <c r="B27" s="119" t="n">
+        <v>15</v>
+      </c>
+      <c r="C27" s="117" t="n">
+        <v>11</v>
+      </c>
+      <c r="D27" s="123" t="n">
+        <v>79</v>
       </c>
       <c r="E27" s="115" t="n">
         <v>0</v>
@@ -2233,14 +2233,14 @@
       <c r="F27" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G27" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H27" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G27" s="131" t="inlineStr">
+        <is>
+          <t>0.000604</t>
+        </is>
+      </c>
+      <c r="H27" s="119" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I27" s="120" t="inlineStr">
@@ -2253,36 +2253,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K27" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L27" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M27" s="120" t="inlineStr">
-        <is>
-          <t>0.8</t>
+      <c r="K27" s="129" t="inlineStr">
+        <is>
+          <t>62.8</t>
+        </is>
+      </c>
+      <c r="L27" s="130" t="inlineStr">
+        <is>
+          <t>30.3</t>
+        </is>
+      </c>
+      <c r="M27" s="128" t="inlineStr">
+        <is>
+          <t>92.6</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="115" t="inlineStr">
         <is>
-          <t>2024-11-25 21:00 Mon</t>
-        </is>
-      </c>
-      <c r="B28" s="121" t="n">
-        <v>9</v>
-      </c>
-      <c r="C28" s="121" t="n">
-        <v>4</v>
-      </c>
-      <c r="D28" s="121" t="n">
-        <v>69</v>
+          <t>2025-01-29 15:00 mer</t>
+        </is>
+      </c>
+      <c r="B28" s="119" t="n">
+        <v>14</v>
+      </c>
+      <c r="C28" s="117" t="n">
+        <v>12</v>
+      </c>
+      <c r="D28" s="123" t="n">
+        <v>85</v>
       </c>
       <c r="E28" s="115" t="n">
         <v>0</v>
@@ -2290,14 +2290,14 @@
       <c r="F28" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G28" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H28" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G28" s="131" t="inlineStr">
+        <is>
+          <t>0.0003004</t>
+        </is>
+      </c>
+      <c r="H28" s="119" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I28" s="120" t="inlineStr">
@@ -2310,36 +2310,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K28" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L28" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M28" s="120" t="inlineStr">
-        <is>
-          <t>0.8</t>
+      <c r="K28" s="128" t="inlineStr">
+        <is>
+          <t>89.6</t>
+        </is>
+      </c>
+      <c r="L28" s="129" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="M28" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="115" t="inlineStr">
         <is>
-          <t>2024-11-26 00:00 Tue</t>
-        </is>
-      </c>
-      <c r="B29" s="121" t="n">
-        <v>8</v>
-      </c>
-      <c r="C29" s="121" t="n">
-        <v>4</v>
+          <t>2025-01-29 18:00 mer</t>
+        </is>
+      </c>
+      <c r="B29" s="127" t="n">
+        <v>13</v>
+      </c>
+      <c r="C29" s="117" t="n">
+        <v>11</v>
       </c>
       <c r="D29" s="123" t="n">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="E29" s="115" t="n">
         <v>0</v>
@@ -2347,14 +2347,14 @@
       <c r="F29" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G29" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H29" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G29" s="131" t="inlineStr">
+        <is>
+          <t>0.0003016</t>
+        </is>
+      </c>
+      <c r="H29" s="119" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I29" s="120" t="inlineStr">
@@ -2367,36 +2367,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K29" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L29" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M29" s="120" t="inlineStr">
-        <is>
-          <t>0.4</t>
+      <c r="K29" s="128" t="inlineStr">
+        <is>
+          <t>90.8</t>
+        </is>
+      </c>
+      <c r="L29" s="128" t="inlineStr">
+        <is>
+          <t>87.6</t>
+        </is>
+      </c>
+      <c r="M29" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="115" t="inlineStr">
         <is>
-          <t>2024-11-26 03:00 Tue</t>
-        </is>
-      </c>
-      <c r="B30" s="121" t="n">
-        <v>8</v>
-      </c>
-      <c r="C30" s="121" t="n">
-        <v>4</v>
+          <t>2025-01-29 21:00 mer</t>
+        </is>
+      </c>
+      <c r="B30" s="127" t="n">
+        <v>12</v>
+      </c>
+      <c r="C30" s="119" t="n">
+        <v>9</v>
       </c>
       <c r="D30" s="123" t="n">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E30" s="115" t="n">
         <v>0</v>
@@ -2404,9 +2404,9 @@
       <c r="F30" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G30" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G30" s="131" t="inlineStr">
+        <is>
+          <t>2.4e-06</t>
         </is>
       </c>
       <c r="H30" s="120" t="inlineStr">
@@ -2424,36 +2424,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K30" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L30" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M30" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K30" s="128" t="inlineStr">
+        <is>
+          <t>98.4</t>
+        </is>
+      </c>
+      <c r="L30" s="129" t="inlineStr">
+        <is>
+          <t>71.1</t>
+        </is>
+      </c>
+      <c r="M30" s="128" t="inlineStr">
+        <is>
+          <t>93.5</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="115" t="inlineStr">
         <is>
-          <t>2024-11-26 06:00 Tue</t>
-        </is>
-      </c>
-      <c r="B31" s="121" t="n">
-        <v>8</v>
-      </c>
-      <c r="C31" s="121" t="n">
-        <v>4</v>
+          <t>2025-01-30 00:00 gio</t>
+        </is>
+      </c>
+      <c r="B31" s="127" t="n">
+        <v>11</v>
+      </c>
+      <c r="C31" s="119" t="n">
+        <v>9</v>
       </c>
       <c r="D31" s="123" t="n">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="E31" s="115" t="n">
         <v>0</v>
@@ -2461,14 +2461,14 @@
       <c r="F31" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G31" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H31" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G31" s="131" t="inlineStr">
+        <is>
+          <t>0.0001488</t>
+        </is>
+      </c>
+      <c r="H31" s="119" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I31" s="120" t="inlineStr">
@@ -2481,36 +2481,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K31" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L31" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M31" s="120" t="inlineStr">
-        <is>
-          <t>0.8</t>
+      <c r="K31" s="130" t="inlineStr">
+        <is>
+          <t>54.6</t>
+        </is>
+      </c>
+      <c r="L31" s="130" t="inlineStr">
+        <is>
+          <t>35.6</t>
+        </is>
+      </c>
+      <c r="M31" s="130" t="inlineStr">
+        <is>
+          <t>48.6</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="115" t="inlineStr">
         <is>
-          <t>2024-11-26 09:00 Tue</t>
-        </is>
-      </c>
-      <c r="B32" s="119" t="n">
-        <v>14</v>
-      </c>
-      <c r="C32" s="121" t="n">
-        <v>2</v>
-      </c>
-      <c r="D32" s="119" t="n">
-        <v>45</v>
+          <t>2025-01-30 03:00 gio</t>
+        </is>
+      </c>
+      <c r="B32" s="121" t="n">
+        <v>10</v>
+      </c>
+      <c r="C32" s="119" t="n">
+        <v>9</v>
+      </c>
+      <c r="D32" s="123" t="n">
+        <v>93</v>
       </c>
       <c r="E32" s="115" t="n">
         <v>0</v>
@@ -2518,14 +2518,14 @@
       <c r="F32" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G32" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H32" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G32" s="131" t="inlineStr">
+        <is>
+          <t>0.000352</t>
+        </is>
+      </c>
+      <c r="H32" s="119" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I32" s="120" t="inlineStr">
@@ -2538,36 +2538,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K32" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L32" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M32" s="120" t="inlineStr">
-        <is>
-          <t>1.7</t>
+      <c r="K32" s="127" t="inlineStr">
+        <is>
+          <t>26.7</t>
+        </is>
+      </c>
+      <c r="L32" s="129" t="inlineStr">
+        <is>
+          <t>66.3</t>
+        </is>
+      </c>
+      <c r="M32" s="130" t="inlineStr">
+        <is>
+          <t>59.5</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="115" t="inlineStr">
         <is>
-          <t>2024-11-26 12:00 Tue</t>
-        </is>
-      </c>
-      <c r="B33" s="119" t="n">
-        <v>16</v>
-      </c>
-      <c r="C33" s="121" t="n">
-        <v>3</v>
-      </c>
-      <c r="D33" s="119" t="n">
-        <v>42</v>
+          <t>2025-01-30 06:00 gio</t>
+        </is>
+      </c>
+      <c r="B33" s="121" t="n">
+        <v>10</v>
+      </c>
+      <c r="C33" s="119" t="n">
+        <v>9</v>
+      </c>
+      <c r="D33" s="123" t="n">
+        <v>92</v>
       </c>
       <c r="E33" s="115" t="n">
         <v>0</v>
@@ -2575,14 +2575,14 @@
       <c r="F33" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G33" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H33" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G33" s="131" t="inlineStr">
+        <is>
+          <t>0.0001688</t>
+        </is>
+      </c>
+      <c r="H33" s="119" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I33" s="120" t="inlineStr">
@@ -2595,36 +2595,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K33" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L33" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M33" s="120" t="inlineStr">
-        <is>
-          <t>0.8</t>
+      <c r="K33" s="129" t="inlineStr">
+        <is>
+          <t>63.4</t>
+        </is>
+      </c>
+      <c r="L33" s="128" t="inlineStr">
+        <is>
+          <t>83.1</t>
+        </is>
+      </c>
+      <c r="M33" s="129" t="inlineStr">
+        <is>
+          <t>75.5</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="115" t="inlineStr">
         <is>
-          <t>2024-11-26 15:00 Tue</t>
-        </is>
-      </c>
-      <c r="B34" s="119" t="n">
-        <v>14</v>
+          <t>2025-01-30 09:00 gio</t>
+        </is>
+      </c>
+      <c r="B34" s="127" t="n">
+        <v>11</v>
       </c>
       <c r="C34" s="119" t="n">
-        <v>6</v>
-      </c>
-      <c r="D34" s="119" t="n">
-        <v>57</v>
+        <v>9</v>
+      </c>
+      <c r="D34" s="123" t="n">
+        <v>85</v>
       </c>
       <c r="E34" s="115" t="n">
         <v>0</v>
@@ -2632,14 +2632,14 @@
       <c r="F34" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G34" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H34" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G34" s="131" t="inlineStr">
+        <is>
+          <t>5.76e-05</t>
+        </is>
+      </c>
+      <c r="H34" s="119" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I34" s="120" t="inlineStr">
@@ -2652,36 +2652,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K34" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L34" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M34" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K34" s="128" t="inlineStr">
+        <is>
+          <t>99.6</t>
+        </is>
+      </c>
+      <c r="L34" s="127" t="inlineStr">
+        <is>
+          <t>29.2</t>
+        </is>
+      </c>
+      <c r="M34" s="127" t="inlineStr">
+        <is>
+          <t>23.6</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="115" t="inlineStr">
         <is>
-          <t>2024-11-26 18:00 Tue</t>
+          <t>2025-01-30 12:00 gio</t>
         </is>
       </c>
       <c r="B35" s="127" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C35" s="119" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D35" s="121" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E35" s="115" t="n">
         <v>0</v>
@@ -2689,14 +2689,14 @@
       <c r="F35" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G35" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H35" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G35" s="131" t="inlineStr">
+        <is>
+          <t>2.48e-05</t>
+        </is>
+      </c>
+      <c r="H35" s="119" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I35" s="120" t="inlineStr">
@@ -2709,36 +2709,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K35" s="120" t="inlineStr">
-        <is>
-          <t>1.7</t>
-        </is>
-      </c>
-      <c r="L35" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M35" s="120" t="inlineStr">
-        <is>
-          <t>1.4</t>
+      <c r="K35" s="128" t="inlineStr">
+        <is>
+          <t>82.1</t>
+        </is>
+      </c>
+      <c r="L35" s="126" t="inlineStr">
+        <is>
+          <t>14.6</t>
+        </is>
+      </c>
+      <c r="M35" s="126" t="inlineStr">
+        <is>
+          <t>12.6</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="115" t="inlineStr">
         <is>
-          <t>2024-11-26 21:00 Tue</t>
+          <t>2025-01-30 15:00 gio</t>
         </is>
       </c>
       <c r="B36" s="127" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C36" s="119" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D36" s="123" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E36" s="115" t="n">
         <v>0</v>
@@ -2746,14 +2746,14 @@
       <c r="F36" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G36" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H36" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G36" s="131" t="inlineStr">
+        <is>
+          <t>1.32e-05</t>
+        </is>
+      </c>
+      <c r="H36" s="119" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I36" s="120" t="inlineStr">
@@ -2766,33 +2766,33 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K36" s="120" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="L36" s="120" t="inlineStr">
-        <is>
-          <t>0.3</t>
+      <c r="K36" s="128" t="inlineStr">
+        <is>
+          <t>82.3</t>
+        </is>
+      </c>
+      <c r="L36" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="M36" s="127" t="inlineStr">
         <is>
-          <t>24.8</t>
+          <t>24.3</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="115" t="inlineStr">
         <is>
-          <t>2024-11-27 00:00 Wed</t>
+          <t>2025-01-30 18:00 gio</t>
         </is>
       </c>
       <c r="B37" s="121" t="n">
         <v>10</v>
       </c>
       <c r="C37" s="119" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D37" s="123" t="n">
         <v>78</v>
@@ -2823,36 +2823,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K37" s="120" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="L37" s="120" t="inlineStr">
-        <is>
-          <t>3.4</t>
+      <c r="K37" s="130" t="inlineStr">
+        <is>
+          <t>53.2</t>
+        </is>
+      </c>
+      <c r="L37" s="126" t="inlineStr">
+        <is>
+          <t>16.4</t>
         </is>
       </c>
       <c r="M37" s="126" t="inlineStr">
         <is>
-          <t>16.8</t>
+          <t>16.3</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="115" t="inlineStr">
         <is>
-          <t>2024-11-27 03:00 Wed</t>
+          <t>2025-01-30 21:00 gio</t>
         </is>
       </c>
       <c r="B38" s="121" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C38" s="119" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D38" s="123" t="n">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E38" s="115" t="n">
         <v>0</v>
@@ -2882,34 +2882,34 @@
       </c>
       <c r="K38" s="120" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="L38" s="120" t="inlineStr">
-        <is>
-          <t>5</t>
+          <t>0.8</t>
+        </is>
+      </c>
+      <c r="L38" s="130" t="inlineStr">
+        <is>
+          <t>54</t>
         </is>
       </c>
       <c r="M38" s="125" t="inlineStr">
         <is>
-          <t>8.9</t>
+          <t>9.4</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="115" t="inlineStr">
         <is>
-          <t>2024-11-27 06:00 Wed</t>
+          <t>2025-01-31 00:00 ven</t>
         </is>
       </c>
       <c r="B39" s="121" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C39" s="119" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D39" s="123" t="n">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E39" s="115" t="n">
         <v>0</v>
@@ -2939,34 +2939,34 @@
       </c>
       <c r="K39" s="120" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="L39" s="120" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="M39" s="126" t="inlineStr">
-        <is>
-          <t>14.5</t>
+          <t>0.4</t>
+        </is>
+      </c>
+      <c r="L39" s="130" t="inlineStr">
+        <is>
+          <t>33.3</t>
+        </is>
+      </c>
+      <c r="M39" s="130" t="inlineStr">
+        <is>
+          <t>54.5</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="115" t="inlineStr">
         <is>
-          <t>2024-11-27 09:00 Wed</t>
-        </is>
-      </c>
-      <c r="B40" s="119" t="n">
-        <v>15</v>
+          <t>2025-01-31 03:00 ven</t>
+        </is>
+      </c>
+      <c r="B40" s="121" t="n">
+        <v>9</v>
       </c>
       <c r="C40" s="119" t="n">
-        <v>8</v>
-      </c>
-      <c r="D40" s="121" t="n">
-        <v>61</v>
+        <v>7</v>
+      </c>
+      <c r="D40" s="123" t="n">
+        <v>84</v>
       </c>
       <c r="E40" s="115" t="n">
         <v>0</v>
@@ -2994,36 +2994,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K40" s="120" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="L40" s="125" t="inlineStr">
-        <is>
-          <t>6.5</t>
+      <c r="K40" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L40" s="127" t="inlineStr">
+        <is>
+          <t>28.3</t>
         </is>
       </c>
       <c r="M40" s="130" t="inlineStr">
         <is>
-          <t>48.6</t>
+          <t>34.9</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="115" t="inlineStr">
         <is>
-          <t>2024-11-27 12:00 Wed</t>
-        </is>
-      </c>
-      <c r="B41" s="119" t="n">
-        <v>18</v>
+          <t>2025-01-31 06:00 ven</t>
+        </is>
+      </c>
+      <c r="B41" s="121" t="n">
+        <v>9</v>
       </c>
       <c r="C41" s="119" t="n">
-        <v>9</v>
-      </c>
-      <c r="D41" s="119" t="n">
-        <v>54</v>
+        <v>7</v>
+      </c>
+      <c r="D41" s="123" t="n">
+        <v>86</v>
       </c>
       <c r="E41" s="115" t="n">
         <v>0</v>
@@ -3051,33 +3051,33 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K41" s="120" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="L41" s="125" t="inlineStr">
-        <is>
-          <t>8.3</t>
-        </is>
-      </c>
-      <c r="M41" s="130" t="inlineStr">
-        <is>
-          <t>36.3</t>
+      <c r="K41" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L41" s="127" t="inlineStr">
+        <is>
+          <t>23.9</t>
+        </is>
+      </c>
+      <c r="M41" s="126" t="inlineStr">
+        <is>
+          <t>18.3</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="115" t="inlineStr">
         <is>
-          <t>2024-11-27 15:00 Wed</t>
-        </is>
-      </c>
-      <c r="B42" s="119" t="n">
-        <v>16</v>
+          <t>2025-01-31 09:00 ven</t>
+        </is>
+      </c>
+      <c r="B42" s="127" t="n">
+        <v>13</v>
       </c>
       <c r="C42" s="119" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D42" s="121" t="n">
         <v>67</v>
@@ -3108,36 +3108,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K42" s="120" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="L42" s="125" t="inlineStr">
-        <is>
-          <t>6.2</t>
-        </is>
-      </c>
-      <c r="M42" s="126" t="inlineStr">
-        <is>
-          <t>17.6</t>
+      <c r="K42" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L42" s="120" t="inlineStr">
+        <is>
+          <t>1.7</t>
+        </is>
+      </c>
+      <c r="M42" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="115" t="inlineStr">
         <is>
-          <t>2024-11-27 18:00 Wed</t>
-        </is>
-      </c>
-      <c r="B43" s="127" t="n">
-        <v>13</v>
+          <t>2025-01-31 12:00 ven</t>
+        </is>
+      </c>
+      <c r="B43" s="119" t="n">
+        <v>15</v>
       </c>
       <c r="C43" s="119" t="n">
-        <v>10</v>
-      </c>
-      <c r="D43" s="123" t="n">
-        <v>80</v>
+        <v>7</v>
+      </c>
+      <c r="D43" s="119" t="n">
+        <v>59</v>
       </c>
       <c r="E43" s="115" t="n">
         <v>0</v>
@@ -3165,36 +3165,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K43" s="120" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="L43" s="125" t="inlineStr">
-        <is>
-          <t>5.6</t>
-        </is>
-      </c>
-      <c r="M43" s="126" t="inlineStr">
-        <is>
-          <t>13.6</t>
+      <c r="K43" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L43" s="120" t="inlineStr">
+        <is>
+          <t>0.8</t>
+        </is>
+      </c>
+      <c r="M43" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="115" t="inlineStr">
         <is>
-          <t>2024-11-27 21:00 Wed</t>
+          <t>2025-01-31 15:00 ven</t>
         </is>
       </c>
       <c r="B44" s="127" t="n">
         <v>13</v>
       </c>
       <c r="C44" s="119" t="n">
-        <v>10</v>
-      </c>
-      <c r="D44" s="123" t="n">
-        <v>84</v>
+        <v>8</v>
+      </c>
+      <c r="D44" s="121" t="n">
+        <v>70</v>
       </c>
       <c r="E44" s="115" t="n">
         <v>0</v>
@@ -3222,36 +3222,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K44" s="125" t="inlineStr">
-        <is>
-          <t>7.4</t>
-        </is>
-      </c>
-      <c r="L44" s="120" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="M44" s="125" t="inlineStr">
-        <is>
-          <t>5</t>
+      <c r="K44" s="120" t="inlineStr">
+        <is>
+          <t>2.6</t>
+        </is>
+      </c>
+      <c r="L44" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M44" s="130" t="inlineStr">
+        <is>
+          <t>30.1</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="115" t="inlineStr">
         <is>
-          <t>2024-11-28 00:00 Thu</t>
+          <t>2025-01-31 18:00 ven</t>
         </is>
       </c>
       <c r="B45" s="127" t="n">
-        <v>13</v>
-      </c>
-      <c r="C45" s="117" t="n">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="C45" s="119" t="n">
+        <v>8</v>
       </c>
       <c r="D45" s="123" t="n">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="E45" s="115" t="n">
         <v>0</v>
@@ -3279,19 +3279,19 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K45" s="127" t="inlineStr">
-        <is>
-          <t>26.7</t>
-        </is>
-      </c>
-      <c r="L45" s="120" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="M45" s="126" t="inlineStr">
-        <is>
-          <t>13.6</t>
+      <c r="K45" s="120" t="inlineStr">
+        <is>
+          <t>1.3</t>
+        </is>
+      </c>
+      <c r="L45" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M45" s="129" t="inlineStr">
+        <is>
+          <t>61.2</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added max and min Pressure on weather graph
</commit_message>
<xml_diff>
--- a/data/simpleWeather.xlsx
+++ b/data/simpleWeather.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Foglio1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Foglio1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
@@ -790,17 +790,17 @@
     <row r="2">
       <c r="A2" s="115" t="inlineStr">
         <is>
-          <t>2025-01-26 09:00 dom</t>
-        </is>
-      </c>
-      <c r="B2" s="119" t="n">
-        <v>14</v>
-      </c>
-      <c r="C2" s="117" t="n">
-        <v>11</v>
-      </c>
-      <c r="D2" s="123" t="n">
-        <v>77</v>
+          <t>2025-06-11 09:00 Wed</t>
+        </is>
+      </c>
+      <c r="B2" s="117" t="n">
+        <v>28</v>
+      </c>
+      <c r="C2" s="118" t="n">
+        <v>13</v>
+      </c>
+      <c r="D2" s="119" t="n">
+        <v>37</v>
       </c>
       <c r="E2" s="115" t="n">
         <v>0</v>
@@ -833,31 +833,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L2" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="M2" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="L2" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M2" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="115" t="inlineStr">
         <is>
-          <t>2025-01-26 12:00 dom</t>
-        </is>
-      </c>
-      <c r="B3" s="119" t="n">
-        <v>16</v>
-      </c>
-      <c r="C3" s="119" t="n">
-        <v>10</v>
-      </c>
-      <c r="D3" s="121" t="n">
-        <v>68</v>
+          <t>2025-06-11 12:00 Wed</t>
+        </is>
+      </c>
+      <c r="B3" s="117" t="n">
+        <v>29</v>
+      </c>
+      <c r="C3" s="117" t="n">
+        <v>12</v>
+      </c>
+      <c r="D3" s="119" t="n">
+        <v>35</v>
       </c>
       <c r="E3" s="115" t="n">
         <v>0</v>
@@ -890,31 +890,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L3" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="M3" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="L3" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M3" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="115" t="inlineStr">
         <is>
-          <t>2025-01-26 15:00 dom</t>
-        </is>
-      </c>
-      <c r="B4" s="119" t="n">
-        <v>14</v>
+          <t>2025-06-11 15:00 Wed</t>
+        </is>
+      </c>
+      <c r="B4" s="117" t="n">
+        <v>28</v>
       </c>
       <c r="C4" s="117" t="n">
-        <v>11</v>
-      </c>
-      <c r="D4" s="123" t="n">
-        <v>82</v>
+        <v>12</v>
+      </c>
+      <c r="D4" s="119" t="n">
+        <v>36</v>
       </c>
       <c r="E4" s="115" t="n">
         <v>0</v>
@@ -947,31 +947,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L4" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="M4" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="L4" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M4" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="115" t="inlineStr">
         <is>
-          <t>2025-01-26 18:00 dom</t>
-        </is>
-      </c>
-      <c r="B5" s="127" t="n">
-        <v>13</v>
-      </c>
-      <c r="C5" s="117" t="n">
-        <v>11</v>
-      </c>
-      <c r="D5" s="123" t="n">
-        <v>90</v>
+          <t>2025-06-11 18:00 Wed</t>
+        </is>
+      </c>
+      <c r="B5" s="117" t="n">
+        <v>23</v>
+      </c>
+      <c r="C5" s="118" t="n">
+        <v>14</v>
+      </c>
+      <c r="D5" s="119" t="n">
+        <v>55</v>
       </c>
       <c r="E5" s="115" t="n">
         <v>0</v>
@@ -1004,31 +1004,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L5" s="128" t="inlineStr">
-        <is>
-          <t>90.3</t>
-        </is>
-      </c>
-      <c r="M5" s="128" t="inlineStr">
-        <is>
-          <t>86</t>
+      <c r="L5" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M5" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="115" t="inlineStr">
         <is>
-          <t>2025-01-26 21:00 dom</t>
-        </is>
-      </c>
-      <c r="B6" s="127" t="n">
-        <v>12</v>
-      </c>
-      <c r="C6" s="117" t="n">
-        <v>11</v>
-      </c>
-      <c r="D6" s="123" t="n">
-        <v>91</v>
+          <t>2025-06-11 21:00 Wed</t>
+        </is>
+      </c>
+      <c r="B6" s="119" t="n">
+        <v>21</v>
+      </c>
+      <c r="C6" s="118" t="n">
+        <v>15</v>
+      </c>
+      <c r="D6" s="121" t="n">
+        <v>70</v>
       </c>
       <c r="E6" s="115" t="n">
         <v>0</v>
@@ -1061,31 +1061,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L6" s="130" t="inlineStr">
-        <is>
-          <t>35.3</t>
-        </is>
-      </c>
-      <c r="M6" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="L6" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M6" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="115" t="inlineStr">
         <is>
-          <t>2025-01-27 00:00 lun</t>
-        </is>
-      </c>
-      <c r="B7" s="127" t="n">
-        <v>11</v>
-      </c>
-      <c r="C7" s="117" t="n">
-        <v>11</v>
+          <t>2025-06-12 00:00 Thu</t>
+        </is>
+      </c>
+      <c r="B7" s="119" t="n">
+        <v>20</v>
+      </c>
+      <c r="C7" s="118" t="n">
+        <v>15</v>
       </c>
       <c r="D7" s="123" t="n">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="E7" s="115" t="n">
         <v>0</v>
@@ -1118,31 +1118,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L7" s="126" t="inlineStr">
-        <is>
-          <t>17.6</t>
-        </is>
-      </c>
-      <c r="M7" s="128" t="inlineStr">
-        <is>
-          <t>97.4</t>
+      <c r="L7" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M7" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="115" t="inlineStr">
         <is>
-          <t>2025-01-27 03:00 lun</t>
-        </is>
-      </c>
-      <c r="B8" s="127" t="n">
-        <v>11</v>
-      </c>
-      <c r="C8" s="119" t="n">
-        <v>10</v>
+          <t>2025-06-12 03:00 Thu</t>
+        </is>
+      </c>
+      <c r="B8" s="119" t="n">
+        <v>19</v>
+      </c>
+      <c r="C8" s="118" t="n">
+        <v>16</v>
       </c>
       <c r="D8" s="123" t="n">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E8" s="115" t="n">
         <v>0</v>
@@ -1180,26 +1180,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M8" s="120" t="inlineStr">
-        <is>
-          <t>0.5</t>
+      <c r="M8" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="115" t="inlineStr">
         <is>
-          <t>2025-01-27 06:00 lun</t>
-        </is>
-      </c>
-      <c r="B9" s="127" t="n">
-        <v>11</v>
-      </c>
-      <c r="C9" s="119" t="n">
-        <v>10</v>
-      </c>
-      <c r="D9" s="123" t="n">
-        <v>96</v>
+          <t>2025-06-12 06:00 Thu</t>
+        </is>
+      </c>
+      <c r="B9" s="117" t="n">
+        <v>25</v>
+      </c>
+      <c r="C9" s="118" t="n">
+        <v>15</v>
+      </c>
+      <c r="D9" s="119" t="n">
+        <v>53</v>
       </c>
       <c r="E9" s="115" t="n">
         <v>0</v>
@@ -1237,26 +1237,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M9" s="125" t="inlineStr">
-        <is>
-          <t>7.3</t>
+      <c r="M9" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="115" t="inlineStr">
         <is>
-          <t>2025-01-27 09:00 lun</t>
-        </is>
-      </c>
-      <c r="B10" s="119" t="n">
+          <t>2025-06-12 09:00 Thu</t>
+        </is>
+      </c>
+      <c r="B10" s="117" t="n">
+        <v>28</v>
+      </c>
+      <c r="C10" s="118" t="n">
         <v>15</v>
       </c>
-      <c r="C10" s="117" t="n">
-        <v>11</v>
-      </c>
-      <c r="D10" s="123" t="n">
-        <v>76</v>
+      <c r="D10" s="119" t="n">
+        <v>43</v>
       </c>
       <c r="E10" s="115" t="n">
         <v>0</v>
@@ -1284,9 +1284,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K10" s="120" t="inlineStr">
-        <is>
-          <t>1.2</t>
+      <c r="K10" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L10" s="115" t="inlineStr">
@@ -1294,26 +1294,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M10" s="125" t="inlineStr">
-        <is>
-          <t>6.5</t>
+      <c r="M10" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="115" t="inlineStr">
         <is>
-          <t>2025-01-27 12:00 lun</t>
-        </is>
-      </c>
-      <c r="B11" s="119" t="n">
-        <v>17</v>
-      </c>
-      <c r="C11" s="119" t="n">
-        <v>9</v>
+          <t>2025-06-12 12:00 Thu</t>
+        </is>
+      </c>
+      <c r="B11" s="117" t="n">
+        <v>29</v>
+      </c>
+      <c r="C11" s="118" t="n">
+        <v>15</v>
       </c>
       <c r="D11" s="119" t="n">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="E11" s="115" t="n">
         <v>0</v>
@@ -1341,9 +1341,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K11" s="120" t="inlineStr">
-        <is>
-          <t>0.6</t>
+      <c r="K11" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L11" s="115" t="inlineStr">
@@ -1351,26 +1351,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M11" s="130" t="inlineStr">
-        <is>
-          <t>37.4</t>
+      <c r="M11" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="115" t="inlineStr">
         <is>
-          <t>2025-01-27 15:00 lun</t>
-        </is>
-      </c>
-      <c r="B12" s="119" t="n">
-        <v>15</v>
-      </c>
-      <c r="C12" s="119" t="n">
-        <v>9</v>
-      </c>
-      <c r="D12" s="121" t="n">
-        <v>65</v>
+          <t>2025-06-12 15:00 Thu</t>
+        </is>
+      </c>
+      <c r="B12" s="117" t="n">
+        <v>28</v>
+      </c>
+      <c r="C12" s="118" t="n">
+        <v>14</v>
+      </c>
+      <c r="D12" s="119" t="n">
+        <v>41</v>
       </c>
       <c r="E12" s="115" t="n">
         <v>0</v>
@@ -1408,26 +1408,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M12" s="130" t="inlineStr">
-        <is>
-          <t>38</t>
+      <c r="M12" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="115" t="inlineStr">
         <is>
-          <t>2025-01-27 18:00 lun</t>
-        </is>
-      </c>
-      <c r="B13" s="127" t="n">
-        <v>12</v>
-      </c>
-      <c r="C13" s="117" t="n">
-        <v>11</v>
-      </c>
-      <c r="D13" s="123" t="n">
-        <v>95</v>
+          <t>2025-06-12 18:00 Thu</t>
+        </is>
+      </c>
+      <c r="B13" s="117" t="n">
+        <v>24</v>
+      </c>
+      <c r="C13" s="118" t="n">
+        <v>16</v>
+      </c>
+      <c r="D13" s="119" t="n">
+        <v>60</v>
       </c>
       <c r="E13" s="115" t="n">
         <v>0</v>
@@ -1465,26 +1465,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M13" s="126" t="inlineStr">
-        <is>
-          <t>21.5</t>
+      <c r="M13" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="115" t="inlineStr">
         <is>
-          <t>2025-01-27 21:00 lun</t>
-        </is>
-      </c>
-      <c r="B14" s="127" t="n">
-        <v>11</v>
-      </c>
-      <c r="C14" s="119" t="n">
-        <v>9</v>
+          <t>2025-06-12 21:00 Thu</t>
+        </is>
+      </c>
+      <c r="B14" s="119" t="n">
+        <v>22</v>
+      </c>
+      <c r="C14" s="118" t="n">
+        <v>17</v>
       </c>
       <c r="D14" s="123" t="n">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="E14" s="115" t="n">
         <v>0</v>
@@ -1512,9 +1512,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K14" s="120" t="inlineStr">
-        <is>
-          <t>0.3</t>
+      <c r="K14" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L14" s="115" t="inlineStr">
@@ -1522,26 +1522,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M14" s="128" t="inlineStr">
-        <is>
-          <t>90.3</t>
+      <c r="M14" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="115" t="inlineStr">
         <is>
-          <t>2025-01-28 00:00 mar</t>
-        </is>
-      </c>
-      <c r="B15" s="127" t="n">
-        <v>11</v>
-      </c>
-      <c r="C15" s="119" t="n">
-        <v>9</v>
+          <t>2025-06-13 00:00 Fri</t>
+        </is>
+      </c>
+      <c r="B15" s="119" t="n">
+        <v>21</v>
+      </c>
+      <c r="C15" s="118" t="n">
+        <v>16</v>
       </c>
       <c r="D15" s="123" t="n">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="E15" s="115" t="n">
         <v>0</v>
@@ -1569,36 +1569,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K15" s="120" t="inlineStr">
-        <is>
-          <t>0.2</t>
-        </is>
-      </c>
-      <c r="L15" s="120" t="inlineStr">
-        <is>
-          <t>1.6</t>
-        </is>
-      </c>
-      <c r="M15" s="129" t="inlineStr">
-        <is>
-          <t>63.3</t>
+      <c r="K15" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L15" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M15" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="115" t="inlineStr">
         <is>
-          <t>2025-01-28 03:00 mar</t>
-        </is>
-      </c>
-      <c r="B16" s="127" t="n">
-        <v>11</v>
-      </c>
-      <c r="C16" s="119" t="n">
-        <v>9</v>
+          <t>2025-06-13 03:00 Fri</t>
+        </is>
+      </c>
+      <c r="B16" s="119" t="n">
+        <v>20</v>
+      </c>
+      <c r="C16" s="118" t="n">
+        <v>17</v>
       </c>
       <c r="D16" s="123" t="n">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="E16" s="115" t="n">
         <v>0</v>
@@ -1631,31 +1631,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L16" s="127" t="inlineStr">
-        <is>
-          <t>23.1</t>
-        </is>
-      </c>
-      <c r="M16" s="130" t="inlineStr">
-        <is>
-          <t>52.6</t>
+      <c r="L16" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M16" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="115" t="inlineStr">
         <is>
-          <t>2025-01-28 06:00 mar</t>
-        </is>
-      </c>
-      <c r="B17" s="127" t="n">
-        <v>11</v>
-      </c>
-      <c r="C17" s="119" t="n">
-        <v>9</v>
-      </c>
-      <c r="D17" s="123" t="n">
-        <v>87</v>
+          <t>2025-06-13 06:00 Fri</t>
+        </is>
+      </c>
+      <c r="B17" s="117" t="n">
+        <v>26</v>
+      </c>
+      <c r="C17" s="118" t="n">
+        <v>15</v>
+      </c>
+      <c r="D17" s="119" t="n">
+        <v>51</v>
       </c>
       <c r="E17" s="115" t="n">
         <v>0</v>
@@ -1688,31 +1688,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L17" s="126" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="M17" s="130" t="inlineStr">
-        <is>
-          <t>56.9</t>
+      <c r="L17" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M17" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="115" t="inlineStr">
         <is>
-          <t>2025-01-28 09:00 mar</t>
-        </is>
-      </c>
-      <c r="B18" s="119" t="n">
-        <v>15</v>
-      </c>
-      <c r="C18" s="117" t="n">
-        <v>11</v>
-      </c>
-      <c r="D18" s="123" t="n">
-        <v>74</v>
+          <t>2025-06-13 09:00 Fri</t>
+        </is>
+      </c>
+      <c r="B18" s="117" t="n">
+        <v>30</v>
+      </c>
+      <c r="C18" s="118" t="n">
+        <v>13</v>
+      </c>
+      <c r="D18" s="119" t="n">
+        <v>35</v>
       </c>
       <c r="E18" s="115" t="n">
         <v>0</v>
@@ -1740,9 +1740,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K18" s="120" t="inlineStr">
-        <is>
-          <t>0.1</t>
+      <c r="K18" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L18" s="115" t="inlineStr">
@@ -1750,26 +1750,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M18" s="129" t="inlineStr">
-        <is>
-          <t>68.1</t>
+      <c r="M18" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="115" t="inlineStr">
         <is>
-          <t>2025-01-28 12:00 mar</t>
-        </is>
-      </c>
-      <c r="B19" s="119" t="n">
-        <v>16</v>
-      </c>
-      <c r="C19" s="119" t="n">
-        <v>10</v>
-      </c>
-      <c r="D19" s="121" t="n">
-        <v>70</v>
+          <t>2025-06-13 12:00 Fri</t>
+        </is>
+      </c>
+      <c r="B19" s="118" t="n">
+        <v>31</v>
+      </c>
+      <c r="C19" s="117" t="n">
+        <v>12</v>
+      </c>
+      <c r="D19" s="119" t="n">
+        <v>32</v>
       </c>
       <c r="E19" s="115" t="n">
         <v>0</v>
@@ -1797,36 +1797,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K19" s="120" t="inlineStr">
-        <is>
-          <t>1.7</t>
-        </is>
-      </c>
-      <c r="L19" s="120" t="inlineStr">
-        <is>
-          <t>3.9</t>
-        </is>
-      </c>
-      <c r="M19" s="129" t="inlineStr">
-        <is>
-          <t>74.5</t>
+      <c r="K19" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L19" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M19" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="115" t="inlineStr">
         <is>
-          <t>2025-01-28 15:00 mar</t>
-        </is>
-      </c>
-      <c r="B20" s="119" t="n">
-        <v>15</v>
+          <t>2025-06-13 15:00 Fri</t>
+        </is>
+      </c>
+      <c r="B20" s="117" t="n">
+        <v>29</v>
       </c>
       <c r="C20" s="117" t="n">
         <v>12</v>
       </c>
-      <c r="D20" s="123" t="n">
-        <v>85</v>
+      <c r="D20" s="119" t="n">
+        <v>35</v>
       </c>
       <c r="E20" s="115" t="n">
         <v>0</v>
@@ -1854,36 +1854,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K20" s="126" t="inlineStr">
-        <is>
-          <t>14.6</t>
-        </is>
-      </c>
-      <c r="L20" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="M20" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="K20" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L20" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M20" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="115" t="inlineStr">
         <is>
-          <t>2025-01-28 18:00 mar</t>
-        </is>
-      </c>
-      <c r="B21" s="127" t="n">
-        <v>13</v>
-      </c>
-      <c r="C21" s="117" t="n">
-        <v>12</v>
-      </c>
-      <c r="D21" s="123" t="n">
-        <v>93</v>
+          <t>2025-06-13 18:00 Fri</t>
+        </is>
+      </c>
+      <c r="B21" s="117" t="n">
+        <v>24</v>
+      </c>
+      <c r="C21" s="118" t="n">
+        <v>16</v>
+      </c>
+      <c r="D21" s="119" t="n">
+        <v>59</v>
       </c>
       <c r="E21" s="115" t="n">
         <v>0</v>
@@ -1911,36 +1911,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K21" s="127" t="inlineStr">
-        <is>
-          <t>26.4</t>
-        </is>
-      </c>
-      <c r="L21" s="128" t="inlineStr">
-        <is>
-          <t>95.5</t>
+      <c r="K21" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L21" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="M21" s="115" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="115" t="inlineStr">
         <is>
-          <t>2025-01-28 21:00 mar</t>
-        </is>
-      </c>
-      <c r="B22" s="127" t="n">
-        <v>13</v>
-      </c>
-      <c r="C22" s="117" t="n">
-        <v>12</v>
+          <t>2025-06-13 21:00 Fri</t>
+        </is>
+      </c>
+      <c r="B22" s="119" t="n">
+        <v>22</v>
+      </c>
+      <c r="C22" s="122" t="n">
+        <v>18</v>
       </c>
       <c r="D22" s="123" t="n">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="E22" s="115" t="n">
         <v>0</v>
@@ -1968,36 +1968,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K22" s="125" t="inlineStr">
-        <is>
-          <t>6.2</t>
-        </is>
-      </c>
-      <c r="L22" s="127" t="inlineStr">
-        <is>
-          <t>24.7</t>
-        </is>
-      </c>
-      <c r="M22" s="130" t="inlineStr">
-        <is>
-          <t>37.6</t>
+      <c r="K22" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L22" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M22" s="120" t="inlineStr">
+        <is>
+          <t>3.3</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="115" t="inlineStr">
         <is>
-          <t>2025-01-29 00:00 mer</t>
-        </is>
-      </c>
-      <c r="B23" s="127" t="n">
-        <v>13</v>
-      </c>
-      <c r="C23" s="117" t="n">
-        <v>12</v>
+          <t>2025-06-14 00:00 Sat</t>
+        </is>
+      </c>
+      <c r="B23" s="119" t="n">
+        <v>21</v>
+      </c>
+      <c r="C23" s="122" t="n">
+        <v>18</v>
       </c>
       <c r="D23" s="123" t="n">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E23" s="115" t="n">
         <v>0</v>
@@ -2025,36 +2025,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K23" s="125" t="inlineStr">
-        <is>
-          <t>6.7</t>
-        </is>
-      </c>
-      <c r="L23" s="126" t="inlineStr">
-        <is>
-          <t>21.7</t>
-        </is>
-      </c>
-      <c r="M23" s="129" t="inlineStr">
-        <is>
-          <t>68.8</t>
+      <c r="K23" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L23" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M23" s="120" t="inlineStr">
+        <is>
+          <t>1.7</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="115" t="inlineStr">
         <is>
-          <t>2025-01-29 03:00 mer</t>
-        </is>
-      </c>
-      <c r="B24" s="127" t="n">
-        <v>13</v>
-      </c>
-      <c r="C24" s="117" t="n">
-        <v>12</v>
+          <t>2025-06-14 03:00 Sat</t>
+        </is>
+      </c>
+      <c r="B24" s="119" t="n">
+        <v>21</v>
+      </c>
+      <c r="C24" s="122" t="n">
+        <v>18</v>
       </c>
       <c r="D24" s="123" t="n">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E24" s="115" t="n">
         <v>0</v>
@@ -2062,14 +2062,14 @@
       <c r="F24" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G24" s="131" t="inlineStr">
-        <is>
-          <t>0.000104</t>
-        </is>
-      </c>
-      <c r="H24" s="119" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="G24" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H24" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="I24" s="120" t="inlineStr">
@@ -2082,36 +2082,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K24" s="120" t="inlineStr">
-        <is>
-          <t>2.1</t>
-        </is>
-      </c>
-      <c r="L24" s="127" t="inlineStr">
-        <is>
-          <t>22.3</t>
-        </is>
-      </c>
-      <c r="M24" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="K24" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L24" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M24" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="115" t="inlineStr">
         <is>
-          <t>2025-01-29 06:00 mer</t>
-        </is>
-      </c>
-      <c r="B25" s="127" t="n">
-        <v>13</v>
-      </c>
-      <c r="C25" s="117" t="n">
-        <v>12</v>
-      </c>
-      <c r="D25" s="123" t="n">
-        <v>94</v>
+          <t>2025-06-14 06:00 Sat</t>
+        </is>
+      </c>
+      <c r="B25" s="117" t="n">
+        <v>26</v>
+      </c>
+      <c r="C25" s="118" t="n">
+        <v>17</v>
+      </c>
+      <c r="D25" s="119" t="n">
+        <v>58</v>
       </c>
       <c r="E25" s="115" t="n">
         <v>0</v>
@@ -2119,14 +2119,14 @@
       <c r="F25" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G25" s="131" t="inlineStr">
-        <is>
-          <t>0.000388</t>
-        </is>
-      </c>
-      <c r="H25" s="119" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="G25" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H25" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="I25" s="120" t="inlineStr">
@@ -2139,36 +2139,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K25" s="125" t="inlineStr">
-        <is>
-          <t>6.1</t>
-        </is>
-      </c>
-      <c r="L25" s="130" t="inlineStr">
-        <is>
-          <t>35.6</t>
+      <c r="K25" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L25" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="M25" s="115" t="inlineStr">
         <is>
-          <t>83.2</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="115" t="inlineStr">
         <is>
-          <t>2025-01-29 09:00 mer</t>
-        </is>
-      </c>
-      <c r="B26" s="119" t="n">
-        <v>15</v>
-      </c>
-      <c r="C26" s="117" t="n">
-        <v>12</v>
-      </c>
-      <c r="D26" s="123" t="n">
-        <v>78</v>
+          <t>2025-06-14 09:00 Sat</t>
+        </is>
+      </c>
+      <c r="B26" s="117" t="n">
+        <v>29</v>
+      </c>
+      <c r="C26" s="118" t="n">
+        <v>17</v>
+      </c>
+      <c r="D26" s="119" t="n">
+        <v>50</v>
       </c>
       <c r="E26" s="115" t="n">
         <v>0</v>
@@ -2176,9 +2176,9 @@
       <c r="F26" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G26" s="131" t="inlineStr">
-        <is>
-          <t>0.000104</t>
+      <c r="G26" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H26" s="120" t="inlineStr">
@@ -2196,36 +2196,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K26" s="129" t="inlineStr">
-        <is>
-          <t>68.5</t>
-        </is>
-      </c>
-      <c r="L26" s="125" t="inlineStr">
-        <is>
-          <t>6.3</t>
-        </is>
-      </c>
-      <c r="M26" s="128" t="inlineStr">
-        <is>
-          <t>85.3</t>
+      <c r="K26" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L26" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M26" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="115" t="inlineStr">
         <is>
-          <t>2025-01-29 12:00 mer</t>
-        </is>
-      </c>
-      <c r="B27" s="119" t="n">
-        <v>15</v>
-      </c>
-      <c r="C27" s="117" t="n">
-        <v>11</v>
-      </c>
-      <c r="D27" s="123" t="n">
-        <v>79</v>
+          <t>2025-06-14 12:00 Sat</t>
+        </is>
+      </c>
+      <c r="B27" s="117" t="n">
+        <v>30</v>
+      </c>
+      <c r="C27" s="118" t="n">
+        <v>14</v>
+      </c>
+      <c r="D27" s="119" t="n">
+        <v>37</v>
       </c>
       <c r="E27" s="115" t="n">
         <v>0</v>
@@ -2233,14 +2233,14 @@
       <c r="F27" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G27" s="131" t="inlineStr">
-        <is>
-          <t>0.000604</t>
-        </is>
-      </c>
-      <c r="H27" s="119" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="G27" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H27" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="I27" s="120" t="inlineStr">
@@ -2253,36 +2253,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K27" s="129" t="inlineStr">
-        <is>
-          <t>62.8</t>
-        </is>
-      </c>
-      <c r="L27" s="130" t="inlineStr">
-        <is>
-          <t>30.3</t>
-        </is>
-      </c>
-      <c r="M27" s="128" t="inlineStr">
-        <is>
-          <t>92.6</t>
+      <c r="K27" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L27" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M27" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="115" t="inlineStr">
         <is>
-          <t>2025-01-29 15:00 mer</t>
-        </is>
-      </c>
-      <c r="B28" s="119" t="n">
-        <v>14</v>
+          <t>2025-06-14 15:00 Sat</t>
+        </is>
+      </c>
+      <c r="B28" s="117" t="n">
+        <v>29</v>
       </c>
       <c r="C28" s="117" t="n">
-        <v>12</v>
-      </c>
-      <c r="D28" s="123" t="n">
-        <v>85</v>
+        <v>11</v>
+      </c>
+      <c r="D28" s="119" t="n">
+        <v>32</v>
       </c>
       <c r="E28" s="115" t="n">
         <v>0</v>
@@ -2290,14 +2290,14 @@
       <c r="F28" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G28" s="131" t="inlineStr">
-        <is>
-          <t>0.0003004</t>
-        </is>
-      </c>
-      <c r="H28" s="119" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="G28" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H28" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="I28" s="120" t="inlineStr">
@@ -2310,36 +2310,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K28" s="128" t="inlineStr">
-        <is>
-          <t>89.6</t>
-        </is>
-      </c>
-      <c r="L28" s="129" t="inlineStr">
-        <is>
-          <t>77</t>
-        </is>
-      </c>
-      <c r="M28" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="K28" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L28" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M28" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="115" t="inlineStr">
         <is>
-          <t>2025-01-29 18:00 mer</t>
-        </is>
-      </c>
-      <c r="B29" s="127" t="n">
-        <v>13</v>
-      </c>
-      <c r="C29" s="117" t="n">
-        <v>11</v>
-      </c>
-      <c r="D29" s="123" t="n">
-        <v>87</v>
+          <t>2025-06-14 18:00 Sat</t>
+        </is>
+      </c>
+      <c r="B29" s="117" t="n">
+        <v>24</v>
+      </c>
+      <c r="C29" s="118" t="n">
+        <v>15</v>
+      </c>
+      <c r="D29" s="119" t="n">
+        <v>55</v>
       </c>
       <c r="E29" s="115" t="n">
         <v>0</v>
@@ -2347,14 +2347,14 @@
       <c r="F29" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G29" s="131" t="inlineStr">
-        <is>
-          <t>0.0003016</t>
-        </is>
-      </c>
-      <c r="H29" s="119" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="G29" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H29" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="I29" s="120" t="inlineStr">
@@ -2367,36 +2367,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K29" s="128" t="inlineStr">
-        <is>
-          <t>90.8</t>
-        </is>
-      </c>
-      <c r="L29" s="128" t="inlineStr">
-        <is>
-          <t>87.6</t>
-        </is>
-      </c>
-      <c r="M29" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="K29" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L29" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M29" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="115" t="inlineStr">
         <is>
-          <t>2025-01-29 21:00 mer</t>
-        </is>
-      </c>
-      <c r="B30" s="127" t="n">
-        <v>12</v>
-      </c>
-      <c r="C30" s="119" t="n">
-        <v>9</v>
-      </c>
-      <c r="D30" s="123" t="n">
-        <v>83</v>
+          <t>2025-06-14 21:00 Sat</t>
+        </is>
+      </c>
+      <c r="B30" s="119" t="n">
+        <v>22</v>
+      </c>
+      <c r="C30" s="118" t="n">
+        <v>16</v>
+      </c>
+      <c r="D30" s="121" t="n">
+        <v>66</v>
       </c>
       <c r="E30" s="115" t="n">
         <v>0</v>
@@ -2404,9 +2404,9 @@
       <c r="F30" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G30" s="131" t="inlineStr">
-        <is>
-          <t>2.4e-06</t>
+      <c r="G30" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H30" s="120" t="inlineStr">
@@ -2424,36 +2424,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K30" s="128" t="inlineStr">
-        <is>
-          <t>98.4</t>
-        </is>
-      </c>
-      <c r="L30" s="129" t="inlineStr">
-        <is>
-          <t>71.1</t>
-        </is>
-      </c>
-      <c r="M30" s="128" t="inlineStr">
-        <is>
-          <t>93.5</t>
+      <c r="K30" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L30" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M30" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="115" t="inlineStr">
         <is>
-          <t>2025-01-30 00:00 gio</t>
-        </is>
-      </c>
-      <c r="B31" s="127" t="n">
-        <v>11</v>
-      </c>
-      <c r="C31" s="119" t="n">
-        <v>9</v>
-      </c>
-      <c r="D31" s="123" t="n">
-        <v>87</v>
+          <t>2025-06-15 00:00 Sun</t>
+        </is>
+      </c>
+      <c r="B31" s="119" t="n">
+        <v>22</v>
+      </c>
+      <c r="C31" s="118" t="n">
+        <v>16</v>
+      </c>
+      <c r="D31" s="121" t="n">
+        <v>70</v>
       </c>
       <c r="E31" s="115" t="n">
         <v>0</v>
@@ -2461,14 +2461,14 @@
       <c r="F31" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G31" s="131" t="inlineStr">
-        <is>
-          <t>0.0001488</t>
-        </is>
-      </c>
-      <c r="H31" s="119" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="G31" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H31" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="I31" s="120" t="inlineStr">
@@ -2481,36 +2481,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K31" s="130" t="inlineStr">
-        <is>
-          <t>54.6</t>
-        </is>
-      </c>
-      <c r="L31" s="130" t="inlineStr">
-        <is>
-          <t>35.6</t>
-        </is>
-      </c>
-      <c r="M31" s="130" t="inlineStr">
-        <is>
-          <t>48.6</t>
+      <c r="K31" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L31" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M31" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="115" t="inlineStr">
         <is>
-          <t>2025-01-30 03:00 gio</t>
-        </is>
-      </c>
-      <c r="B32" s="121" t="n">
-        <v>10</v>
-      </c>
-      <c r="C32" s="119" t="n">
-        <v>9</v>
+          <t>2025-06-15 03:00 Sun</t>
+        </is>
+      </c>
+      <c r="B32" s="119" t="n">
+        <v>21</v>
+      </c>
+      <c r="C32" s="118" t="n">
+        <v>17</v>
       </c>
       <c r="D32" s="123" t="n">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="E32" s="115" t="n">
         <v>0</v>
@@ -2518,14 +2518,14 @@
       <c r="F32" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G32" s="131" t="inlineStr">
-        <is>
-          <t>0.000352</t>
-        </is>
-      </c>
-      <c r="H32" s="119" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="G32" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H32" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="I32" s="120" t="inlineStr">
@@ -2538,36 +2538,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K32" s="127" t="inlineStr">
-        <is>
-          <t>26.7</t>
-        </is>
-      </c>
-      <c r="L32" s="129" t="inlineStr">
-        <is>
-          <t>66.3</t>
-        </is>
-      </c>
-      <c r="M32" s="130" t="inlineStr">
-        <is>
-          <t>59.5</t>
+      <c r="K32" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L32" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M32" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="115" t="inlineStr">
         <is>
-          <t>2025-01-30 06:00 gio</t>
-        </is>
-      </c>
-      <c r="B33" s="121" t="n">
-        <v>10</v>
-      </c>
-      <c r="C33" s="119" t="n">
-        <v>9</v>
-      </c>
-      <c r="D33" s="123" t="n">
-        <v>92</v>
+          <t>2025-06-15 06:00 Sun</t>
+        </is>
+      </c>
+      <c r="B33" s="117" t="n">
+        <v>25</v>
+      </c>
+      <c r="C33" s="117" t="n">
+        <v>12</v>
+      </c>
+      <c r="D33" s="119" t="n">
+        <v>45</v>
       </c>
       <c r="E33" s="115" t="n">
         <v>0</v>
@@ -2575,14 +2575,14 @@
       <c r="F33" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G33" s="131" t="inlineStr">
-        <is>
-          <t>0.0001688</t>
-        </is>
-      </c>
-      <c r="H33" s="119" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="G33" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H33" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="I33" s="120" t="inlineStr">
@@ -2595,36 +2595,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K33" s="129" t="inlineStr">
-        <is>
-          <t>63.4</t>
-        </is>
-      </c>
-      <c r="L33" s="128" t="inlineStr">
-        <is>
-          <t>83.1</t>
-        </is>
-      </c>
-      <c r="M33" s="129" t="inlineStr">
-        <is>
-          <t>75.5</t>
+      <c r="K33" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L33" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M33" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="115" t="inlineStr">
         <is>
-          <t>2025-01-30 09:00 gio</t>
-        </is>
-      </c>
-      <c r="B34" s="127" t="n">
-        <v>11</v>
-      </c>
-      <c r="C34" s="119" t="n">
-        <v>9</v>
-      </c>
-      <c r="D34" s="123" t="n">
-        <v>85</v>
+          <t>2025-06-15 09:00 Sun</t>
+        </is>
+      </c>
+      <c r="B34" s="117" t="n">
+        <v>27</v>
+      </c>
+      <c r="C34" s="118" t="n">
+        <v>13</v>
+      </c>
+      <c r="D34" s="119" t="n">
+        <v>39</v>
       </c>
       <c r="E34" s="115" t="n">
         <v>0</v>
@@ -2632,14 +2632,14 @@
       <c r="F34" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G34" s="131" t="inlineStr">
-        <is>
-          <t>5.76e-05</t>
-        </is>
-      </c>
-      <c r="H34" s="119" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="G34" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H34" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="I34" s="120" t="inlineStr">
@@ -2652,36 +2652,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K34" s="128" t="inlineStr">
-        <is>
-          <t>99.6</t>
-        </is>
-      </c>
-      <c r="L34" s="127" t="inlineStr">
-        <is>
-          <t>29.2</t>
-        </is>
-      </c>
-      <c r="M34" s="127" t="inlineStr">
-        <is>
-          <t>23.6</t>
+      <c r="K34" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L34" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M34" s="120" t="inlineStr">
+        <is>
+          <t>0.5</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="115" t="inlineStr">
         <is>
-          <t>2025-01-30 12:00 gio</t>
-        </is>
-      </c>
-      <c r="B35" s="127" t="n">
-        <v>13</v>
+          <t>2025-06-15 12:00 Sun</t>
+        </is>
+      </c>
+      <c r="B35" s="117" t="n">
+        <v>29</v>
       </c>
       <c r="C35" s="119" t="n">
-        <v>7</v>
-      </c>
-      <c r="D35" s="121" t="n">
-        <v>64</v>
+        <v>10</v>
+      </c>
+      <c r="D35" s="119" t="n">
+        <v>31</v>
       </c>
       <c r="E35" s="115" t="n">
         <v>0</v>
@@ -2689,14 +2689,14 @@
       <c r="F35" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G35" s="131" t="inlineStr">
-        <is>
-          <t>2.48e-05</t>
-        </is>
-      </c>
-      <c r="H35" s="119" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="G35" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H35" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="I35" s="120" t="inlineStr">
@@ -2709,36 +2709,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K35" s="128" t="inlineStr">
-        <is>
-          <t>82.1</t>
-        </is>
-      </c>
-      <c r="L35" s="126" t="inlineStr">
-        <is>
-          <t>14.6</t>
-        </is>
-      </c>
-      <c r="M35" s="126" t="inlineStr">
-        <is>
-          <t>12.6</t>
+      <c r="K35" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L35" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M35" s="120" t="inlineStr">
+        <is>
+          <t>0.2</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="115" t="inlineStr">
         <is>
-          <t>2025-01-30 15:00 gio</t>
-        </is>
-      </c>
-      <c r="B36" s="127" t="n">
-        <v>13</v>
+          <t>2025-06-15 15:00 Sun</t>
+        </is>
+      </c>
+      <c r="B36" s="117" t="n">
+        <v>28</v>
       </c>
       <c r="C36" s="119" t="n">
-        <v>8</v>
-      </c>
-      <c r="D36" s="123" t="n">
-        <v>72</v>
+        <v>10</v>
+      </c>
+      <c r="D36" s="119" t="n">
+        <v>32</v>
       </c>
       <c r="E36" s="115" t="n">
         <v>0</v>
@@ -2746,14 +2746,14 @@
       <c r="F36" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G36" s="131" t="inlineStr">
-        <is>
-          <t>1.32e-05</t>
-        </is>
-      </c>
-      <c r="H36" s="119" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="G36" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H36" s="120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="I36" s="120" t="inlineStr">
@@ -2766,9 +2766,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K36" s="128" t="inlineStr">
-        <is>
-          <t>82.3</t>
+      <c r="K36" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L36" s="115" t="inlineStr">
@@ -2776,26 +2776,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M36" s="127" t="inlineStr">
-        <is>
-          <t>24.3</t>
+      <c r="M36" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="115" t="inlineStr">
         <is>
-          <t>2025-01-30 18:00 gio</t>
-        </is>
-      </c>
-      <c r="B37" s="121" t="n">
-        <v>10</v>
-      </c>
-      <c r="C37" s="119" t="n">
-        <v>6</v>
-      </c>
-      <c r="D37" s="123" t="n">
-        <v>78</v>
+          <t>2025-06-15 18:00 Sun</t>
+        </is>
+      </c>
+      <c r="B37" s="117" t="n">
+        <v>23</v>
+      </c>
+      <c r="C37" s="118" t="n">
+        <v>14</v>
+      </c>
+      <c r="D37" s="119" t="n">
+        <v>56</v>
       </c>
       <c r="E37" s="115" t="n">
         <v>0</v>
@@ -2823,36 +2823,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K37" s="130" t="inlineStr">
-        <is>
-          <t>53.2</t>
-        </is>
-      </c>
-      <c r="L37" s="126" t="inlineStr">
-        <is>
-          <t>16.4</t>
-        </is>
-      </c>
-      <c r="M37" s="126" t="inlineStr">
-        <is>
-          <t>16.3</t>
+      <c r="K37" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L37" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M37" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="115" t="inlineStr">
         <is>
-          <t>2025-01-30 21:00 gio</t>
-        </is>
-      </c>
-      <c r="B38" s="121" t="n">
-        <v>9</v>
-      </c>
-      <c r="C38" s="119" t="n">
-        <v>6</v>
-      </c>
-      <c r="D38" s="123" t="n">
-        <v>79</v>
+          <t>2025-06-15 21:00 Sun</t>
+        </is>
+      </c>
+      <c r="B38" s="119" t="n">
+        <v>20</v>
+      </c>
+      <c r="C38" s="118" t="n">
+        <v>14</v>
+      </c>
+      <c r="D38" s="121" t="n">
+        <v>66</v>
       </c>
       <c r="E38" s="115" t="n">
         <v>0</v>
@@ -2880,36 +2880,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K38" s="120" t="inlineStr">
-        <is>
-          <t>0.8</t>
-        </is>
-      </c>
-      <c r="L38" s="130" t="inlineStr">
-        <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="M38" s="125" t="inlineStr">
-        <is>
-          <t>9.4</t>
+      <c r="K38" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L38" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M38" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="115" t="inlineStr">
         <is>
-          <t>2025-01-31 00:00 ven</t>
-        </is>
-      </c>
-      <c r="B39" s="121" t="n">
-        <v>9</v>
-      </c>
-      <c r="C39" s="119" t="n">
-        <v>6</v>
-      </c>
-      <c r="D39" s="123" t="n">
-        <v>81</v>
+          <t>2025-06-16 00:00 Mon</t>
+        </is>
+      </c>
+      <c r="B39" s="119" t="n">
+        <v>20</v>
+      </c>
+      <c r="C39" s="118" t="n">
+        <v>13</v>
+      </c>
+      <c r="D39" s="121" t="n">
+        <v>63</v>
       </c>
       <c r="E39" s="115" t="n">
         <v>0</v>
@@ -2937,36 +2937,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K39" s="120" t="inlineStr">
-        <is>
-          <t>0.4</t>
-        </is>
-      </c>
-      <c r="L39" s="130" t="inlineStr">
-        <is>
-          <t>33.3</t>
-        </is>
-      </c>
-      <c r="M39" s="130" t="inlineStr">
-        <is>
-          <t>54.5</t>
+      <c r="K39" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L39" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M39" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="115" t="inlineStr">
         <is>
-          <t>2025-01-31 03:00 ven</t>
-        </is>
-      </c>
-      <c r="B40" s="121" t="n">
-        <v>9</v>
-      </c>
-      <c r="C40" s="119" t="n">
-        <v>7</v>
-      </c>
-      <c r="D40" s="123" t="n">
-        <v>84</v>
+          <t>2025-06-16 03:00 Mon</t>
+        </is>
+      </c>
+      <c r="B40" s="119" t="n">
+        <v>19</v>
+      </c>
+      <c r="C40" s="118" t="n">
+        <v>13</v>
+      </c>
+      <c r="D40" s="121" t="n">
+        <v>65</v>
       </c>
       <c r="E40" s="115" t="n">
         <v>0</v>
@@ -2999,31 +2999,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L40" s="127" t="inlineStr">
-        <is>
-          <t>28.3</t>
-        </is>
-      </c>
-      <c r="M40" s="130" t="inlineStr">
-        <is>
-          <t>34.9</t>
+      <c r="L40" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M40" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="115" t="inlineStr">
         <is>
-          <t>2025-01-31 06:00 ven</t>
-        </is>
-      </c>
-      <c r="B41" s="121" t="n">
-        <v>9</v>
-      </c>
-      <c r="C41" s="119" t="n">
-        <v>7</v>
-      </c>
-      <c r="D41" s="123" t="n">
-        <v>86</v>
+          <t>2025-06-16 06:00 Mon</t>
+        </is>
+      </c>
+      <c r="B41" s="117" t="n">
+        <v>24</v>
+      </c>
+      <c r="C41" s="118" t="n">
+        <v>13</v>
+      </c>
+      <c r="D41" s="119" t="n">
+        <v>47</v>
       </c>
       <c r="E41" s="115" t="n">
         <v>0</v>
@@ -3056,31 +3056,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L41" s="127" t="inlineStr">
-        <is>
-          <t>23.9</t>
-        </is>
-      </c>
-      <c r="M41" s="126" t="inlineStr">
-        <is>
-          <t>18.3</t>
+      <c r="L41" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M41" s="125" t="inlineStr">
+        <is>
+          <t>5.9</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="115" t="inlineStr">
         <is>
-          <t>2025-01-31 09:00 ven</t>
-        </is>
-      </c>
-      <c r="B42" s="127" t="n">
-        <v>13</v>
-      </c>
-      <c r="C42" s="119" t="n">
-        <v>8</v>
-      </c>
-      <c r="D42" s="121" t="n">
-        <v>67</v>
+          <t>2025-06-16 09:00 Mon</t>
+        </is>
+      </c>
+      <c r="B42" s="117" t="n">
+        <v>29</v>
+      </c>
+      <c r="C42" s="117" t="n">
+        <v>11</v>
+      </c>
+      <c r="D42" s="119" t="n">
+        <v>33</v>
       </c>
       <c r="E42" s="115" t="n">
         <v>0</v>
@@ -3113,31 +3113,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L42" s="120" t="inlineStr">
-        <is>
-          <t>1.7</t>
-        </is>
-      </c>
-      <c r="M42" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="L42" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M42" s="128" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="115" t="inlineStr">
         <is>
-          <t>2025-01-31 12:00 ven</t>
-        </is>
-      </c>
-      <c r="B43" s="119" t="n">
-        <v>15</v>
-      </c>
-      <c r="C43" s="119" t="n">
-        <v>7</v>
+          <t>2025-06-16 12:00 Mon</t>
+        </is>
+      </c>
+      <c r="B43" s="118" t="n">
+        <v>31</v>
+      </c>
+      <c r="C43" s="118" t="n">
+        <v>13</v>
       </c>
       <c r="D43" s="119" t="n">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="E43" s="115" t="n">
         <v>0</v>
@@ -3170,31 +3170,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L43" s="120" t="inlineStr">
-        <is>
-          <t>0.8</t>
-        </is>
-      </c>
-      <c r="M43" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="L43" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M43" s="128" t="inlineStr">
+        <is>
+          <t>88.6</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="115" t="inlineStr">
         <is>
-          <t>2025-01-31 15:00 ven</t>
-        </is>
-      </c>
-      <c r="B44" s="127" t="n">
+          <t>2025-06-16 15:00 Mon</t>
+        </is>
+      </c>
+      <c r="B44" s="117" t="n">
+        <v>30</v>
+      </c>
+      <c r="C44" s="118" t="n">
         <v>13</v>
       </c>
-      <c r="C44" s="119" t="n">
-        <v>8</v>
-      </c>
-      <c r="D44" s="121" t="n">
-        <v>70</v>
+      <c r="D44" s="119" t="n">
+        <v>36</v>
       </c>
       <c r="E44" s="115" t="n">
         <v>0</v>
@@ -3222,36 +3222,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K44" s="120" t="inlineStr">
-        <is>
-          <t>2.6</t>
-        </is>
-      </c>
-      <c r="L44" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M44" s="130" t="inlineStr">
-        <is>
-          <t>30.1</t>
+      <c r="K44" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L44" s="120" t="inlineStr">
+        <is>
+          <t>1.7</t>
+        </is>
+      </c>
+      <c r="M44" s="126" t="inlineStr">
+        <is>
+          <t>16.8</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="115" t="inlineStr">
         <is>
-          <t>2025-01-31 18:00 ven</t>
-        </is>
-      </c>
-      <c r="B45" s="127" t="n">
-        <v>11</v>
-      </c>
-      <c r="C45" s="119" t="n">
-        <v>8</v>
-      </c>
-      <c r="D45" s="123" t="n">
-        <v>83</v>
+          <t>2025-06-16 18:00 Mon</t>
+        </is>
+      </c>
+      <c r="B45" s="117" t="n">
+        <v>24</v>
+      </c>
+      <c r="C45" s="118" t="n">
+        <v>14</v>
+      </c>
+      <c r="D45" s="119" t="n">
+        <v>52</v>
       </c>
       <c r="E45" s="115" t="n">
         <v>0</v>
@@ -3279,19 +3279,19 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K45" s="120" t="inlineStr">
-        <is>
-          <t>1.3</t>
-        </is>
-      </c>
-      <c r="L45" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M45" s="129" t="inlineStr">
-        <is>
-          <t>61.2</t>
+      <c r="K45" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L45" s="120" t="inlineStr">
+        <is>
+          <t>2.6</t>
+        </is>
+      </c>
+      <c r="M45" s="126" t="inlineStr">
+        <is>
+          <t>13.8</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Tropical night temp for Temperture and Weather graphs.
</commit_message>
<xml_diff>
--- a/data/simpleWeather.xlsx
+++ b/data/simpleWeather.xlsx
@@ -790,17 +790,17 @@
     <row r="2">
       <c r="A2" s="115" t="inlineStr">
         <is>
-          <t>2025-06-11 09:00 Wed</t>
-        </is>
-      </c>
-      <c r="B2" s="117" t="n">
-        <v>28</v>
-      </c>
-      <c r="C2" s="118" t="n">
-        <v>13</v>
+          <t>2025-06-16 03:00 Mon</t>
+        </is>
+      </c>
+      <c r="B2" s="119" t="n">
+        <v>20</v>
+      </c>
+      <c r="C2" s="119" t="n">
+        <v>10</v>
       </c>
       <c r="D2" s="119" t="n">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="E2" s="115" t="n">
         <v>0</v>
@@ -847,17 +847,17 @@
     <row r="3">
       <c r="A3" s="115" t="inlineStr">
         <is>
-          <t>2025-06-11 12:00 Wed</t>
+          <t>2025-06-16 06:00 Mon</t>
         </is>
       </c>
       <c r="B3" s="117" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C3" s="117" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="119" t="n">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E3" s="115" t="n">
         <v>0</v>
@@ -904,17 +904,17 @@
     <row r="4">
       <c r="A4" s="115" t="inlineStr">
         <is>
-          <t>2025-06-11 15:00 Wed</t>
+          <t>2025-06-16 09:00 Mon</t>
         </is>
       </c>
       <c r="B4" s="117" t="n">
-        <v>28</v>
-      </c>
-      <c r="C4" s="117" t="n">
-        <v>12</v>
-      </c>
-      <c r="D4" s="119" t="n">
-        <v>36</v>
+        <v>30</v>
+      </c>
+      <c r="C4" s="119" t="n">
+        <v>9</v>
+      </c>
+      <c r="D4" s="117" t="n">
+        <v>26</v>
       </c>
       <c r="E4" s="115" t="n">
         <v>0</v>
@@ -961,17 +961,17 @@
     <row r="5">
       <c r="A5" s="115" t="inlineStr">
         <is>
-          <t>2025-06-11 18:00 Wed</t>
-        </is>
-      </c>
-      <c r="B5" s="117" t="n">
-        <v>23</v>
-      </c>
-      <c r="C5" s="118" t="n">
-        <v>14</v>
-      </c>
-      <c r="D5" s="119" t="n">
-        <v>55</v>
+          <t>2025-06-16 12:00 Mon</t>
+        </is>
+      </c>
+      <c r="B5" s="118" t="n">
+        <v>32</v>
+      </c>
+      <c r="C5" s="117" t="n">
+        <v>11</v>
+      </c>
+      <c r="D5" s="117" t="n">
+        <v>27</v>
       </c>
       <c r="E5" s="115" t="n">
         <v>0</v>
@@ -1009,26 +1009,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M5" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M5" s="120" t="inlineStr">
+        <is>
+          <t>1.5</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="115" t="inlineStr">
         <is>
-          <t>2025-06-11 21:00 Wed</t>
-        </is>
-      </c>
-      <c r="B6" s="119" t="n">
-        <v>21</v>
-      </c>
-      <c r="C6" s="118" t="n">
-        <v>15</v>
-      </c>
-      <c r="D6" s="121" t="n">
-        <v>70</v>
+          <t>2025-06-16 15:00 Mon</t>
+        </is>
+      </c>
+      <c r="B6" s="118" t="n">
+        <v>31</v>
+      </c>
+      <c r="C6" s="117" t="n">
+        <v>11</v>
+      </c>
+      <c r="D6" s="117" t="n">
+        <v>28</v>
       </c>
       <c r="E6" s="115" t="n">
         <v>0</v>
@@ -1066,26 +1066,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M6" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M6" s="120" t="inlineStr">
+        <is>
+          <t>1.7</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="115" t="inlineStr">
         <is>
-          <t>2025-06-12 00:00 Thu</t>
-        </is>
-      </c>
-      <c r="B7" s="119" t="n">
-        <v>20</v>
+          <t>2025-06-16 18:00 Mon</t>
+        </is>
+      </c>
+      <c r="B7" s="117" t="n">
+        <v>27</v>
       </c>
       <c r="C7" s="118" t="n">
-        <v>15</v>
-      </c>
-      <c r="D7" s="123" t="n">
-        <v>76</v>
+        <v>13</v>
+      </c>
+      <c r="D7" s="119" t="n">
+        <v>42</v>
       </c>
       <c r="E7" s="115" t="n">
         <v>0</v>
@@ -1123,26 +1123,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M7" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M7" s="130" t="inlineStr">
+        <is>
+          <t>50.8</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="115" t="inlineStr">
         <is>
-          <t>2025-06-12 03:00 Thu</t>
-        </is>
-      </c>
-      <c r="B8" s="119" t="n">
-        <v>19</v>
+          <t>2025-06-16 21:00 Mon</t>
+        </is>
+      </c>
+      <c r="B8" s="117" t="n">
+        <v>24</v>
       </c>
       <c r="C8" s="118" t="n">
-        <v>16</v>
-      </c>
-      <c r="D8" s="123" t="n">
-        <v>83</v>
+        <v>13</v>
+      </c>
+      <c r="D8" s="119" t="n">
+        <v>49</v>
       </c>
       <c r="E8" s="115" t="n">
         <v>0</v>
@@ -1175,31 +1175,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L8" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="L8" s="120" t="inlineStr">
+        <is>
+          <t>1.7</t>
         </is>
       </c>
       <c r="M8" s="115" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>84.7</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="115" t="inlineStr">
         <is>
-          <t>2025-06-12 06:00 Thu</t>
+          <t>2025-06-17 00:00 Tue</t>
         </is>
       </c>
       <c r="B9" s="117" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" s="118" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="119" t="n">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E9" s="115" t="n">
         <v>0</v>
@@ -1232,31 +1232,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L9" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M9" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="L9" s="126" t="inlineStr">
+        <is>
+          <t>10.9</t>
+        </is>
+      </c>
+      <c r="M9" s="128" t="inlineStr">
+        <is>
+          <t>92.1</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="115" t="inlineStr">
         <is>
-          <t>2025-06-12 09:00 Thu</t>
-        </is>
-      </c>
-      <c r="B10" s="117" t="n">
-        <v>28</v>
+          <t>2025-06-17 03:00 Tue</t>
+        </is>
+      </c>
+      <c r="B10" s="119" t="n">
+        <v>22</v>
       </c>
       <c r="C10" s="118" t="n">
-        <v>15</v>
-      </c>
-      <c r="D10" s="119" t="n">
-        <v>43</v>
+        <v>14</v>
+      </c>
+      <c r="D10" s="121" t="n">
+        <v>63</v>
       </c>
       <c r="E10" s="115" t="n">
         <v>0</v>
@@ -1289,31 +1289,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L10" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M10" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="L10" s="129" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="M10" s="130" t="inlineStr">
+        <is>
+          <t>37.3</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="115" t="inlineStr">
         <is>
-          <t>2025-06-12 12:00 Thu</t>
+          <t>2025-06-17 06:00 Tue</t>
         </is>
       </c>
       <c r="B11" s="117" t="n">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C11" s="118" t="n">
         <v>15</v>
       </c>
       <c r="D11" s="119" t="n">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E11" s="115" t="n">
         <v>0</v>
@@ -1341,36 +1341,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K11" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L11" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M11" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K11" s="120" t="inlineStr">
+        <is>
+          <t>0.8</t>
+        </is>
+      </c>
+      <c r="L11" s="128" t="inlineStr">
+        <is>
+          <t>86.6</t>
+        </is>
+      </c>
+      <c r="M11" s="129" t="inlineStr">
+        <is>
+          <t>68.7</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="115" t="inlineStr">
         <is>
-          <t>2025-06-12 15:00 Thu</t>
+          <t>2025-06-17 09:00 Tue</t>
         </is>
       </c>
       <c r="B12" s="117" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" s="118" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" s="119" t="n">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E12" s="115" t="n">
         <v>0</v>
@@ -1398,36 +1398,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K12" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L12" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M12" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K12" s="126" t="inlineStr">
+        <is>
+          <t>14.3</t>
+        </is>
+      </c>
+      <c r="L12" s="129" t="inlineStr">
+        <is>
+          <t>66.5</t>
+        </is>
+      </c>
+      <c r="M12" s="128" t="inlineStr">
+        <is>
+          <t>90.8</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="115" t="inlineStr">
         <is>
-          <t>2025-06-12 18:00 Thu</t>
-        </is>
-      </c>
-      <c r="B13" s="117" t="n">
-        <v>24</v>
+          <t>2025-06-17 12:00 Tue</t>
+        </is>
+      </c>
+      <c r="B13" s="118" t="n">
+        <v>31</v>
       </c>
       <c r="C13" s="118" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D13" s="119" t="n">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="E13" s="115" t="n">
         <v>0</v>
@@ -1455,36 +1455,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K13" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L13" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M13" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K13" s="125" t="inlineStr">
+        <is>
+          <t>7.1</t>
+        </is>
+      </c>
+      <c r="L13" s="130" t="inlineStr">
+        <is>
+          <t>36.8</t>
+        </is>
+      </c>
+      <c r="M13" s="130" t="inlineStr">
+        <is>
+          <t>57.4</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="115" t="inlineStr">
         <is>
-          <t>2025-06-12 21:00 Thu</t>
-        </is>
-      </c>
-      <c r="B14" s="119" t="n">
-        <v>22</v>
+          <t>2025-06-17 15:00 Tue</t>
+        </is>
+      </c>
+      <c r="B14" s="117" t="n">
+        <v>30</v>
       </c>
       <c r="C14" s="118" t="n">
-        <v>17</v>
-      </c>
-      <c r="D14" s="123" t="n">
-        <v>72</v>
+        <v>13</v>
+      </c>
+      <c r="D14" s="119" t="n">
+        <v>34</v>
       </c>
       <c r="E14" s="115" t="n">
         <v>0</v>
@@ -1492,9 +1492,9 @@
       <c r="F14" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G14" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G14" s="131" t="inlineStr">
+        <is>
+          <t>6.08e-05</t>
         </is>
       </c>
       <c r="H14" s="120" t="inlineStr">
@@ -1517,31 +1517,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L14" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M14" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="L14" s="126" t="inlineStr">
+        <is>
+          <t>14.1</t>
+        </is>
+      </c>
+      <c r="M14" s="125" t="inlineStr">
+        <is>
+          <t>8.6</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="115" t="inlineStr">
         <is>
-          <t>2025-06-13 00:00 Fri</t>
-        </is>
-      </c>
-      <c r="B15" s="119" t="n">
-        <v>21</v>
+          <t>2025-06-17 18:00 Tue</t>
+        </is>
+      </c>
+      <c r="B15" s="117" t="n">
+        <v>26</v>
       </c>
       <c r="C15" s="118" t="n">
-        <v>16</v>
-      </c>
-      <c r="D15" s="123" t="n">
-        <v>74</v>
+        <v>15</v>
+      </c>
+      <c r="D15" s="119" t="n">
+        <v>49</v>
       </c>
       <c r="E15" s="115" t="n">
         <v>0</v>
@@ -1574,31 +1574,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L15" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M15" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="L15" s="125" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="M15" s="125" t="inlineStr">
+        <is>
+          <t>6.4</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="115" t="inlineStr">
         <is>
-          <t>2025-06-13 03:00 Fri</t>
-        </is>
-      </c>
-      <c r="B16" s="119" t="n">
-        <v>20</v>
+          <t>2025-06-17 21:00 Tue</t>
+        </is>
+      </c>
+      <c r="B16" s="117" t="n">
+        <v>23</v>
       </c>
       <c r="C16" s="118" t="n">
         <v>17</v>
       </c>
-      <c r="D16" s="123" t="n">
-        <v>79</v>
+      <c r="D16" s="121" t="n">
+        <v>69</v>
       </c>
       <c r="E16" s="115" t="n">
         <v>0</v>
@@ -1631,31 +1631,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L16" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M16" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="L16" s="120" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M16" s="125" t="inlineStr">
+        <is>
+          <t>5.6</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="115" t="inlineStr">
         <is>
-          <t>2025-06-13 06:00 Fri</t>
-        </is>
-      </c>
-      <c r="B17" s="117" t="n">
-        <v>26</v>
-      </c>
-      <c r="C17" s="118" t="n">
-        <v>15</v>
-      </c>
-      <c r="D17" s="119" t="n">
-        <v>51</v>
+          <t>2025-06-18 00:00 Wed</t>
+        </is>
+      </c>
+      <c r="B17" s="119" t="n">
+        <v>22</v>
+      </c>
+      <c r="C17" s="122" t="n">
+        <v>18</v>
+      </c>
+      <c r="D17" s="123" t="n">
+        <v>77</v>
       </c>
       <c r="E17" s="115" t="n">
         <v>0</v>
@@ -1688,31 +1688,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L17" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M17" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="L17" s="120" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M17" s="126" t="inlineStr">
+        <is>
+          <t>12.2</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="115" t="inlineStr">
         <is>
-          <t>2025-06-13 09:00 Fri</t>
-        </is>
-      </c>
-      <c r="B18" s="117" t="n">
-        <v>30</v>
-      </c>
-      <c r="C18" s="118" t="n">
-        <v>13</v>
-      </c>
-      <c r="D18" s="119" t="n">
-        <v>35</v>
+          <t>2025-06-18 03:00 Wed</t>
+        </is>
+      </c>
+      <c r="B18" s="119" t="n">
+        <v>21</v>
+      </c>
+      <c r="C18" s="122" t="n">
+        <v>18</v>
+      </c>
+      <c r="D18" s="123" t="n">
+        <v>81</v>
       </c>
       <c r="E18" s="115" t="n">
         <v>0</v>
@@ -1745,31 +1745,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L18" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M18" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="L18" s="120" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M18" s="125" t="inlineStr">
+        <is>
+          <t>6.1</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="115" t="inlineStr">
         <is>
-          <t>2025-06-13 12:00 Fri</t>
-        </is>
-      </c>
-      <c r="B19" s="118" t="n">
-        <v>31</v>
-      </c>
-      <c r="C19" s="117" t="n">
-        <v>12</v>
-      </c>
-      <c r="D19" s="119" t="n">
-        <v>32</v>
+          <t>2025-06-18 06:00 Wed</t>
+        </is>
+      </c>
+      <c r="B19" s="117" t="n">
+        <v>25</v>
+      </c>
+      <c r="C19" s="118" t="n">
+        <v>17</v>
+      </c>
+      <c r="D19" s="121" t="n">
+        <v>61</v>
       </c>
       <c r="E19" s="115" t="n">
         <v>0</v>
@@ -1802,31 +1802,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L19" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M19" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="L19" s="120" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+      <c r="M19" s="120" t="inlineStr">
+        <is>
+          <t>4.6</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="115" t="inlineStr">
         <is>
-          <t>2025-06-13 15:00 Fri</t>
+          <t>2025-06-18 09:00 Wed</t>
         </is>
       </c>
       <c r="B20" s="117" t="n">
-        <v>29</v>
-      </c>
-      <c r="C20" s="117" t="n">
-        <v>12</v>
+        <v>28</v>
+      </c>
+      <c r="C20" s="118" t="n">
+        <v>16</v>
       </c>
       <c r="D20" s="119" t="n">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="E20" s="115" t="n">
         <v>0</v>
@@ -1859,31 +1859,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L20" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M20" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="L20" s="120" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M20" s="120" t="inlineStr">
+        <is>
+          <t>3.2</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="115" t="inlineStr">
         <is>
-          <t>2025-06-13 18:00 Fri</t>
+          <t>2025-06-18 12:00 Wed</t>
         </is>
       </c>
       <c r="B21" s="117" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C21" s="118" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D21" s="119" t="n">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="E21" s="115" t="n">
         <v>0</v>
@@ -1916,31 +1916,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L21" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M21" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="L21" s="120" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M21" s="130" t="inlineStr">
+        <is>
+          <t>32.6</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="115" t="inlineStr">
         <is>
-          <t>2025-06-13 21:00 Fri</t>
-        </is>
-      </c>
-      <c r="B22" s="119" t="n">
-        <v>22</v>
-      </c>
-      <c r="C22" s="122" t="n">
-        <v>18</v>
-      </c>
-      <c r="D22" s="123" t="n">
-        <v>80</v>
+          <t>2025-06-18 15:00 Wed</t>
+        </is>
+      </c>
+      <c r="B22" s="117" t="n">
+        <v>28</v>
+      </c>
+      <c r="C22" s="118" t="n">
+        <v>16</v>
+      </c>
+      <c r="D22" s="119" t="n">
+        <v>47</v>
       </c>
       <c r="E22" s="115" t="n">
         <v>0</v>
@@ -1968,36 +1968,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K22" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L22" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M22" s="120" t="inlineStr">
-        <is>
-          <t>3.3</t>
+      <c r="K22" s="120" t="inlineStr">
+        <is>
+          <t>2.6</t>
+        </is>
+      </c>
+      <c r="L22" s="120" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M22" s="129" t="inlineStr">
+        <is>
+          <t>71.4</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="115" t="inlineStr">
         <is>
-          <t>2025-06-14 00:00 Sat</t>
-        </is>
-      </c>
-      <c r="B23" s="119" t="n">
-        <v>21</v>
+          <t>2025-06-18 18:00 Wed</t>
+        </is>
+      </c>
+      <c r="B23" s="117" t="n">
+        <v>24</v>
       </c>
       <c r="C23" s="122" t="n">
         <v>18</v>
       </c>
-      <c r="D23" s="123" t="n">
-        <v>83</v>
+      <c r="D23" s="121" t="n">
+        <v>68</v>
       </c>
       <c r="E23" s="115" t="n">
         <v>0</v>
@@ -2025,36 +2025,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K23" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L23" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M23" s="120" t="inlineStr">
-        <is>
-          <t>1.7</t>
+      <c r="K23" s="120" t="inlineStr">
+        <is>
+          <t>3.1</t>
+        </is>
+      </c>
+      <c r="L23" s="120" t="inlineStr">
+        <is>
+          <t>4.7</t>
+        </is>
+      </c>
+      <c r="M23" s="130" t="inlineStr">
+        <is>
+          <t>47.4</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="115" t="inlineStr">
         <is>
-          <t>2025-06-14 03:00 Sat</t>
+          <t>2025-06-18 21:00 Wed</t>
         </is>
       </c>
       <c r="B24" s="119" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C24" s="122" t="n">
         <v>18</v>
       </c>
       <c r="D24" s="123" t="n">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E24" s="115" t="n">
         <v>0</v>
@@ -2082,36 +2082,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K24" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L24" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M24" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K24" s="120" t="inlineStr">
+        <is>
+          <t>1.3</t>
+        </is>
+      </c>
+      <c r="L24" s="120" t="inlineStr">
+        <is>
+          <t>0.1</t>
+        </is>
+      </c>
+      <c r="M24" s="130" t="inlineStr">
+        <is>
+          <t>30.3</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="115" t="inlineStr">
         <is>
-          <t>2025-06-14 06:00 Sat</t>
-        </is>
-      </c>
-      <c r="B25" s="117" t="n">
-        <v>26</v>
-      </c>
-      <c r="C25" s="118" t="n">
-        <v>17</v>
-      </c>
-      <c r="D25" s="119" t="n">
-        <v>58</v>
+          <t>2025-06-19 00:00 Thu</t>
+        </is>
+      </c>
+      <c r="B25" s="119" t="n">
+        <v>22</v>
+      </c>
+      <c r="C25" s="122" t="n">
+        <v>19</v>
+      </c>
+      <c r="D25" s="123" t="n">
+        <v>83</v>
       </c>
       <c r="E25" s="115" t="n">
         <v>0</v>
@@ -2139,36 +2139,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K25" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L25" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M25" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K25" s="120" t="inlineStr">
+        <is>
+          <t>0.6</t>
+        </is>
+      </c>
+      <c r="L25" s="120" t="inlineStr">
+        <is>
+          <t>1.3</t>
+        </is>
+      </c>
+      <c r="M25" s="127" t="inlineStr">
+        <is>
+          <t>27.9</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="115" t="inlineStr">
         <is>
-          <t>2025-06-14 09:00 Sat</t>
-        </is>
-      </c>
-      <c r="B26" s="117" t="n">
-        <v>29</v>
-      </c>
-      <c r="C26" s="118" t="n">
-        <v>17</v>
-      </c>
-      <c r="D26" s="119" t="n">
-        <v>50</v>
+          <t>2025-06-19 03:00 Thu</t>
+        </is>
+      </c>
+      <c r="B26" s="119" t="n">
+        <v>21</v>
+      </c>
+      <c r="C26" s="122" t="n">
+        <v>18</v>
+      </c>
+      <c r="D26" s="123" t="n">
+        <v>85</v>
       </c>
       <c r="E26" s="115" t="n">
         <v>0</v>
@@ -2196,9 +2196,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K26" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K26" s="120" t="inlineStr">
+        <is>
+          <t>0.4</t>
         </is>
       </c>
       <c r="L26" s="115" t="inlineStr">
@@ -2206,26 +2206,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M26" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M26" s="126" t="inlineStr">
+        <is>
+          <t>12.8</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="115" t="inlineStr">
         <is>
-          <t>2025-06-14 12:00 Sat</t>
+          <t>2025-06-19 06:00 Thu</t>
         </is>
       </c>
       <c r="B27" s="117" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C27" s="118" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D27" s="119" t="n">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="E27" s="115" t="n">
         <v>0</v>
@@ -2253,9 +2253,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K27" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K27" s="120" t="inlineStr">
+        <is>
+          <t>0.2</t>
         </is>
       </c>
       <c r="L27" s="115" t="inlineStr">
@@ -2263,26 +2263,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M27" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M27" s="125" t="inlineStr">
+        <is>
+          <t>6.6</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="115" t="inlineStr">
         <is>
-          <t>2025-06-14 15:00 Sat</t>
+          <t>2025-06-19 09:00 Thu</t>
         </is>
       </c>
       <c r="B28" s="117" t="n">
-        <v>29</v>
-      </c>
-      <c r="C28" s="117" t="n">
-        <v>11</v>
+        <v>28</v>
+      </c>
+      <c r="C28" s="118" t="n">
+        <v>16</v>
       </c>
       <c r="D28" s="119" t="n">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="E28" s="115" t="n">
         <v>0</v>
@@ -2329,17 +2329,17 @@
     <row r="29">
       <c r="A29" s="115" t="inlineStr">
         <is>
-          <t>2025-06-14 18:00 Sat</t>
+          <t>2025-06-19 12:00 Thu</t>
         </is>
       </c>
       <c r="B29" s="117" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C29" s="118" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D29" s="119" t="n">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E29" s="115" t="n">
         <v>0</v>
@@ -2386,17 +2386,17 @@
     <row r="30">
       <c r="A30" s="115" t="inlineStr">
         <is>
-          <t>2025-06-14 21:00 Sat</t>
-        </is>
-      </c>
-      <c r="B30" s="119" t="n">
-        <v>22</v>
+          <t>2025-06-19 15:00 Thu</t>
+        </is>
+      </c>
+      <c r="B30" s="117" t="n">
+        <v>29</v>
       </c>
       <c r="C30" s="118" t="n">
         <v>16</v>
       </c>
-      <c r="D30" s="121" t="n">
-        <v>66</v>
+      <c r="D30" s="119" t="n">
+        <v>46</v>
       </c>
       <c r="E30" s="115" t="n">
         <v>0</v>
@@ -2443,17 +2443,17 @@
     <row r="31">
       <c r="A31" s="115" t="inlineStr">
         <is>
-          <t>2025-06-15 00:00 Sun</t>
-        </is>
-      </c>
-      <c r="B31" s="119" t="n">
-        <v>22</v>
-      </c>
-      <c r="C31" s="118" t="n">
-        <v>16</v>
+          <t>2025-06-19 18:00 Thu</t>
+        </is>
+      </c>
+      <c r="B31" s="117" t="n">
+        <v>24</v>
+      </c>
+      <c r="C31" s="122" t="n">
+        <v>18</v>
       </c>
       <c r="D31" s="121" t="n">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E31" s="115" t="n">
         <v>0</v>
@@ -2491,26 +2491,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M31" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M31" s="120" t="inlineStr">
+        <is>
+          <t>0.1</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="115" t="inlineStr">
         <is>
-          <t>2025-06-15 03:00 Sun</t>
+          <t>2025-06-19 21:00 Thu</t>
         </is>
       </c>
       <c r="B32" s="119" t="n">
-        <v>21</v>
-      </c>
-      <c r="C32" s="118" t="n">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="C32" s="122" t="n">
+        <v>19</v>
       </c>
       <c r="D32" s="123" t="n">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E32" s="115" t="n">
         <v>0</v>
@@ -2548,26 +2548,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M32" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M32" s="128" t="inlineStr">
+        <is>
+          <t>99.1</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="115" t="inlineStr">
         <is>
-          <t>2025-06-15 06:00 Sun</t>
-        </is>
-      </c>
-      <c r="B33" s="117" t="n">
-        <v>25</v>
-      </c>
-      <c r="C33" s="117" t="n">
-        <v>12</v>
-      </c>
-      <c r="D33" s="119" t="n">
-        <v>45</v>
+          <t>2025-06-20 00:00 Fri</t>
+        </is>
+      </c>
+      <c r="B33" s="119" t="n">
+        <v>22</v>
+      </c>
+      <c r="C33" s="122" t="n">
+        <v>18</v>
+      </c>
+      <c r="D33" s="123" t="n">
+        <v>82</v>
       </c>
       <c r="E33" s="115" t="n">
         <v>0</v>
@@ -2605,26 +2605,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M33" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M33" s="130" t="inlineStr">
+        <is>
+          <t>52.1</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="115" t="inlineStr">
         <is>
-          <t>2025-06-15 09:00 Sun</t>
-        </is>
-      </c>
-      <c r="B34" s="117" t="n">
-        <v>27</v>
-      </c>
-      <c r="C34" s="118" t="n">
-        <v>13</v>
-      </c>
-      <c r="D34" s="119" t="n">
-        <v>39</v>
+          <t>2025-06-20 03:00 Fri</t>
+        </is>
+      </c>
+      <c r="B34" s="119" t="n">
+        <v>21</v>
+      </c>
+      <c r="C34" s="122" t="n">
+        <v>19</v>
+      </c>
+      <c r="D34" s="123" t="n">
+        <v>89</v>
       </c>
       <c r="E34" s="115" t="n">
         <v>0</v>
@@ -2662,26 +2662,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M34" s="120" t="inlineStr">
-        <is>
-          <t>0.5</t>
+      <c r="M34" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="115" t="inlineStr">
         <is>
-          <t>2025-06-15 12:00 Sun</t>
+          <t>2025-06-20 06:00 Fri</t>
         </is>
       </c>
       <c r="B35" s="117" t="n">
-        <v>29</v>
-      </c>
-      <c r="C35" s="119" t="n">
-        <v>10</v>
-      </c>
-      <c r="D35" s="119" t="n">
-        <v>31</v>
+        <v>26</v>
+      </c>
+      <c r="C35" s="122" t="n">
+        <v>18</v>
+      </c>
+      <c r="D35" s="121" t="n">
+        <v>63</v>
       </c>
       <c r="E35" s="115" t="n">
         <v>0</v>
@@ -2719,26 +2719,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M35" s="120" t="inlineStr">
-        <is>
-          <t>0.2</t>
+      <c r="M35" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="115" t="inlineStr">
         <is>
-          <t>2025-06-15 15:00 Sun</t>
+          <t>2025-06-20 09:00 Fri</t>
         </is>
       </c>
       <c r="B36" s="117" t="n">
-        <v>28</v>
-      </c>
-      <c r="C36" s="119" t="n">
-        <v>10</v>
+        <v>29</v>
+      </c>
+      <c r="C36" s="118" t="n">
+        <v>17</v>
       </c>
       <c r="D36" s="119" t="n">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="E36" s="115" t="n">
         <v>0</v>
@@ -2771,31 +2771,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L36" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M36" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="L36" s="120" t="inlineStr">
+        <is>
+          <t>0.1</t>
+        </is>
+      </c>
+      <c r="M36" s="120" t="inlineStr">
+        <is>
+          <t>0.1</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="115" t="inlineStr">
         <is>
-          <t>2025-06-15 18:00 Sun</t>
+          <t>2025-06-20 12:00 Fri</t>
         </is>
       </c>
       <c r="B37" s="117" t="n">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C37" s="118" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D37" s="119" t="n">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="E37" s="115" t="n">
         <v>0</v>
@@ -2828,31 +2828,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L37" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M37" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="L37" s="120" t="inlineStr">
+        <is>
+          <t>2.1</t>
+        </is>
+      </c>
+      <c r="M37" s="120" t="inlineStr">
+        <is>
+          <t>0.8</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="115" t="inlineStr">
         <is>
-          <t>2025-06-15 21:00 Sun</t>
-        </is>
-      </c>
-      <c r="B38" s="119" t="n">
-        <v>20</v>
+          <t>2025-06-20 15:00 Fri</t>
+        </is>
+      </c>
+      <c r="B38" s="117" t="n">
+        <v>29</v>
       </c>
       <c r="C38" s="118" t="n">
-        <v>14</v>
-      </c>
-      <c r="D38" s="121" t="n">
-        <v>66</v>
+        <v>17</v>
+      </c>
+      <c r="D38" s="119" t="n">
+        <v>46</v>
       </c>
       <c r="E38" s="115" t="n">
         <v>0</v>
@@ -2890,26 +2890,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M38" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M38" s="120" t="inlineStr">
+        <is>
+          <t>1.3</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="115" t="inlineStr">
         <is>
-          <t>2025-06-16 00:00 Mon</t>
-        </is>
-      </c>
-      <c r="B39" s="119" t="n">
-        <v>20</v>
+          <t>2025-06-20 18:00 Fri</t>
+        </is>
+      </c>
+      <c r="B39" s="117" t="n">
+        <v>23</v>
       </c>
       <c r="C39" s="118" t="n">
-        <v>13</v>
-      </c>
-      <c r="D39" s="121" t="n">
-        <v>63</v>
+        <v>15</v>
+      </c>
+      <c r="D39" s="119" t="n">
+        <v>60</v>
       </c>
       <c r="E39" s="115" t="n">
         <v>0</v>
@@ -2942,31 +2942,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L39" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M39" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="L39" s="120" t="inlineStr">
+        <is>
+          <t>1.8</t>
+        </is>
+      </c>
+      <c r="M39" s="130" t="inlineStr">
+        <is>
+          <t>50.6</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="115" t="inlineStr">
         <is>
-          <t>2025-06-16 03:00 Mon</t>
+          <t>2025-06-20 21:00 Fri</t>
         </is>
       </c>
       <c r="B40" s="119" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C40" s="118" t="n">
-        <v>13</v>
-      </c>
-      <c r="D40" s="121" t="n">
-        <v>65</v>
+        <v>17</v>
+      </c>
+      <c r="D40" s="123" t="n">
+        <v>83</v>
       </c>
       <c r="E40" s="115" t="n">
         <v>0</v>
@@ -2974,14 +2974,14 @@
       <c r="F40" s="115" t="n">
         <v>0</v>
       </c>
-      <c r="G40" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H40" s="120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G40" s="131" t="inlineStr">
+        <is>
+          <t>0.0006024</t>
+        </is>
+      </c>
+      <c r="H40" s="119" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I40" s="120" t="inlineStr">
@@ -2994,36 +2994,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K40" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L40" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M40" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K40" s="120" t="inlineStr">
+        <is>
+          <t>3.4</t>
+        </is>
+      </c>
+      <c r="L40" s="130" t="inlineStr">
+        <is>
+          <t>37.5</t>
+        </is>
+      </c>
+      <c r="M40" s="129" t="inlineStr">
+        <is>
+          <t>68.8</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="115" t="inlineStr">
         <is>
-          <t>2025-06-16 06:00 Mon</t>
-        </is>
-      </c>
-      <c r="B41" s="117" t="n">
-        <v>24</v>
-      </c>
-      <c r="C41" s="118" t="n">
-        <v>13</v>
-      </c>
-      <c r="D41" s="119" t="n">
-        <v>47</v>
+          <t>2025-06-21 00:00 Sat</t>
+        </is>
+      </c>
+      <c r="B41" s="119" t="n">
+        <v>22</v>
+      </c>
+      <c r="C41" s="122" t="n">
+        <v>18</v>
+      </c>
+      <c r="D41" s="123" t="n">
+        <v>77</v>
       </c>
       <c r="E41" s="115" t="n">
         <v>0</v>
@@ -3051,36 +3051,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K41" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L41" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M41" s="125" t="inlineStr">
-        <is>
-          <t>5.9</t>
+      <c r="K41" s="120" t="inlineStr">
+        <is>
+          <t>1.7</t>
+        </is>
+      </c>
+      <c r="L41" s="127" t="inlineStr">
+        <is>
+          <t>24.2</t>
+        </is>
+      </c>
+      <c r="M41" s="129" t="inlineStr">
+        <is>
+          <t>75.8</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="115" t="inlineStr">
         <is>
-          <t>2025-06-16 09:00 Mon</t>
-        </is>
-      </c>
-      <c r="B42" s="117" t="n">
-        <v>29</v>
-      </c>
-      <c r="C42" s="117" t="n">
-        <v>11</v>
-      </c>
-      <c r="D42" s="119" t="n">
-        <v>33</v>
+          <t>2025-06-21 03:00 Sat</t>
+        </is>
+      </c>
+      <c r="B42" s="119" t="n">
+        <v>22</v>
+      </c>
+      <c r="C42" s="122" t="n">
+        <v>20</v>
+      </c>
+      <c r="D42" s="123" t="n">
+        <v>87</v>
       </c>
       <c r="E42" s="115" t="n">
         <v>0</v>
@@ -3118,26 +3118,26 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M42" s="128" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="M42" s="130" t="inlineStr">
+        <is>
+          <t>36.7</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="115" t="inlineStr">
         <is>
-          <t>2025-06-16 12:00 Mon</t>
-        </is>
-      </c>
-      <c r="B43" s="118" t="n">
-        <v>31</v>
+          <t>2025-06-21 06:00 Sat</t>
+        </is>
+      </c>
+      <c r="B43" s="117" t="n">
+        <v>25</v>
       </c>
       <c r="C43" s="118" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D43" s="119" t="n">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="E43" s="115" t="n">
         <v>0</v>
@@ -3165,36 +3165,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K43" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L43" s="115" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M43" s="128" t="inlineStr">
-        <is>
-          <t>88.6</t>
+      <c r="K43" s="120" t="inlineStr">
+        <is>
+          <t>0.7</t>
+        </is>
+      </c>
+      <c r="L43" s="120" t="inlineStr">
+        <is>
+          <t>1.6</t>
+        </is>
+      </c>
+      <c r="M43" s="126" t="inlineStr">
+        <is>
+          <t>18.3</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="115" t="inlineStr">
         <is>
-          <t>2025-06-16 15:00 Mon</t>
+          <t>2025-06-21 09:00 Sat</t>
         </is>
       </c>
       <c r="B44" s="117" t="n">
-        <v>30</v>
-      </c>
-      <c r="C44" s="118" t="n">
-        <v>13</v>
+        <v>28</v>
+      </c>
+      <c r="C44" s="117" t="n">
+        <v>12</v>
       </c>
       <c r="D44" s="119" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E44" s="115" t="n">
         <v>0</v>
@@ -3227,31 +3227,31 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L44" s="120" t="inlineStr">
-        <is>
-          <t>1.7</t>
-        </is>
-      </c>
-      <c r="M44" s="126" t="inlineStr">
-        <is>
-          <t>16.8</t>
+      <c r="L44" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M44" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="115" t="inlineStr">
         <is>
-          <t>2025-06-16 18:00 Mon</t>
+          <t>2025-06-21 12:00 Sat</t>
         </is>
       </c>
       <c r="B45" s="117" t="n">
-        <v>24</v>
-      </c>
-      <c r="C45" s="118" t="n">
-        <v>14</v>
-      </c>
-      <c r="D45" s="119" t="n">
-        <v>52</v>
+        <v>29</v>
+      </c>
+      <c r="C45" s="119" t="n">
+        <v>9</v>
+      </c>
+      <c r="D45" s="117" t="n">
+        <v>29</v>
       </c>
       <c r="E45" s="115" t="n">
         <v>0</v>
@@ -3284,14 +3284,14 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L45" s="120" t="inlineStr">
-        <is>
-          <t>2.6</t>
-        </is>
-      </c>
-      <c r="M45" s="126" t="inlineStr">
-        <is>
-          <t>13.8</t>
+      <c r="L45" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M45" s="115" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>